<commit_message>
EPBDS - renamed TablePropertiesDefinition to TablePropertyDefinition, generated DefaultTablePropertyDefinitions
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stanislav Shor</author>
+  </authors>
+  <commentList>
+    <comment ref="E40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stanislav Shor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+this type should be the table return type</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="138">
   <si>
     <t>name</t>
   </si>
@@ -324,9 +358,6 @@
     <t>yes (coma separated filter specification by user role: category/role pairs)</t>
   </si>
   <si>
-    <t>yes (used as a key to navigate across multiple tables with the same name - e.g. versioning)</t>
-  </si>
-  <si>
     <t>Primary Key</t>
   </si>
   <si>
@@ -373,9 +404,6 @@
   </si>
   <si>
     <t>returnOnMiss</t>
-  </si>
-  <si>
-    <t>table Type</t>
   </si>
   <si>
     <t>only one active version per dimension</t>
@@ -441,12 +469,21 @@
   <si>
     <t>-default value if property is not defined or inherited</t>
   </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>org.openl.rules.table.properties</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +498,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -536,10 +586,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -548,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:J10"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -871,23 +921,23 @@
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="C1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="2:14" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>125</v>
+      <c r="C2" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -899,10 +949,10 @@
     </row>
     <row r="3" spans="2:14" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -916,8 +966,8 @@
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>127</v>
+      <c r="C4" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -931,23 +981,23 @@
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="C5" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="2:14" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -959,10 +1009,10 @@
     </row>
     <row r="7" spans="2:14" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -974,25 +1024,25 @@
     </row>
     <row r="8" spans="2:14" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+        <v>129</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="2:14" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -1006,8 +1056,8 @@
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>132</v>
+      <c r="C10" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -1021,8 +1071,8 @@
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>133</v>
+      <c r="C11" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -1036,8 +1086,8 @@
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>134</v>
+      <c r="C12" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1051,16 +1101,16 @@
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="C13" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="2:14" s="6" customFormat="1"/>
     <row r="15" spans="2:14">
@@ -1264,7 +1314,7 @@
         <v>4</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="45">
@@ -1312,7 +1362,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>11</v>
@@ -1839,44 +1889,44 @@
     </row>
     <row r="37" spans="2:14" ht="105">
       <c r="B37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="30">
       <c r="B38" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1885,24 +1935,24 @@
         <v>1</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="2:14" ht="75">
       <c r="B39" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>54</v>
@@ -1919,20 +1969,18 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="2:14" ht="60">
       <c r="B40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
         <v>54</v>
       </c>
@@ -1946,7 +1994,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1968,17 +2016,34 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B5:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
EPBDS change property values to ObjectValue. Write date prop values to excel with date format of cell.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="139">
   <si>
     <t>name</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>org.openl.rules.table.properties</t>
+  </si>
+  <si>
+    <t>MM/dd/yyyy</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,9 +614,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -651,7 +654,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -721,7 +724,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -897,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1381,7 +1384,9 @@
       <c r="K22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="M22" s="3" t="s">
         <v>83</v>
       </c>
@@ -1416,7 +1421,9 @@
       <c r="K23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="4"/>
+      <c r="L23" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="M23" s="3" t="s">
         <v>83</v>
       </c>
@@ -1486,7 +1493,9 @@
       <c r="K25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="4"/>
+      <c r="L25" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="M25" s="3" t="s">
         <v>12</v>
       </c>
@@ -1556,7 +1565,9 @@
       <c r="K27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="M27" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-646 Updated methods overload feature.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="148">
   <si>
     <t>name</t>
   </si>
@@ -477,6 +477,33 @@
   </si>
   <si>
     <t>org.openl.rules.table.properties</t>
+  </si>
+  <si>
+    <t>Data ContextPropertyDefinition contextDefinitions</t>
+  </si>
+  <si>
+    <t>currentDate</t>
+  </si>
+  <si>
+    <t>org.openl.rules.context.properties</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>dimensional</t>
+  </si>
+  <si>
+    <t>Is Business Dimension</t>
+  </si>
+  <si>
+    <t>Match expression</t>
+  </si>
+  <si>
+    <t>tableProperties.getExpirationDate().compareTo(context.getCurrentDate())  &gt;= 0</t>
+  </si>
+  <si>
+    <t>tableProperties.getEffectiveDate().compareTo(context.getCurrentDate())  &lt;= 0</t>
   </si>
   <si>
     <t>MM/dd/yyyy</t>
@@ -524,7 +551,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -556,11 +583,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -579,9 +643,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,9 +665,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,9 +693,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -654,7 +733,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -724,7 +803,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -898,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:N40"/>
+  <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -911,229 +990,233 @@
     <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="8" width="18.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37" style="1" customWidth="1"/>
+    <col min="7" max="8" width="18.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="33" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
     <col min="12" max="13" width="11.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="25.140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="6" customFormat="1" ht="11.25" customHeight="1">
+    <row r="1" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-    </row>
-    <row r="2" spans="2:14" s="6" customFormat="1" ht="11.25" customHeight="1">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="2:14" ht="57.75" customHeight="1">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="2:14" s="6" customFormat="1" ht="22.5" customHeight="1">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="2:14" s="6" customFormat="1" ht="22.5" customHeight="1">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="2:14" s="6" customFormat="1" ht="51.75" customHeight="1">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="2:14" ht="42.75" customHeight="1">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="2:14" ht="33" customHeight="1">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="2:14" s="6" customFormat="1" ht="33" customHeight="1">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="2:14" s="6" customFormat="1" ht="33" customHeight="1">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="2:14" s="6" customFormat="1">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="2:14" s="6" customFormat="1">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="2:14" s="6" customFormat="1"/>
-    <row r="15" spans="2:14">
-      <c r="B15" s="7" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" s="6" customFormat="1"/>
+    <row r="15" spans="2:16" ht="15" customHeight="1">
+      <c r="B15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="2:14">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+    </row>
+    <row r="16" spans="2:16" ht="30">
       <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1147,34 +1230,40 @@
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="30">
+    <row r="17" spans="2:16" ht="45">
       <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
@@ -1188,34 +1277,40 @@
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="30">
+    <row r="18" spans="2:16" ht="30">
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1228,29 +1323,33 @@
       <c r="E18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3" t="s">
+      <c r="J18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N18" s="3" t="s">
+      <c r="N18" s="4"/>
+      <c r="O18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="75">
+    <row r="19" spans="2:16" ht="105">
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
@@ -1263,29 +1362,33 @@
       <c r="E19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L19" s="4"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="P19" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:14" s="6" customFormat="1" ht="30">
+    <row r="20" spans="2:16" s="6" customFormat="1" ht="30">
       <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1298,29 +1401,33 @@
       <c r="E20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L20" s="4"/>
+      <c r="J20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
       <c r="M20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="N20" s="4"/>
+      <c r="O20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="45">
+    <row r="21" spans="2:16" ht="45">
       <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1333,31 +1440,35 @@
       <c r="E21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="4" t="s">
+      <c r="J21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N21" s="3" t="s">
+      <c r="O21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="90">
+    <row r="22" spans="2:16" ht="90">
       <c r="B22" s="3" t="s">
         <v>93</v>
       </c>
@@ -1371,30 +1482,36 @@
         <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>97</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="P22" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="30">
+    <row r="23" spans="2:16" ht="60">
       <c r="B23" s="3" t="s">
         <v>94</v>
       </c>
@@ -1408,30 +1525,36 @@
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>97</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="M23" s="3" t="s">
+      <c r="N23" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="P23" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="45">
+    <row r="24" spans="2:16" ht="30">
       <c r="B24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1444,29 +1567,33 @@
       <c r="E24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" s="4"/>
+      <c r="J24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="P24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:14" ht="45">
+    <row r="25" spans="2:16" ht="30">
       <c r="B25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1479,31 +1606,35 @@
       <c r="E25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="J25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
       <c r="M25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="P25" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:16">
       <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
@@ -1516,29 +1647,33 @@
       <c r="E26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="4"/>
+      <c r="I26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
       <c r="M26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N26" s="4"/>
+      <c r="O26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="30">
+    <row r="27" spans="2:16" ht="30">
       <c r="B27" s="3" t="s">
         <v>34</v>
       </c>
@@ -1551,31 +1686,35 @@
       <c r="E27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="I27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
       <c r="M27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="N27" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:14" ht="45">
+    <row r="28" spans="2:16" ht="60">
       <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1588,29 +1727,33 @@
       <c r="E28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="I28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="P28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:14" ht="45">
+    <row r="29" spans="2:16" ht="45">
       <c r="B29" s="4" t="s">
         <v>58</v>
       </c>
@@ -1623,31 +1766,35 @@
       <c r="E29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="I29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="P29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="2:14" ht="75">
+    <row r="30" spans="2:16" ht="105">
       <c r="B30" s="4" t="s">
         <v>63</v>
       </c>
@@ -1660,29 +1807,33 @@
       <c r="E30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="I30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="J30" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3" t="s">
+      <c r="N30" s="3"/>
+      <c r="O30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="4" t="s">
+      <c r="P30" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="2:14" ht="75">
+    <row r="31" spans="2:16" ht="105">
       <c r="B31" s="4" t="s">
         <v>68</v>
       </c>
@@ -1695,29 +1846,33 @@
       <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="P31" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:14" ht="75">
+    <row r="32" spans="2:16" ht="105">
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
@@ -1730,31 +1885,35 @@
       <c r="E32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="4" t="s">
+      <c r="I32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3" t="s">
+      <c r="K32" s="3"/>
+      <c r="L32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3" t="s">
+      <c r="N32" s="3"/>
+      <c r="O32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="P32" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="30">
+    <row r="33" spans="2:16" ht="30">
       <c r="B33" s="4" t="s">
         <v>70</v>
       </c>
@@ -1767,31 +1926,35 @@
       <c r="E33" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3" t="s">
+      <c r="I33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3" t="s">
+      <c r="N33" s="3"/>
+      <c r="O33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="P33" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:14" ht="30">
+    <row r="34" spans="2:16" ht="30">
       <c r="B34" s="4" t="s">
         <v>71</v>
       </c>
@@ -1804,31 +1967,35 @@
       <c r="E34" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3" t="s">
+      <c r="I34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="M34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3" t="s">
+      <c r="N34" s="3"/>
+      <c r="O34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="P34" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="2:14" ht="75">
+    <row r="35" spans="2:16" ht="105">
       <c r="B35" s="4" t="s">
         <v>72</v>
       </c>
@@ -1841,29 +2008,33 @@
       <c r="E35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N35" s="4" t="s">
+      <c r="P35" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="2:14" ht="75">
+    <row r="36" spans="2:16" ht="105">
       <c r="B36" s="4" t="s">
         <v>67</v>
       </c>
@@ -1876,29 +2047,33 @@
       <c r="E36" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N36" s="4" t="s">
+      <c r="P36" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="105">
+    <row r="37" spans="2:16" ht="105">
       <c r="B37" s="3" t="s">
         <v>107</v>
       </c>
@@ -1909,23 +2084,27 @@
       <c r="E37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="3" t="s">
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3" t="s">
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="2:14" ht="30">
+    <row r="38" spans="2:16" ht="60">
       <c r="B38" s="3" t="s">
         <v>109</v>
       </c>
@@ -1936,25 +2115,29 @@
       <c r="E38" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="3"/>
+      <c r="G38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="3" t="b">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="M38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3" t="s">
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="75">
+    <row r="39" spans="2:16" ht="75">
       <c r="B39" s="3" t="s">
         <v>114</v>
       </c>
@@ -1965,25 +2148,27 @@
       <c r="E39" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J39" s="3" t="b">
+      <c r="L39" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
       <c r="M39" s="3"/>
-      <c r="N39" s="3" t="s">
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="60">
+    <row r="40" spans="2:16" ht="60">
       <c r="B40" s="3" t="s">
         <v>115</v>
       </c>
@@ -1991,26 +2176,38 @@
         <v>117</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
+      <c r="E40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-      <c r="N40" s="3" t="s">
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="B15:O15"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C7:J7"/>
@@ -2018,12 +2215,6 @@
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2033,10 +2224,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:C6"/>
+  <dimension ref="B5:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2047,26 +2238,89 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
         <v>136</v>
       </c>
       <c r="C6" t="s">
         <v>137</v>
       </c>
     </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="16"/>
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:B7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15" customHeight="1">
+      <c r="B2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS description for format property added
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -445,9 +445,6 @@
     <t>-validation constraints, applied in validation phase</t>
   </si>
   <si>
-    <t>-properties format,  used in to display,  edit and validate</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">-if property is inheritable, shows possible levels of inheritnce; possible levels:  </t>
     </r>
@@ -508,12 +505,28 @@
   <si>
     <t>MM/dd/yyyy</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">-properties format,  used in to display,  edit and validate. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For all the properties with type Date format must be declared.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +554,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -644,25 +665,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -670,6 +676,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -685,7 +706,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,9 +714,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -733,7 +754,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -803,7 +824,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -979,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1006,215 +1027,215 @@
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="C9" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="C11" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="C12" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="C13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:16" s="6" customFormat="1"/>
     <row r="15" spans="2:16" ht="15" customHeight="1">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" spans="2:16" ht="30">
       <c r="B16" s="2" t="s">
@@ -1230,10 +1251,10 @@
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>50</v>
@@ -1277,10 +1298,10 @@
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>51</v>
@@ -1482,7 +1503,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>97</v>
@@ -1502,7 +1523,7 @@
         <v>19</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>83</v>
@@ -1525,7 +1546,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>97</v>
@@ -1545,7 +1566,7 @@
         <v>19</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>83</v>
@@ -1625,7 +1646,7 @@
         <v>4</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>12</v>
@@ -1705,7 +1726,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>4</v>
@@ -2201,6 +2222,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="B15:O15"/>
     <mergeCell ref="C8:J8"/>
@@ -2208,13 +2236,6 @@
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2234,21 +2255,21 @@
   <sheetData>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
         <v>136</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="16"/>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2277,7 +2298,7 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
       <c r="B2" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="19"/>
@@ -2306,7 +2327,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
EPBDS notes for Integer and Double types
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="149">
   <si>
     <t>name</t>
   </si>
@@ -521,12 +521,15 @@
       <t>For all the properties with type Date format must be declared.</t>
     </r>
   </si>
+  <si>
+    <t>NOTE!! Now there is no properties of type Integer and Double in definitions. When they appear, our functionality must be improved to work with it.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,6 +564,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -645,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -665,10 +675,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -676,21 +701,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -702,6 +712,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1000,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:J11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,7 +1025,8 @@
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="37" style="1" customWidth="1"/>
-    <col min="7" max="8" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
@@ -1027,215 +1041,225 @@
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
     </row>
     <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="2:16" s="6" customFormat="1"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B14" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+    </row>
     <row r="15" spans="2:16" ht="15" customHeight="1">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
     </row>
     <row r="16" spans="2:16" ht="30">
       <c r="B16" s="2" t="s">
@@ -2221,7 +2245,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="B15:O15"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="B14:H14"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C7:J7"/>
@@ -2229,13 +2261,6 @@
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="B15:O15"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-646 Updated method overload feature: added Velocity base code generation, updated implementation of the feature.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -497,12 +497,6 @@
     <t>Match expression</t>
   </si>
   <si>
-    <t>tableProperties.getExpirationDate().compareTo(context.getCurrentDate())  &gt;= 0</t>
-  </si>
-  <si>
-    <t>tableProperties.getEffectiveDate().compareTo(context.getCurrentDate())  &lt;= 0</t>
-  </si>
-  <si>
     <t>MM/dd/yyyy</t>
   </si>
   <si>
@@ -523,6 +517,12 @@
   </si>
   <si>
     <t>NOTE!! Now there is no properties of type Integer and Double in definitions. When they appear, our functionality must be improved to work with it.</t>
+  </si>
+  <si>
+    <t>le(currentDate)</t>
+  </si>
+  <si>
+    <t>gt(currentDate)</t>
   </si>
 </sst>
 </file>
@@ -675,25 +675,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -701,6 +686,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,12 +717,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -727,9 +727,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -767,7 +767,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -837,7 +837,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:H14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1024,7 +1024,7 @@
     <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="37" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
@@ -1041,225 +1041,225 @@
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="C11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B14" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="B14" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" spans="2:16" ht="30">
       <c r="B16" s="2" t="s">
@@ -1527,7 +1527,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>97</v>
@@ -1547,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>83</v>
@@ -1570,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>97</v>
@@ -1590,7 +1590,7 @@
         <v>19</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>83</v>
@@ -1670,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>12</v>
@@ -1750,7 +1750,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>4</v>
@@ -2246,6 +2246,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="B15:O15"/>
     <mergeCell ref="C8:J8"/>
@@ -2254,13 +2261,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="B14:H14"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2284,7 +2284,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>135</v>
       </c>
       <c r="C6" t="s">
@@ -2292,7 +2292,7 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" t="s">
         <v>139</v>
       </c>
@@ -2322,11 +2322,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="2" t="s">

</xml_diff>

<commit_message>
EPBDS: Updated table properties definitions. Added method overload support tests for TestMethod and RunMethod components.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <author>Stanislav Shor</author>
   </authors>
   <commentList>
-    <comment ref="E40" authorId="0">
+    <comment ref="E41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="156">
   <si>
     <t>name</t>
   </si>
@@ -524,17 +524,54 @@
   <si>
     <t>gt(currentDate)</t>
   </si>
+  <si>
+    <t>eq(lob)</t>
+  </si>
+  <si>
+    <t>eq(usRegion)</t>
+  </si>
+  <si>
+    <t>eq(country)</t>
+  </si>
+  <si>
+    <t>eq(usState)</t>
+  </si>
+  <si>
+    <t>usRegion</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>usState</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -574,15 +611,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -651,16 +693,211 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -669,33 +906,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -717,9 +987,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1011,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P40"/>
+  <dimension ref="B1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1041,365 +1321,338 @@
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B14" s="13" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+    </row>
+    <row r="14" spans="2:16" s="7" customFormat="1">
+      <c r="B14" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="2:16" ht="15" customHeight="1">
-      <c r="B15" s="9" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:16" ht="15" customHeight="1">
+      <c r="B16" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-    </row>
-    <row r="16" spans="2:16" ht="30">
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+    </row>
+    <row r="17" spans="2:16" ht="30">
+      <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="45">
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="2:16" ht="45">
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="30">
-      <c r="B18" s="3" t="s">
+    <row r="19" spans="2:16" ht="30">
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="105">
-      <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>4</v>
@@ -1417,28 +1670,28 @@
       <c r="I19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>101</v>
+      <c r="J19" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" s="6" customFormat="1" ht="30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="105">
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
@@ -1457,7 +1710,7 @@
         <v>97</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1466,18 +1719,18 @@
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" s="6" customFormat="1" ht="30">
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>4</v>
@@ -1495,7 +1748,7 @@
       <c r="I21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K21" s="3"/>
@@ -1503,37 +1756,33 @@
       <c r="M21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="N21" s="4"/>
       <c r="O21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="90">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="45">
       <c r="B22" s="3" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>147</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>97</v>
@@ -1544,33 +1793,33 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" ht="60">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="90">
       <c r="B23" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>97</v>
@@ -1596,28 +1845,30 @@
         <v>83</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" ht="30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="60">
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="G24" s="3" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>97</v>
@@ -1628,28 +1879,30 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N24" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="O24" s="3" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="30">
       <c r="B25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
@@ -1669,28 +1922,26 @@
       <c r="M25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="4" t="s">
-        <v>144</v>
-      </c>
+      <c r="N25" s="4"/>
       <c r="O25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="30">
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
@@ -1700,7 +1951,7 @@
         <v>52</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>4</v>
@@ -1710,26 +1961,28 @@
       <c r="M26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N26" s="4"/>
+      <c r="N26" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="O26" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" ht="30">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
@@ -1749,35 +2002,33 @@
       <c r="M27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="4" t="s">
-        <v>144</v>
-      </c>
+      <c r="N27" s="4"/>
       <c r="O27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" ht="60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="30">
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>4</v>
@@ -1788,22 +2039,24 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N28" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="O28" s="3" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" ht="45">
-      <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="60">
+      <c r="B29" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>4</v>
@@ -1824,66 +2077,66 @@
       <c r="J29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" ht="105">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="45">
       <c r="B30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="L30" s="3"/>
-      <c r="M30" s="4" t="s">
-        <v>65</v>
+      <c r="M30" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P30" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="105">
       <c r="B31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>4</v>
@@ -1891,9 +2144,11 @@
       <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="G31" s="4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>53</v>
@@ -1906,23 +2161,23 @@
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="3" t="s">
-        <v>78</v>
+      <c r="M31" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="105">
       <c r="B32" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>4</v>
@@ -1930,40 +2185,40 @@
       <c r="E32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="G32" s="4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>101</v>
       </c>
       <c r="K32" s="3"/>
-      <c r="L32" s="3" t="s">
-        <v>90</v>
-      </c>
+      <c r="L32" s="3"/>
       <c r="M32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3" t="s">
         <v>83</v>
       </c>
       <c r="P32" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="105">
+      <c r="B33" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" ht="30">
-      <c r="B33" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>4</v>
@@ -1971,9 +2226,11 @@
       <c r="E33" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="G33" s="4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>53</v>
@@ -1982,29 +2239,29 @@
         <v>4</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3" t="s">
         <v>83</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="30">
       <c r="B34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>4</v>
@@ -2027,64 +2284,66 @@
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
         <v>83</v>
       </c>
       <c r="P34" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" ht="30">
+      <c r="B35" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" ht="105">
-      <c r="B35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>77</v>
+      <c r="C35" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3" t="s">
+      <c r="F35" s="4"/>
+      <c r="G35" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="L35" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="M35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="s">
         <v>83</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="105">
       <c r="B36" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>4</v>
@@ -2092,9 +2351,11 @@
       <c r="E36" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="G36" s="3" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>53</v>
@@ -2108,24 +2369,26 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3" t="s">
         <v>83</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="105">
-      <c r="B37" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="3"/>
+      <c r="B37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="E37" s="3" t="s">
         <v>1</v>
       </c>
@@ -2133,32 +2396,38 @@
       <c r="G37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="H37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" ht="60">
+      <c r="O37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" ht="105">
       <c r="B38" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
@@ -2170,55 +2439,55 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="L38" s="3"/>
       <c r="M38" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" ht="75">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="60">
       <c r="B39" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
         <v>112</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="H39" s="3" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
-      <c r="K39" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="K39" s="3"/>
       <c r="L39" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M39" s="3"/>
+      <c r="M39" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" ht="60">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="75">
       <c r="B40" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
@@ -2236,11 +2505,44 @@
       <c r="K40" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L40" s="3"/>
+      <c r="L40" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" ht="60">
+      <c r="B41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2253,14 +2555,14 @@
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:J5"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B16:P16"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="B15:O15"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
-    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2284,7 +2586,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="28" t="s">
         <v>135</v>
       </c>
       <c r="C6" t="s">
@@ -2292,7 +2594,7 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="17"/>
+      <c r="B7" s="28"/>
       <c r="C7" t="s">
         <v>139</v>
       </c>
@@ -2309,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2322,11 +2624,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="2" t="s">
@@ -2351,17 +2653,60 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" customHeight="1"/>
+    <row r="6" spans="2:4">
+      <c r="B6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>

</xml_diff>

<commit_message>
EPBDS - added "scope" property
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -544,6 +544,24 @@
   </si>
   <si>
     <t>usState</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>xls.props</t>
+  </si>
+  <si>
+    <t>Worksheet, Workbook, Module</t>
+  </si>
+  <si>
+    <t>Use in properties table to provide scope of the properties</t>
   </si>
 </sst>
 </file>
@@ -892,7 +910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -945,6 +963,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -958,24 +1006,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -986,15 +1016,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1291,10 +1312,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P41"/>
+  <dimension ref="B1:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1324,13 +1347,13 @@
       <c r="C1" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
@@ -1339,28 +1362,28 @@
       <c r="C2" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
@@ -1369,13 +1392,13 @@
       <c r="C4" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
@@ -1396,61 +1419,61 @@
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
@@ -1459,71 +1482,71 @@
       <c r="C10" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
     </row>
     <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="2:16" s="7" customFormat="1">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1535,23 +1558,23 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
     </row>
     <row r="17" spans="2:16" ht="30">
       <c r="B17" s="2" t="s">
@@ -2546,15 +2569,43 @@
         <v>119</v>
       </c>
     </row>
+    <row r="42" spans="2:16" ht="45">
+      <c r="B42" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="K42" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="O42" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P42" s="18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16">
+      <c r="P43" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
     <mergeCell ref="B14:J14"/>
     <mergeCell ref="B16:P16"/>
     <mergeCell ref="C13:J13"/>
@@ -2563,6 +2614,13 @@
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2586,7 +2644,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="32" t="s">
         <v>135</v>
       </c>
       <c r="C6" t="s">
@@ -2594,7 +2652,7 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="28"/>
+      <c r="B7" s="32"/>
       <c r="C7" t="s">
         <v>139</v>
       </c>
@@ -2611,7 +2669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2624,11 +2682,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="2" t="s">
@@ -2686,13 +2744,13 @@
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="21" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-784 Added java enum types generation.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="171">
   <si>
     <t>name</t>
   </si>
@@ -563,12 +564,39 @@
   <si>
     <t>Use in properties table to provide scope of the properties</t>
   </si>
+  <si>
+    <t>Data EnumPropertyDefinition countries</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display name</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>org.openl.rules.enumeration.properties</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,8 +656,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -639,6 +674,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -910,7 +963,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -975,36 +1028,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1016,6 +1069,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1314,10 +1379,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1344,52 +1409,52 @@
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="28" t="s">
         <v>125</v>
       </c>
       <c r="D4" s="27"/>
@@ -1404,46 +1469,46 @@
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
@@ -1452,13 +1517,13 @@
       <c r="C8" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
@@ -1479,7 +1544,7 @@
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>130</v>
       </c>
       <c r="D10" s="27"/>
@@ -1494,7 +1559,7 @@
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="25" t="s">
         <v>145</v>
       </c>
       <c r="D11" s="27"/>
@@ -1509,7 +1574,7 @@
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="25" t="s">
         <v>131</v>
       </c>
       <c r="D12" s="27"/>
@@ -1524,29 +1589,29 @@
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="2:16" s="7" customFormat="1">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1558,23 +1623,23 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
     </row>
     <row r="17" spans="2:16" ht="30">
       <c r="B17" s="2" t="s">
@@ -2606,6 +2671,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
     <mergeCell ref="B14:J14"/>
     <mergeCell ref="B16:P16"/>
     <mergeCell ref="C13:J13"/>
@@ -2614,13 +2686,6 @@
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2630,10 +2695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:C7"/>
+  <dimension ref="B5:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2657,9 +2722,15 @@
         <v>139</v>
       </c>
     </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="32"/>
+      <c r="C8" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2772,4 +2843,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="43"/>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-849 Implement Constraint model Add validation of effective and expiration dates
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="173">
   <si>
     <t>name</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>constraints</t>
-  </si>
-  <si>
-    <t>effectiveDate &lt; expirationDate</t>
   </si>
   <si>
     <t>buildPhase</t>
@@ -590,6 +587,15 @@
   </si>
   <si>
     <t>org.openl.rules.enumeration.properties</t>
+  </si>
+  <si>
+    <t>org.openl.rules.table.constraints</t>
+  </si>
+  <si>
+    <t>&lt; expirationDate</t>
+  </si>
+  <si>
+    <t>&gt; effectiveDate</t>
   </si>
 </sst>
 </file>
@@ -1028,54 +1034,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1084,8 +1090,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Текст предупреждения" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1093,9 +1099,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1133,7 +1139,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1203,7 +1209,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1379,10 +1385,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1398,7 +1404,8 @@
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="11.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="25.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="26.85546875" style="1" customWidth="1"/>
@@ -1407,211 +1414,211 @@
   <sheetData>
     <row r="1" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+        <v>38</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="C2" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="2:16" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+        <v>101</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+        <v>39</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+        <v>50</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+        <v>102</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
     </row>
     <row r="7" spans="2:16" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="2:16" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
     </row>
     <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+        <v>87</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
     </row>
     <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+        <v>40</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
     </row>
     <row r="12" spans="2:16" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
     </row>
     <row r="13" spans="2:16" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
+        <v>44</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="2:16" s="7" customFormat="1">
-      <c r="B14" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="B14" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1623,57 +1630,57 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1">
-      <c r="B16" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
+      <c r="B16" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
     </row>
     <row r="17" spans="2:16" ht="30">
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>18</v>
@@ -1685,54 +1692,54 @@
         <v>3</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="45">
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="30">
@@ -1753,10 +1760,10 @@
         <v>4</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>4</v>
@@ -1764,19 +1771,19 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="105">
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -1792,13 +1799,13 @@
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1810,15 +1817,15 @@
         <v>6</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="6" customFormat="1" ht="30">
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>4</v>
@@ -1831,10 +1838,10 @@
         <v>4</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>4</v>
@@ -1849,12 +1856,12 @@
         <v>4</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="45">
       <c r="B22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>7</v>
@@ -1870,10 +1877,10 @@
         <v>4</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>4</v>
@@ -1890,33 +1897,33 @@
         <v>4</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="90">
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>4</v>
@@ -1924,21 +1931,21 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3" t="s">
-        <v>19</v>
+        <v>171</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" ht="60">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="30">
       <c r="B24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>13</v>
@@ -1950,16 +1957,16 @@
         <v>11</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>4</v>
@@ -1967,21 +1974,21 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3" t="s">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="30">
       <c r="B25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>14</v>
@@ -1997,10 +2004,10 @@
         <v>4</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>4</v>
@@ -2015,12 +2022,12 @@
         <v>12</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="30">
       <c r="B26" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>16</v>
@@ -2036,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>4</v>
@@ -2050,21 +2057,21 @@
         <v>4</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:16">
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
@@ -2077,7 +2084,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>4</v>
@@ -2095,12 +2102,12 @@
         <v>4</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="30">
       <c r="B28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>17</v>
@@ -2116,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>4</v>
@@ -2130,21 +2137,21 @@
         <v>4</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="60">
       <c r="B29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>4</v>
@@ -2157,7 +2164,7 @@
         <v>4</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>4</v>
@@ -2168,22 +2175,22 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="45">
       <c r="B30" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
@@ -2196,7 +2203,7 @@
         <v>4</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>4</v>
@@ -2205,26 +2212,26 @@
         <v>4</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="105">
       <c r="B31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>4</v>
@@ -2233,39 +2240,39 @@
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="105">
       <c r="B32" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>4</v>
@@ -2274,39 +2281,39 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="105">
       <c r="B33" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>4</v>
@@ -2315,41 +2322,41 @@
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="30">
       <c r="B34" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>4</v>
@@ -2362,7 +2369,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>4</v>
@@ -2372,25 +2379,25 @@
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="30">
       <c r="B35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>4</v>
@@ -2403,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>4</v>
@@ -2413,25 +2420,25 @@
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="105">
       <c r="B36" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>4</v>
@@ -2440,39 +2447,39 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="105">
       <c r="B37" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>4</v>
@@ -2485,33 +2492,33 @@
         <v>4</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="2:16" ht="105">
       <c r="B38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
@@ -2522,38 +2529,38 @@
         <v>4</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="2:16" ht="60">
       <c r="B39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -2562,36 +2569,36 @@
         <v>1</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="2:16" ht="75">
       <c r="B40" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L40" s="3" t="b">
         <v>1</v>
@@ -2600,46 +2607,46 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="2:16" ht="60">
       <c r="B41" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="2:16" ht="45">
       <c r="B42" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>156</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>157</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>1</v>
@@ -2648,22 +2655,22 @@
         <v>4</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I42" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="K42" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="K42" s="18" t="s">
+      <c r="M42" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="M42" s="18" t="s">
+      <c r="O42" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P42" s="18" t="s">
         <v>160</v>
-      </c>
-      <c r="O42" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="P42" s="18" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="43" spans="2:16">
@@ -2671,13 +2678,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
     <mergeCell ref="B14:J14"/>
     <mergeCell ref="B16:P16"/>
     <mergeCell ref="C13:J13"/>
@@ -2686,6 +2686,13 @@
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2695,42 +2702,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:C8"/>
+  <dimension ref="B5:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="38" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="32" t="s">
+      <c r="C6" t="s">
         <v>135</v>
       </c>
-      <c r="C6" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="32"/>
+      <c r="B7" s="38"/>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="32"/>
+      <c r="B8" s="38"/>
       <c r="C8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="38"/>
+      <c r="C9" t="s">
         <v>170</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2753,11 +2766,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="2" t="s">
@@ -2767,7 +2780,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -2775,15 +2788,15 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>11</v>
@@ -2794,46 +2807,46 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2849,7 +2862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2861,48 +2874,48 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="43"/>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="43"/>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="36" t="s">
+      <c r="C5" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="37" t="s">
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="39" t="s">
+    <row r="7" spans="2:3">
+      <c r="B7" s="24" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="38" t="s">
+      <c r="C7" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="39" t="s">
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="40" t="s">
+      <c r="C8" s="27" t="s">
         <v>168</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-909 System properties definitions added. Changes in gen process.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -596,6 +596,33 @@
   </si>
   <si>
     <t>&gt; effectiveDate</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>currentUser</t>
+  </si>
+  <si>
+    <t>Save policy for property system value</t>
+  </si>
+  <si>
+    <t>Is set by system?</t>
+  </si>
+  <si>
+    <t>policyEnum</t>
+  </si>
+  <si>
+    <t>IF_BLANK_ONLY</t>
+  </si>
+  <si>
+    <t>ON_EACH_EDIT</t>
+  </si>
+  <si>
+    <t>systemValueDescriptor</t>
+  </si>
+  <si>
+    <t>Property system value descriptor</t>
   </si>
 </sst>
 </file>
@@ -670,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,6 +727,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -969,7 +1002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1040,6 +1073,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1383,12 +1422,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P43"/>
+  <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1402,225 +1441,270 @@
     <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="26.85546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="13.140625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="28" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="28" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
+    <row r="1" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-    </row>
-    <row r="2" spans="2:16" s="6" customFormat="1" ht="11.25" customHeight="1">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+    </row>
+    <row r="2" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-    </row>
-    <row r="3" spans="2:16" ht="57.75" customHeight="1">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+    </row>
+    <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="2:16" s="6" customFormat="1" ht="22.5" customHeight="1">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+    </row>
+    <row r="5" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-    </row>
-    <row r="6" spans="2:16" s="6" customFormat="1" ht="51.75" customHeight="1">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-    </row>
-    <row r="7" spans="2:16" ht="42.75" customHeight="1">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+    </row>
+    <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="2:16" ht="33" customHeight="1">
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+    </row>
+    <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-    </row>
-    <row r="9" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+    </row>
+    <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="2:16" s="6" customFormat="1" ht="33" customHeight="1">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+    </row>
+    <row r="10" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="2:16">
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+    </row>
+    <row r="11" spans="2:19">
       <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="2:16" s="6" customFormat="1">
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+    </row>
+    <row r="12" spans="2:19" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="2:16" s="6" customFormat="1">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+    </row>
+    <row r="13" spans="2:19" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-    </row>
-    <row r="14" spans="2:16" s="7" customFormat="1">
-      <c r="B14" s="34" t="s">
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+    </row>
+    <row r="14" spans="2:19" s="7" customFormat="1">
+      <c r="B14" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="2:16" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+    </row>
+    <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1628,27 +1712,33 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="2:16" ht="15" customHeight="1">
-      <c r="B16" s="35" t="s">
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="2:19" ht="15" customHeight="1">
+      <c r="B16" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-    </row>
-    <row r="17" spans="2:16" ht="30">
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+    </row>
+    <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1674,28 +1764,37 @@
         <v>91</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="R17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="S17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="45">
+    <row r="18" spans="2:19" ht="45">
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1721,28 +1820,37 @@
         <v>97</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="Q18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="30">
+    <row r="19" spans="2:19" ht="30">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1765,23 +1873,28 @@
       <c r="I19" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="M19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q19" s="4"/>
+      <c r="R19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S19" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="105">
+    <row r="20" spans="2:19" ht="105">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1804,23 +1917,28 @@
       <c r="I20" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="3" t="s">
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="S20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:16" s="6" customFormat="1" ht="30">
+    <row r="21" spans="2:19" s="6" customFormat="1" ht="30">
       <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1843,23 +1961,28 @@
       <c r="I21" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="L21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
       <c r="P21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="45">
+    <row r="22" spans="2:19" ht="45">
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1882,25 +2005,30 @@
       <c r="I22" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="M22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P22" s="3" t="s">
+      <c r="R22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="90">
+    <row r="23" spans="2:19" ht="90">
       <c r="B23" s="3" t="s">
         <v>92</v>
       </c>
@@ -1925,25 +2053,30 @@
       <c r="I23" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="M23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="Q23" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="R23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="S23" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="30">
+    <row r="24" spans="2:19" ht="30">
       <c r="B24" s="3" t="s">
         <v>93</v>
       </c>
@@ -1968,25 +2101,30 @@
       <c r="I24" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="M24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="Q24" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="R24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P24" s="3" t="s">
+      <c r="S24" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="30">
+    <row r="25" spans="2:19" ht="30">
       <c r="B25" s="3" t="s">
         <v>30</v>
       </c>
@@ -2009,23 +2147,32 @@
       <c r="I25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="J25" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>96</v>
+      </c>
       <c r="M25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="3" t="s">
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="S25" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="30">
+    <row r="26" spans="2:19" ht="30">
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
@@ -2048,25 +2195,34 @@
       <c r="I26" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="J26" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="L26" s="29" t="s">
+        <v>96</v>
+      </c>
       <c r="M26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="R26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="S26" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
         <v>32</v>
       </c>
@@ -2089,23 +2245,32 @@
       <c r="I27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="J27" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>96</v>
+      </c>
       <c r="M27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="4"/>
-      <c r="O27" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
       <c r="P27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S27" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="30">
+    <row r="28" spans="2:19" ht="30">
       <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
@@ -2128,25 +2293,34 @@
       <c r="I28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="J28" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>96</v>
+      </c>
       <c r="M28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="O28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P28" s="3" t="s">
+      <c r="R28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S28" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="60">
+    <row r="29" spans="2:19" ht="45">
       <c r="B29" s="3" t="s">
         <v>34</v>
       </c>
@@ -2169,23 +2343,28 @@
       <c r="I29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="L29" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="M29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3" t="s">
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="S29" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="45">
+    <row r="30" spans="2:19" ht="45">
       <c r="B30" s="4" t="s">
         <v>57</v>
       </c>
@@ -2208,25 +2387,30 @@
       <c r="I30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="3" t="s">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3" t="s">
+      <c r="O30" s="3"/>
+      <c r="P30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3" t="s">
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P30" s="3" t="s">
+      <c r="S30" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="105">
+    <row r="31" spans="2:19" ht="105">
       <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
@@ -2251,23 +2435,28 @@
       <c r="I31" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="4" t="s">
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3" t="s">
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P31" s="4" t="s">
+      <c r="S31" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="2:16" ht="105">
+    <row r="32" spans="2:19" ht="105">
       <c r="B32" s="4" t="s">
         <v>67</v>
       </c>
@@ -2292,23 +2481,28 @@
       <c r="I32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3" t="s">
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3" t="s">
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P32" s="4" t="s">
+      <c r="S32" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="2:16" ht="105">
+    <row r="33" spans="2:19" ht="105">
       <c r="B33" s="4" t="s">
         <v>68</v>
       </c>
@@ -2333,25 +2527,30 @@
       <c r="I33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P33" s="4" t="s">
+      <c r="S33" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="2:16" ht="30">
+    <row r="34" spans="2:19" ht="30">
       <c r="B34" s="4" t="s">
         <v>69</v>
       </c>
@@ -2374,25 +2573,30 @@
       <c r="I34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K34" s="3"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
       <c r="L34" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="S34" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="2:16" ht="30">
+    <row r="35" spans="2:19" ht="30">
       <c r="B35" s="4" t="s">
         <v>70</v>
       </c>
@@ -2415,25 +2619,30 @@
       <c r="I35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="3"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
       <c r="L35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>80</v>
+        <v>4</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P35" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P35" s="4" t="s">
+      <c r="S35" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="2:16" ht="105">
+    <row r="36" spans="2:19" ht="105">
       <c r="B36" s="4" t="s">
         <v>71</v>
       </c>
@@ -2458,23 +2667,28 @@
       <c r="I36" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3" t="s">
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3" t="s">
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P36" s="4" t="s">
+      <c r="S36" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="2:16" ht="105">
+    <row r="37" spans="2:19" ht="105">
       <c r="B37" s="4" t="s">
         <v>66</v>
       </c>
@@ -2497,23 +2711,28 @@
       <c r="I37" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3" t="s">
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3" t="s">
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P37" s="4" t="s">
+      <c r="S37" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="2:16" ht="105">
+    <row r="38" spans="2:19" ht="105">
       <c r="B38" s="3" t="s">
         <v>106</v>
       </c>
@@ -2534,17 +2753,22 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="L38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="2:16" ht="60">
+    <row r="39" spans="2:19" ht="45">
       <c r="B39" s="3" t="s">
         <v>108</v>
       </c>
@@ -2565,19 +2789,24 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="3" t="b">
+      <c r="L39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M39" s="3" t="s">
+      <c r="P39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3" t="s">
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="2:16" ht="75">
+    <row r="40" spans="2:19" ht="75">
       <c r="B40" s="3" t="s">
         <v>113</v>
       </c>
@@ -2597,20 +2826,25 @@
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
-      <c r="K40" s="3" t="s">
+      <c r="K40" s="3"/>
+      <c r="L40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L40" s="3" t="b">
+      <c r="O40" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3" t="s">
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="2:16" ht="60">
+    <row r="41" spans="2:19" ht="60">
       <c r="B41" s="3" t="s">
         <v>114</v>
       </c>
@@ -2630,18 +2864,23 @@
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
-      <c r="K41" s="3" t="s">
+      <c r="K41" s="3"/>
+      <c r="L41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="3" t="s">
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="2:16" ht="45">
+    <row r="42" spans="2:19" ht="45">
       <c r="B42" s="18" t="s">
         <v>155</v>
       </c>
@@ -2660,39 +2899,42 @@
       <c r="I42" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="K42" s="18" t="s">
+      <c r="L42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="M42" s="18" t="s">
+      <c r="P42" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="O42" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="P42" s="18" t="s">
+      <c r="R42" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S42" s="18" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="2:16">
-      <c r="P43" s="18"/>
+    <row r="43" spans="2:19">
+      <c r="S43" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B16:P16"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B16:S16"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="C8:M8"/>
+    <mergeCell ref="C9:M9"/>
+    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C11:M11"/>
+    <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2716,7 +2958,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="40" t="s">
         <v>134</v>
       </c>
       <c r="C6" t="s">
@@ -2724,19 +2966,19 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="38"/>
+      <c r="B7" s="40"/>
       <c r="C7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="38"/>
+      <c r="B8" s="40"/>
       <c r="C8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="38"/>
+      <c r="B9" s="40"/>
       <c r="C9" t="s">
         <v>170</v>
       </c>
@@ -2766,11 +3008,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="2" t="s">
@@ -2873,10 +3115,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="45"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="22" t="s">

</xml_diff>

<commit_message>
EPBDS-909 code style changes
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -610,9 +610,6 @@
     <t>Is set by system?</t>
   </si>
   <si>
-    <t>policyEnum</t>
-  </si>
-  <si>
     <t>IF_BLANK_ONLY</t>
   </si>
   <si>
@@ -623,6 +620,9 @@
   </si>
   <si>
     <t>Property system value descriptor</t>
+  </si>
+  <si>
+    <t>systemValuePolicy</t>
   </si>
 </sst>
 </file>
@@ -1079,34 +1079,34 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1427,7 +1427,7 @@
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1458,61 +1458,61 @@
       <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
     </row>
     <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="36" t="s">
         <v>124</v>
       </c>
       <c r="D4" s="35"/>
@@ -1530,55 +1530,55 @@
       <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
     </row>
     <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
@@ -1587,16 +1587,16 @@
       <c r="C8" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
     </row>
     <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
@@ -1620,7 +1620,7 @@
       <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="36" t="s">
         <v>129</v>
       </c>
       <c r="D10" s="35"/>
@@ -1638,7 +1638,7 @@
       <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="33" t="s">
         <v>144</v>
       </c>
       <c r="D11" s="35"/>
@@ -1656,7 +1656,7 @@
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="33" t="s">
         <v>130</v>
       </c>
       <c r="D12" s="35"/>
@@ -1674,35 +1674,35 @@
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:19" s="7" customFormat="1">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1717,26 +1717,26 @@
       <c r="L15" s="28"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
@@ -1764,10 +1764,10 @@
         <v>91</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>173</v>
@@ -1820,7 +1820,7 @@
         <v>97</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>175</v>
@@ -2151,7 +2151,7 @@
         <v>174</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L25" s="29" t="s">
         <v>96</v>
@@ -2199,7 +2199,7 @@
         <v>137</v>
       </c>
       <c r="K26" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L26" s="29" t="s">
         <v>96</v>
@@ -2249,7 +2249,7 @@
         <v>174</v>
       </c>
       <c r="K27" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L27" s="29" t="s">
         <v>96</v>
@@ -2297,7 +2297,7 @@
         <v>137</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L28" s="29" t="s">
         <v>96</v>
@@ -2920,6 +2920,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B16:S16"/>
     <mergeCell ref="C13:M13"/>
@@ -2928,13 +2935,6 @@
     <mergeCell ref="C10:M10"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C12:M12"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-946 Level at which properties can be defined and overridden
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -62,18 +62,12 @@
     <t>type</t>
   </si>
   <si>
-    <t>inheritable</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>category</t>
   </si>
   <si>
-    <t>worksheet</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>worksheet,workbook, module</t>
-  </si>
-  <si>
     <t>expirationDate</t>
   </si>
   <si>
@@ -158,9 +149,6 @@
     <t>Build Phase</t>
   </si>
   <si>
-    <t>worksheet, workbook</t>
-  </si>
-  <si>
     <t>one of: common, vocabulary[N], main[N]</t>
   </si>
   <si>
@@ -218,9 +206,6 @@
     <t>one of: on, off, gaps, overlaps</t>
   </si>
   <si>
-    <t>worksheet, workbook, module</t>
-  </si>
-  <si>
     <t>Defines validation mode for DT</t>
   </si>
   <si>
@@ -297,9 +282,6 @@
   </si>
   <si>
     <t>list: US States</t>
-  </si>
-  <si>
-    <t>worksheet,workbook</t>
   </si>
   <si>
     <t>region</t>
@@ -623,6 +605,24 @@
   </si>
   <si>
     <t>systemValuePolicy</t>
+  </si>
+  <si>
+    <t>Level at which property can be defined and overriden</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t>CATEGORY, TABLE</t>
+  </si>
+  <si>
+    <t>MODULE, CATEGORY, TABLE</t>
+  </si>
+  <si>
+    <t>inheritanceLevel</t>
+  </si>
+  <si>
+    <t>MODULE, CATEGORY</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1077,6 +1077,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1424,10 +1427,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1456,253 +1459,253 @@
   <sheetData>
     <row r="1" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+        <v>34</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+        <v>12</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+        <v>95</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+        <v>35</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
     </row>
     <row r="5" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
     </row>
     <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+        <v>96</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+        <v>97</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
+        <v>121</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+        <v>81</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
     </row>
     <row r="10" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+        <v>36</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
+        <v>39</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
     </row>
     <row r="12" spans="2:19" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
+        <v>37</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
     </row>
     <row r="13" spans="2:19" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
     </row>
     <row r="14" spans="2:19" s="7" customFormat="1">
-      <c r="B14" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
+      <c r="B14" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1717,1027 +1720,1027 @@
       <c r="L15" s="28"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1">
-      <c r="B16" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="B16" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
     </row>
     <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="60">
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" ht="45">
-      <c r="B18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="J18" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="30">
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="3" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:19" ht="105">
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="3" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:19" s="6" customFormat="1" ht="30">
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="3" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:19" ht="45">
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:19" ht="90">
       <c r="B23" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:19" ht="30">
       <c r="B24" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="2:19" ht="30">
       <c r="B25" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J25" s="29" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L25" s="29" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="3" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:19" ht="30">
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K26" s="29" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L26" s="29" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K27" s="29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L27" s="29" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="3" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:19" ht="30">
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L28" s="29" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:19" ht="45">
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="3" t="s">
-        <v>35</v>
+        <v>179</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" ht="30">
       <c r="B30" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="3" t="s">
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="2:19" ht="105">
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="2:19" ht="105">
       <c r="B32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="2:19" ht="105">
       <c r="B33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:19" ht="30">
       <c r="B34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="2:19" ht="30">
       <c r="B35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="2:19" ht="105">
       <c r="B36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="3" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="S36" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="2:19" ht="105">
       <c r="B37" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3" t="s">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="S37" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="2:19" ht="105">
       <c r="B38" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
@@ -2745,52 +2748,54 @@
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
+      <c r="R38" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="S38" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="2:19" ht="45">
       <c r="B39" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -2798,121 +2803,127 @@
         <v>1</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
+      <c r="R39" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="S39" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="2:19" ht="75">
       <c r="B40" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O40" s="3" t="b">
         <v>1</v>
       </c>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
+      <c r="R40" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="S40" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="2:19" ht="60">
       <c r="B41" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
+      <c r="R41" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="S41" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="2:19" ht="45">
       <c r="B42" s="18" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>1</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I42" s="18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N42" s="18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="P42" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="R42" s="18" t="s">
-        <v>4</v>
+        <v>153</v>
+      </c>
+      <c r="R42" s="30" t="s">
+        <v>181</v>
       </c>
       <c r="S42" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="2:19">
@@ -2954,33 +2965,33 @@
   <sheetData>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="40" t="s">
-        <v>134</v>
+      <c r="B6" s="41" t="s">
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="40"/>
+      <c r="B7" s="41"/>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="40"/>
+      <c r="B8" s="41"/>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="40"/>
+      <c r="B9" s="41"/>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3008,11 +3019,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="2" t="s">
@@ -3022,73 +3033,73 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="19" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3115,49 +3126,49 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="45"/>
+      <c r="B3" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="24" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="24" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="26" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-946 docs, test, packages for properties classes
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,9 +453,6 @@
     <t>import</t>
   </si>
   <si>
-    <t>org.openl.rules.table.properties</t>
-  </si>
-  <si>
     <t>Data ContextPropertyDefinition contextDefinitions</t>
   </si>
   <si>
@@ -623,6 +620,9 @@
   </si>
   <si>
     <t>MODULE, CATEGORY</t>
+  </si>
+  <si>
+    <t>org.openl.rules.table.properties.def</t>
   </si>
 </sst>
 </file>
@@ -1082,6 +1082,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1092,24 +1110,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1427,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+    <sheetView topLeftCell="F10" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="R42" sqref="R42"/>
@@ -1461,61 +1461,61 @@
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
     </row>
     <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="33" t="s">
         <v>118</v>
       </c>
       <c r="D4" s="36"/>
@@ -1533,55 +1533,55 @@
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
     </row>
     <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
@@ -1590,16 +1590,16 @@
       <c r="C8" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
     </row>
     <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
@@ -1623,7 +1623,7 @@
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="33" t="s">
         <v>123</v>
       </c>
       <c r="D10" s="36"/>
@@ -1641,8 +1641,8 @@
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>138</v>
+      <c r="C11" s="40" t="s">
+        <v>137</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
@@ -1659,7 +1659,7 @@
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="40" t="s">
         <v>124</v>
       </c>
       <c r="D12" s="36"/>
@@ -1677,35 +1677,35 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:19" s="7" customFormat="1">
-      <c r="B14" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
+      <c r="B14" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
     </row>
     <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1720,26 +1720,26 @@
       <c r="L15" s="28"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
     </row>
     <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
@@ -1755,10 +1755,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>45</v>
@@ -1767,13 +1767,13 @@
         <v>85</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>92</v>
@@ -1791,7 +1791,7 @@
         <v>6</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>17</v>
@@ -1811,10 +1811,10 @@
         <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>46</v>
@@ -1823,13 +1823,13 @@
         <v>91</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>93</v>
@@ -1847,7 +1847,7 @@
         <v>39</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>40</v>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>18</v>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>19</v>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>117</v>
@@ -2025,7 +2025,7 @@
         <v>7</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S22" s="3" t="s">
         <v>20</v>
@@ -2045,7 +2045,7 @@
         <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>90</v>
@@ -2067,13 +2067,13 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S23" s="3" t="s">
         <v>21</v>
@@ -2093,7 +2093,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>90</v>
@@ -2115,13 +2115,13 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>56</v>
@@ -2151,10 +2151,10 @@
         <v>90</v>
       </c>
       <c r="J25" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L25" s="29" t="s">
         <v>90</v>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>54</v>
@@ -2199,10 +2199,10 @@
         <v>90</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K26" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L26" s="29" t="s">
         <v>90</v>
@@ -2216,10 +2216,10 @@
         <v>3</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>55</v>
@@ -2249,10 +2249,10 @@
         <v>3</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K27" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L27" s="29" t="s">
         <v>90</v>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S27" s="3" t="s">
         <v>54</v>
@@ -2297,10 +2297,10 @@
         <v>3</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L28" s="29" t="s">
         <v>90</v>
@@ -2314,10 +2314,10 @@
         <v>3</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S28" s="3" t="s">
         <v>53</v>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>23</v>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>51</v>
@@ -2427,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>90</v>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>60</v>
@@ -2473,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>90</v>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>62</v>
@@ -2519,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>90</v>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>63</v>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>64</v>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>65</v>
@@ -2659,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>90</v>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>66</v>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>79</v>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S38" s="3" t="s">
         <v>106</v>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="Q39" s="3"/>
       <c r="R39" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S39" s="3" t="s">
         <v>114</v>
@@ -2847,7 +2847,7 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S40" s="3" t="s">
         <v>113</v>
@@ -2885,7 +2885,7 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S41" s="3" t="s">
         <v>112</v>
@@ -2893,10 +2893,10 @@
     </row>
     <row r="42" spans="2:19" ht="45">
       <c r="B42" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>150</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>1</v>
@@ -2908,22 +2908,22 @@
         <v>49</v>
       </c>
       <c r="I42" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N42" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="L42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N42" s="18" t="s">
+      <c r="P42" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="P42" s="18" t="s">
+      <c r="R42" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="S42" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="R42" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="S42" s="18" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="43" spans="2:19">
@@ -2931,13 +2931,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B16:S16"/>
     <mergeCell ref="C13:M13"/>
@@ -2946,6 +2939,13 @@
     <mergeCell ref="C10:M10"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2957,8 +2957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B5:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2973,25 +2973,25 @@
         <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="41"/>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="41"/>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="41"/>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3020,7 +3020,7 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" customHeight="1">
       <c r="B2" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="44"/>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>9</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>1</v>
@@ -3099,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3127,7 +3127,7 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="46"/>
     </row>
@@ -3141,10 +3141,10 @@
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>156</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -3152,23 +3152,23 @@
         <v>83</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>159</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>161</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-782 Updated code generation: added enumerations support.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="185">
   <si>
     <t>name</t>
   </si>
@@ -270,9 +270,6 @@
   </si>
   <si>
     <t>list: East, West, Midwest, South</t>
-  </si>
-  <si>
-    <t>list: countries</t>
   </si>
   <si>
     <t>list: currencies</t>
@@ -508,9 +505,6 @@
     <t>eq(usRegion)</t>
   </si>
   <si>
-    <t>eq(country)</t>
-  </si>
-  <si>
     <t>eq(usState)</t>
   </si>
   <si>
@@ -623,6 +617,21 @@
   </si>
   <si>
     <t>org.openl.rules.table.properties.def</t>
+  </si>
+  <si>
+    <t>Enum[]</t>
+  </si>
+  <si>
+    <t>contains(country)</t>
+  </si>
+  <si>
+    <t>data: countries</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>org.openl.rules.enumeration</t>
   </si>
 </sst>
 </file>
@@ -734,7 +743,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -997,12 +1006,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1047,9 +1106,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1082,58 +1138,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Текст предупреждения" xfId="1" builtinId="11"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1141,9 +1212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1181,7 +1252,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1251,7 +1322,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1428,9 +1499,9 @@
   <dimension ref="B1:S43"/>
   <sheetViews>
     <sheetView topLeftCell="F10" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="R42" sqref="R42"/>
+      <selection pane="bottomLeft" activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1444,9 +1515,9 @@
     <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="28" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="27" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="27" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
@@ -1461,8 +1532,8 @@
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>115</v>
+      <c r="C1" s="36" t="s">
+        <v>114</v>
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
@@ -1479,116 +1550,116 @@
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
+      <c r="C2" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+        <v>94</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
     </row>
     <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
+      <c r="C4" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
     </row>
     <row r="5" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
+      <c r="C5" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
     </row>
     <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+        <v>95</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="35" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>122</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -1603,82 +1674,82 @@
     </row>
     <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
+        <v>80</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
+      <c r="C10" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
+      <c r="C11" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" spans="2:19" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
+      <c r="C12" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
     </row>
     <row r="13" spans="2:19" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>125</v>
+      <c r="C13" s="33" t="s">
+        <v>124</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -1692,20 +1763,20 @@
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:19" s="7" customFormat="1">
-      <c r="B14" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
+      <c r="B14" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1715,31 +1786,31 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
@@ -1749,40 +1820,40 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="L17" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>41</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>15</v>
@@ -1791,7 +1862,7 @@
         <v>6</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>17</v>
@@ -1805,40 +1876,40 @@
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>36</v>
@@ -1847,7 +1918,7 @@
         <v>39</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>40</v>
@@ -1874,7 +1945,7 @@
         <v>47</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1891,7 +1962,7 @@
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>18</v>
@@ -1918,7 +1989,7 @@
         <v>47</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1926,7 +1997,7 @@
         <v>3</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1935,7 +2006,7 @@
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>19</v>
@@ -1962,7 +2033,7 @@
         <v>47</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1979,10 +2050,10 @@
       </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="2:19" ht="45">
@@ -2006,7 +2077,7 @@
         <v>47</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2025,7 +2096,7 @@
         <v>7</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S22" s="3" t="s">
         <v>20</v>
@@ -2033,28 +2104,28 @@
     </row>
     <row r="23" spans="2:19" ht="90">
       <c r="B23" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2067,13 +2138,13 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S23" s="3" t="s">
         <v>21</v>
@@ -2081,7 +2152,7 @@
     </row>
     <row r="24" spans="2:19" ht="30">
       <c r="B24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
@@ -2093,16 +2164,16 @@
         <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2115,13 +2186,13 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>56</v>
@@ -2148,16 +2219,16 @@
         <v>47</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="K25" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="L25" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>3</v>
@@ -2169,7 +2240,7 @@
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>54</v>
@@ -2196,16 +2267,16 @@
         <v>47</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="K26" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="L26" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="L26" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>3</v>
@@ -2216,10 +2287,10 @@
         <v>3</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>55</v>
@@ -2248,14 +2319,14 @@
       <c r="I27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="K27" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="L27" s="29" t="s">
-        <v>90</v>
+      <c r="J27" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>3</v>
@@ -2267,7 +2338,7 @@
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S27" s="3" t="s">
         <v>54</v>
@@ -2296,14 +2367,14 @@
       <c r="I28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="K28" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="L28" s="29" t="s">
-        <v>90</v>
+      <c r="J28" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>3</v>
@@ -2314,10 +2385,10 @@
         <v>3</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S28" s="3" t="s">
         <v>53</v>
@@ -2361,7 +2432,7 @@
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>23</v>
@@ -2407,7 +2478,7 @@
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>51</v>
@@ -2427,16 +2498,16 @@
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2444,7 +2515,7 @@
         <v>3</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
@@ -2453,7 +2524,7 @@
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>60</v>
@@ -2473,16 +2544,16 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -2490,7 +2561,7 @@
         <v>3</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
@@ -2499,7 +2570,7 @@
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>62</v>
@@ -2516,13 +2587,13 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>48</v>
@@ -2536,18 +2607,16 @@
         <v>3</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N33" s="3"/>
-      <c r="O33" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>63</v>
@@ -2586,14 +2655,14 @@
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>64</v>
@@ -2632,14 +2701,14 @@
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>65</v>
@@ -2659,16 +2728,16 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2676,16 +2745,16 @@
         <v>3</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>66</v>
@@ -2696,7 +2765,7 @@
         <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>3</v>
@@ -2712,7 +2781,7 @@
         <v>48</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2720,27 +2789,27 @@
         <v>3</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S37" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="2:19" ht="105">
       <c r="B38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
@@ -2751,7 +2820,7 @@
         <v>3</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -2763,33 +2832,33 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="2:19" ht="45">
       <c r="B39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -2803,26 +2872,26 @@
         <v>1</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q39" s="3"/>
       <c r="R39" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:19" ht="75">
       <c r="B40" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
@@ -2847,22 +2916,22 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="2:19" ht="60">
       <c r="B41" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
@@ -2885,52 +2954,59 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="2:19" ht="45">
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I42" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="L42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N42" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I42" s="18" t="s">
+      <c r="P42" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="L42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N42" s="18" t="s">
+      <c r="R42" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="S42" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="P42" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="R42" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="S42" s="18" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="43" spans="2:19">
-      <c r="S43" s="18"/>
+      <c r="S43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B16:S16"/>
     <mergeCell ref="C13:M13"/>
@@ -2939,13 +3015,6 @@
     <mergeCell ref="C10:M10"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C12:M12"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2955,48 +3024,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:C9"/>
+  <dimension ref="B5:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="40" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="41" t="s">
-        <v>128</v>
-      </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="41"/>
+      <c r="B7" s="40"/>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="41"/>
+      <c r="B8" s="40"/>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="41"/>
+      <c r="B9" s="40"/>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="40"/>
+      <c r="C10" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B6:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3004,28 +3079,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="43"/>
+    <row r="2" spans="2:5" ht="15" customHeight="1">
+      <c r="B2" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="44"/>
       <c r="D2" s="44"/>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="E2" s="45"/>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3033,10 +3109,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:5">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3044,68 +3123,75 @@
         <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:5">
       <c r="B5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="46"/>
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="B6" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="47"/>
+      <c r="E6" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:5">
       <c r="B7" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="47"/>
+      <c r="E7" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="20" t="s">
+    <row r="8" spans="2:5">
+      <c r="B8" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="48"/>
+      <c r="E8" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:5">
       <c r="B9" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>146</v>
+      <c r="C9" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:D2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3126,49 +3212,49 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="42"/>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="46"/>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="22" t="s">
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="23" t="s">
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="23" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="24" t="s">
+    <row r="8" spans="2:3">
+      <c r="B8" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C8" s="26" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-860 Wizard for new Properties table
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1138,6 +1138,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1151,24 +1193,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1177,34 +1201,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Текст предупреждения" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1212,9 +1212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1252,7 +1252,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1322,7 +1322,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1498,10 +1498,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="P33" sqref="P33"/>
+      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1532,251 +1532,251 @@
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
     </row>
     <row r="2" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
     </row>
     <row r="5" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
     </row>
     <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
     </row>
     <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
     </row>
     <row r="10" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="2:19" s="6" customFormat="1">
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
     </row>
     <row r="13" spans="2:19" s="6" customFormat="1">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
     </row>
     <row r="14" spans="2:19" s="7" customFormat="1">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
     </row>
     <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1791,26 +1791,26 @@
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
     </row>
     <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
@@ -2198,7 +2198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="30">
+    <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>54</v>
@@ -2290,7 +2290,7 @@
         <v>135</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>55</v>
@@ -3000,13 +3000,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B16:S16"/>
     <mergeCell ref="C13:M13"/>
@@ -3015,6 +3008,13 @@
     <mergeCell ref="C10:M10"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3038,7 +3038,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="48" t="s">
         <v>127</v>
       </c>
       <c r="C6" t="s">
@@ -3046,25 +3046,25 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="40"/>
+      <c r="B7" s="48"/>
       <c r="C7" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="40"/>
+      <c r="B8" s="48"/>
       <c r="C8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="40"/>
+      <c r="B9" s="48"/>
       <c r="C9" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="40"/>
+      <c r="B10" s="48"/>
       <c r="C10" t="s">
         <v>184</v>
       </c>
@@ -3081,7 +3081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3094,12 +3094,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="2" t="s">
@@ -3136,7 +3136,7 @@
       <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="14" t="s">
         <v>57</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="14" t="s">
         <v>62</v>
       </c>
@@ -3172,7 +3172,7 @@
       <c r="C8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="20" t="s">
         <v>66</v>
       </c>
@@ -3181,10 +3181,10 @@
       <c r="B9" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="36" t="s">
         <v>182</v>
       </c>
       <c r="E9" s="16" t="s">
@@ -3212,10 +3212,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="50"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="21" t="s">

</xml_diff>

<commit_message>
EPBDS-781 Added currencies sample table
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Properties" sheetId="1" r:id="rId1"/>
+    <sheet name="Environment" sheetId="2" r:id="rId2"/>
+    <sheet name="Runtime Scope" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Enums" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="192">
   <si>
     <t>name</t>
   </si>
@@ -270,9 +270,6 @@
   </si>
   <si>
     <t>list: East, West, Midwest, South</t>
-  </si>
-  <si>
-    <t>list: currencies</t>
   </si>
   <si>
     <t>list: languages</t>
@@ -632,6 +629,30 @@
   </si>
   <si>
     <t>org.openl.rules.enumeration</t>
+  </si>
+  <si>
+    <t>String[]</t>
+  </si>
+  <si>
+    <t>data: currencies</t>
+  </si>
+  <si>
+    <t>Data EnumPropertyDefinition currencies</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>BYR</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>Russian Ruble</t>
+  </si>
+  <si>
+    <t>Belarusian Ruble</t>
   </si>
 </sst>
 </file>
@@ -1162,36 +1183,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1203,8 +1224,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Текст предупреждения" xfId="1" builtinId="11"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1212,9 +1233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1252,7 +1273,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1322,7 +1343,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1498,10 +1519,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="H10" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1532,62 +1553,62 @@
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
+      <c r="C1" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="2:19" s="6" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
+      <c r="C2" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+        <v>93</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="6" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>117</v>
+      <c r="C4" s="44" t="s">
+        <v>116</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43"/>
@@ -1604,80 +1625,80 @@
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
+      <c r="C5" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
     </row>
     <row r="6" spans="2:19" s="6" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+        <v>94</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
     </row>
     <row r="9" spans="2:19" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="43"/>
@@ -1694,8 +1715,8 @@
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>122</v>
+      <c r="C10" s="44" t="s">
+        <v>121</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
@@ -1712,8 +1733,8 @@
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>136</v>
+      <c r="C11" s="41" t="s">
+        <v>135</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
@@ -1730,8 +1751,8 @@
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="47" t="s">
-        <v>123</v>
+      <c r="C12" s="41" t="s">
+        <v>122</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -1748,35 +1769,35 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
+      <c r="C13" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
     </row>
     <row r="14" spans="2:19" s="7" customFormat="1">
-      <c r="B14" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
+      <c r="B14" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
     </row>
     <row r="15" spans="2:19" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="B15" s="8"/>
@@ -1791,26 +1812,26 @@
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="2:19" ht="15" customHeight="1">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
     </row>
     <row r="17" spans="2:19" ht="30">
       <c r="B17" s="2" t="s">
@@ -1820,40 +1841,40 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>45</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>41</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>15</v>
@@ -1862,7 +1883,7 @@
         <v>6</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>17</v>
@@ -1876,40 +1897,40 @@
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="M18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>36</v>
@@ -1918,7 +1939,7 @@
         <v>39</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>40</v>
@@ -1945,7 +1966,7 @@
         <v>47</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1962,7 +1983,7 @@
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>18</v>
@@ -1989,7 +2010,7 @@
         <v>47</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1997,7 +2018,7 @@
         <v>3</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -2006,7 +2027,7 @@
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>19</v>
@@ -2033,7 +2054,7 @@
         <v>47</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2050,10 +2071,10 @@
       </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="2:19" ht="45">
@@ -2067,7 +2088,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
@@ -2077,7 +2098,7 @@
         <v>47</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2096,7 +2117,7 @@
         <v>7</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S22" s="3" t="s">
         <v>20</v>
@@ -2104,28 +2125,28 @@
     </row>
     <row r="23" spans="2:19" ht="90">
       <c r="B23" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2138,13 +2159,13 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S23" s="3" t="s">
         <v>21</v>
@@ -2152,7 +2173,7 @@
     </row>
     <row r="24" spans="2:19" ht="30">
       <c r="B24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
@@ -2164,16 +2185,16 @@
         <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2186,13 +2207,13 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>56</v>
@@ -2219,16 +2240,16 @@
         <v>47</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J25" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K25" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L25" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>3</v>
@@ -2240,7 +2261,7 @@
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>54</v>
@@ -2267,16 +2288,16 @@
         <v>47</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J26" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K26" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>3</v>
@@ -2287,10 +2308,10 @@
         <v>3</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>55</v>
@@ -2320,13 +2341,13 @@
         <v>3</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L27" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>3</v>
@@ -2338,7 +2359,7 @@
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S27" s="3" t="s">
         <v>54</v>
@@ -2368,13 +2389,13 @@
         <v>3</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L28" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>3</v>
@@ -2385,10 +2406,10 @@
         <v>3</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S28" s="3" t="s">
         <v>53</v>
@@ -2432,7 +2453,7 @@
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>23</v>
@@ -2478,7 +2499,7 @@
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>51</v>
@@ -2498,16 +2519,16 @@
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2515,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
@@ -2524,7 +2545,7 @@
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>60</v>
@@ -2544,16 +2565,16 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -2561,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
@@ -2570,7 +2591,7 @@
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>62</v>
@@ -2587,13 +2608,13 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="G33" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>48</v>
@@ -2607,16 +2628,16 @@
         <v>3</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>63</v>
@@ -2633,7 +2654,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>1</v>
+        <v>182</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
@@ -2655,14 +2676,14 @@
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>64</v>
@@ -2701,14 +2722,14 @@
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>65</v>
@@ -2728,16 +2749,16 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2745,16 +2766,16 @@
         <v>3</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>66</v>
@@ -2765,7 +2786,7 @@
         <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>3</v>
@@ -2781,7 +2802,7 @@
         <v>48</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2789,27 +2810,27 @@
         <v>3</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S37" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="2:19" ht="105">
       <c r="B38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
@@ -2820,7 +2841,7 @@
         <v>3</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -2832,33 +2853,33 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="2:19" ht="45">
       <c r="B39" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -2872,26 +2893,26 @@
         <v>1</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q39" s="3"/>
       <c r="R39" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="2:19" ht="75">
       <c r="B40" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
@@ -2916,22 +2937,22 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="2:19" ht="60">
       <c r="B41" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
@@ -2954,18 +2975,18 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="2:19" ht="45">
       <c r="B42" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="E42" s="17" t="s">
         <v>1</v>
@@ -2977,22 +2998,22 @@
         <v>49</v>
       </c>
       <c r="I42" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N42" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="L42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N42" s="17" t="s">
+      <c r="P42" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="P42" s="17" t="s">
+      <c r="R42" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="S42" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="R42" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="S42" s="17" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="43" spans="2:19">
@@ -3000,6 +3021,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B16:S16"/>
     <mergeCell ref="C13:M13"/>
@@ -3008,13 +3036,6 @@
     <mergeCell ref="C10:M10"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C12:M12"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3034,39 +3055,39 @@
   <sheetData>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="48"/>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="48"/>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="48"/>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="48"/>
       <c r="C10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3081,8 +3102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3095,7 +3116,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1">
       <c r="B2" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -3131,7 +3152,7 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>9</v>
@@ -3155,7 +3176,7 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
@@ -3167,7 +3188,7 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>1</v>
@@ -3182,13 +3203,13 @@
         <v>68</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3199,10 +3220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:C8"/>
+  <dimension ref="B3:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3213,7 +3234,7 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="50"/>
     </row>
@@ -3227,39 +3248,86 @@
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>153</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>156</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>159</v>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="50"/>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-1075, EPBDS-1076. Added "active" property validator and test.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -13,7 +13,7 @@
     <sheet name="Runtime Scope" sheetId="3" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -366,9 +366,6 @@
     <t>returnOnMiss</t>
   </si>
   <si>
-    <t>only one active version per dimension</t>
-  </si>
-  <si>
     <t>Value to return if no rules were matched. The type is compatible with table return type</t>
   </si>
   <si>
@@ -1182,6 +1179,9 @@
   </si>
   <si>
     <t>xls.properties</t>
+  </si>
+  <si>
+    <t>unique in:TableGroup</t>
   </si>
 </sst>
 </file>
@@ -1719,30 +1719,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1779,12 +1782,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1792,9 +1792,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1832,7 +1832,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1902,7 +1902,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2092,53 +2092,53 @@
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="C2" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="C3" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>111</v>
+      <c r="C5" s="48" t="s">
+        <v>110</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
@@ -2152,68 +2152,68 @@
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="C7" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1">
       <c r="B9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1">
       <c r="B10" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
@@ -2227,8 +2227,8 @@
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>116</v>
+      <c r="C11" s="48" t="s">
+        <v>115</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="47"/>
@@ -2242,8 +2242,8 @@
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="49" t="s">
-        <v>130</v>
+      <c r="C12" s="42" t="s">
+        <v>129</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="47"/>
@@ -2257,8 +2257,8 @@
       <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="49" t="s">
-        <v>117</v>
+      <c r="C13" s="42" t="s">
+        <v>116</v>
       </c>
       <c r="D13" s="47"/>
       <c r="E13" s="47"/>
@@ -2272,32 +2272,38 @@
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
+      <c r="C14" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1">
-      <c r="B15" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
+      <c r="B15" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -2306,12 +2312,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2322,9 +2322,9 @@
   <dimension ref="B1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2355,62 +2355,62 @@
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="C1" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="C2" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>111</v>
+      <c r="C4" s="48" t="s">
+        <v>110</v>
       </c>
       <c r="D4" s="47"/>
       <c r="E4" s="47"/>
@@ -2427,80 +2427,80 @@
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
+      <c r="C5" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
+      <c r="C6" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
     </row>
     <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="47"/>
       <c r="E9" s="47"/>
@@ -2526,26 +2526,26 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="2:19" ht="15" customHeight="1">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
     </row>
     <row r="12" spans="2:19" ht="30">
       <c r="B12" s="18" t="s">
@@ -2561,10 +2561,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>126</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>45</v>
@@ -2573,13 +2573,13 @@
         <v>78</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M12" s="18" t="s">
         <v>85</v>
@@ -2597,7 +2597,7 @@
         <v>6</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="S12" s="18" t="s">
         <v>17</v>
@@ -2617,10 +2617,10 @@
         <v>35</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>46</v>
@@ -2629,13 +2629,13 @@
         <v>84</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K13" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="L13" s="18" t="s">
         <v>157</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>158</v>
       </c>
       <c r="M13" s="18" t="s">
         <v>86</v>
@@ -2653,7 +2653,7 @@
         <v>39</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S13" s="18" t="s">
         <v>40</v>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="Q14" s="38"/>
       <c r="R14" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S14" s="38" t="s">
         <v>18</v>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="Q15" s="38"/>
       <c r="R15" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S15" s="38" t="s">
         <v>19</v>
@@ -2785,10 +2785,10 @@
       </c>
       <c r="Q16" s="38"/>
       <c r="R16" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S16" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="2:19" ht="45">
@@ -2802,7 +2802,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="38" t="s">
@@ -2831,7 +2831,7 @@
         <v>7</v>
       </c>
       <c r="R17" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S17" s="38" t="s">
         <v>20</v>
@@ -2851,7 +2851,7 @@
         <v>9</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G18" s="38" t="s">
         <v>83</v>
@@ -2873,13 +2873,13 @@
       <c r="N18" s="38"/>
       <c r="O18" s="38"/>
       <c r="P18" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q18" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R18" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S18" s="38" t="s">
         <v>21</v>
@@ -2899,7 +2899,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" s="38" t="s">
         <v>83</v>
@@ -2921,13 +2921,13 @@
       <c r="N19" s="38"/>
       <c r="O19" s="38"/>
       <c r="P19" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q19" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R19" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S19" s="38" t="s">
         <v>56</v>
@@ -2957,10 +2957,10 @@
         <v>83</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K20" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L20" s="38" t="s">
         <v>83</v>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="Q20" s="38"/>
       <c r="R20" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S20" s="38" t="s">
         <v>54</v>
@@ -3005,10 +3005,10 @@
         <v>83</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K21" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L21" s="38" t="s">
         <v>83</v>
@@ -3022,10 +3022,10 @@
         <v>3</v>
       </c>
       <c r="Q21" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R21" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S21" s="38" t="s">
         <v>55</v>
@@ -3055,10 +3055,10 @@
         <v>3</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K22" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L22" s="38" t="s">
         <v>83</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="Q22" s="38"/>
       <c r="R22" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S22" s="38" t="s">
         <v>54</v>
@@ -3103,10 +3103,10 @@
         <v>3</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L23" s="38" t="s">
         <v>83</v>
@@ -3120,10 +3120,10 @@
         <v>3</v>
       </c>
       <c r="Q23" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R23" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S23" s="38" t="s">
         <v>53</v>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="Q24" s="38"/>
       <c r="R24" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S24" s="38" t="s">
         <v>23</v>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="Q25" s="38"/>
       <c r="R25" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S25" s="38" t="s">
         <v>51</v>
@@ -3233,7 +3233,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G26" s="38" t="s">
         <v>83</v>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="Q26" s="38"/>
       <c r="R26" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S26" s="38" t="s">
         <v>60</v>
@@ -3276,10 +3276,10 @@
         <v>3</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" s="38" t="s">
         <v>83</v>
@@ -3301,11 +3301,11 @@
       <c r="N27" s="38"/>
       <c r="O27" s="38"/>
       <c r="P27" s="38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q27" s="38"/>
       <c r="R27" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S27" s="38" t="s">
         <v>62</v>
@@ -3322,10 +3322,10 @@
         <v>3</v>
       </c>
       <c r="E28" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="38" t="s">
         <v>171</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>172</v>
       </c>
       <c r="G28" s="38" t="s">
         <v>83</v>
@@ -3347,11 +3347,11 @@
       <c r="N28" s="38"/>
       <c r="O28" s="38"/>
       <c r="P28" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q28" s="38"/>
       <c r="R28" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S28" s="38" t="s">
         <v>63</v>
@@ -3368,7 +3368,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F29" s="38"/>
       <c r="G29" s="38" t="s">
@@ -3393,11 +3393,11 @@
         <v>76</v>
       </c>
       <c r="P29" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q29" s="38"/>
       <c r="R29" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S29" s="38" t="s">
         <v>64</v>
@@ -3414,7 +3414,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F30" s="38"/>
       <c r="G30" s="38" t="s">
@@ -3436,14 +3436,14 @@
       </c>
       <c r="N30" s="38"/>
       <c r="O30" s="38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P30" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q30" s="38"/>
       <c r="R30" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S30" s="38" t="s">
         <v>65</v>
@@ -3460,10 +3460,10 @@
         <v>3</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G31" s="38" t="s">
         <v>83</v>
@@ -3485,11 +3485,11 @@
       <c r="N31" s="38"/>
       <c r="O31" s="38"/>
       <c r="P31" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q31" s="38"/>
       <c r="R31" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S31" s="38" t="s">
         <v>66</v>
@@ -3506,7 +3506,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="38" t="s">
@@ -3529,11 +3529,11 @@
       <c r="N32" s="38"/>
       <c r="O32" s="38"/>
       <c r="P32" s="38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q32" s="38"/>
       <c r="R32" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S32" s="38" t="s">
         <v>73</v>
@@ -3571,13 +3571,13 @@
       </c>
       <c r="Q33" s="38"/>
       <c r="R33" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S33" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="45">
+    <row r="34" spans="2:19" ht="30">
       <c r="B34" s="38" t="s">
         <v>95</v>
       </c>
@@ -3607,14 +3607,14 @@
         <v>1</v>
       </c>
       <c r="P34" s="38" t="s">
-        <v>104</v>
+        <v>367</v>
       </c>
       <c r="Q34" s="38"/>
       <c r="R34" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S34" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="2:19" ht="75">
@@ -3651,10 +3651,10 @@
       <c r="P35" s="38"/>
       <c r="Q35" s="38"/>
       <c r="R35" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S35" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="2:19" ht="60">
@@ -3689,18 +3689,18 @@
       <c r="P36" s="38"/>
       <c r="Q36" s="38"/>
       <c r="R36" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S36" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="2:19" ht="45">
       <c r="B37" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="38" t="s">
         <v>140</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>141</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="38" t="s">
@@ -3714,7 +3714,7 @@
         <v>49</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J37" s="38"/>
       <c r="K37" s="38"/>
@@ -3723,18 +3723,18 @@
       </c>
       <c r="M37" s="38"/>
       <c r="N37" s="38" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O37" s="38"/>
       <c r="P37" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q37" s="38"/>
       <c r="R37" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S37" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="2:19">
@@ -3743,16 +3743,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
     <mergeCell ref="B11:S11"/>
     <mergeCell ref="C8:M8"/>
     <mergeCell ref="C9:M9"/>
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="C6:M6"/>
     <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3771,60 +3771,60 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="5" spans="2:6">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="50" t="s">
-        <v>121</v>
-      </c>
       <c r="C6" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="50"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="50"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="50"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="50"/>
-      <c r="C10" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3853,12 +3853,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1">
-      <c r="B2" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="17" t="s">
@@ -3890,7 +3890,7 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>9</v>
@@ -3914,13 +3914,13 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>62</v>
@@ -3928,13 +3928,13 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>66</v>
@@ -3945,13 +3945,13 @@
         <v>68</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3983,18 +3983,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11">
-      <c r="B3" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="F3" s="60" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" s="61"/>
-      <c r="J3" s="60" t="s">
-        <v>251</v>
-      </c>
-      <c r="K3" s="61"/>
+      <c r="B3" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="F3" s="61" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" s="62"/>
+      <c r="J3" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="K3" s="62"/>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="7" t="s">
@@ -4018,170 +4018,170 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="F5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="J5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>195</v>
-      </c>
       <c r="F6" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>255</v>
-      </c>
       <c r="J6" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>361</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="F7" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>257</v>
-      </c>
       <c r="J7" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>363</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>193</v>
-      </c>
       <c r="F8" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>259</v>
-      </c>
       <c r="J8" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>365</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>191</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>205</v>
-      </c>
       <c r="F10" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>201</v>
-      </c>
       <c r="F11" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>199</v>
-      </c>
       <c r="F12" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>264</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>197</v>
-      </c>
       <c r="F13" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="J13" s="60" t="s">
-        <v>350</v>
-      </c>
-      <c r="K13" s="61"/>
+        <v>265</v>
+      </c>
+      <c r="J13" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>203</v>
-      </c>
       <c r="F14" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>267</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>268</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>0</v>
@@ -4192,102 +4192,102 @@
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="F15" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>270</v>
-      </c>
       <c r="J15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>187</v>
-      </c>
       <c r="F16" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>272</v>
-      </c>
       <c r="J16" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>189</v>
-      </c>
       <c r="F17" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>274</v>
-      </c>
       <c r="J17" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>209</v>
-      </c>
       <c r="F18" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>276</v>
-      </c>
       <c r="J18" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>150</v>
-      </c>
       <c r="F19" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -4295,77 +4295,77 @@
         <v>77</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F20" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>279</v>
-      </c>
       <c r="J20" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>211</v>
-      </c>
       <c r="F21" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>280</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="F22" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>282</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="F23" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>284</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="F24" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>286</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="F25" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="G25" s="10" t="s">
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="61" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="62"/>
+      <c r="F26" s="9" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="B26" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="C26" s="61"/>
-      <c r="F26" s="9" t="s">
+      <c r="G26" s="10" t="s">
         <v>290</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="27" spans="2:11">
@@ -4376,192 +4376,192 @@
         <v>24</v>
       </c>
       <c r="F27" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="F28" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>221</v>
-      </c>
       <c r="F29" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>296</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>213</v>
-      </c>
       <c r="F30" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>298</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>219</v>
-      </c>
       <c r="F31" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>300</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>302</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>233</v>
-      </c>
       <c r="F33" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>304</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>225</v>
-      </c>
       <c r="F34" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>306</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>223</v>
-      </c>
       <c r="F35" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="G35" s="10" t="s">
         <v>308</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>229</v>
-      </c>
       <c r="F36" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="G36" s="10" t="s">
         <v>310</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="14.25" customHeight="1">
       <c r="B37" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>227</v>
-      </c>
       <c r="F37" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="G37" s="10" t="s">
         <v>312</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>215</v>
-      </c>
       <c r="F38" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G38" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>217</v>
-      </c>
       <c r="F39" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>316</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="40" spans="2:7">
       <c r="B40" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>318</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="41" spans="2:7">
@@ -4569,55 +4569,55 @@
         <v>76</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F41" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>320</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>231</v>
-      </c>
       <c r="F42" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="G42" s="10" t="s">
         <v>322</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="43" spans="2:7">
       <c r="F43" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="G43" s="10" t="s">
         <v>324</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="44" spans="2:7">
       <c r="F44" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="G44" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="G44" s="10" t="s">
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="C45" s="62"/>
+      <c r="F45" s="9" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="45" spans="2:7">
-      <c r="B45" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="C45" s="61"/>
-      <c r="F45" s="9" t="s">
+      <c r="G45" s="10" t="s">
         <v>328</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="46" spans="2:7">
@@ -4628,130 +4628,130 @@
         <v>24</v>
       </c>
       <c r="F46" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>330</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="F47" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="G47" s="10" t="s">
         <v>332</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>246</v>
-      </c>
       <c r="F48" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="G48" s="10" t="s">
         <v>334</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="49" spans="2:7">
       <c r="B49" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>236</v>
-      </c>
       <c r="F49" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="G49" s="10" t="s">
         <v>336</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="50" spans="2:7">
       <c r="B50" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>242</v>
-      </c>
       <c r="F50" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="G50" s="10" t="s">
         <v>338</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="51" spans="2:7">
       <c r="B51" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>248</v>
-      </c>
       <c r="F51" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="G51" s="10" t="s">
         <v>340</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="52" spans="2:7">
       <c r="B52" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>244</v>
-      </c>
       <c r="F52" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="G52" s="10" t="s">
         <v>342</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>238</v>
-      </c>
       <c r="F53" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>344</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>240</v>
-      </c>
       <c r="F54" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="G54" s="10" t="s">
         <v>346</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="55" spans="2:7">
       <c r="F55" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="G55" s="12" t="s">
         <v>348</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS 'failOnMiss' property value changed to false as default.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -13,7 +13,7 @@
     <sheet name="Runtime Scope" sheetId="3" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1719,30 +1719,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1784,7 +1784,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1792,9 +1792,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1832,7 +1832,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1902,7 +1902,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2092,52 +2092,52 @@
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="44" t="s">
         <v>110</v>
       </c>
       <c r="D5" s="47"/>
@@ -2152,46 +2152,46 @@
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1">
       <c r="B9" s="3" t="s">
@@ -2200,13 +2200,13 @@
       <c r="C9" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1">
       <c r="B10" s="3" t="s">
@@ -2227,7 +2227,7 @@
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="44" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="47"/>
@@ -2242,7 +2242,7 @@
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="48" t="s">
         <v>129</v>
       </c>
       <c r="D12" s="47"/>
@@ -2257,7 +2257,7 @@
       <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="48" t="s">
         <v>116</v>
       </c>
       <c r="D13" s="47"/>
@@ -2272,38 +2272,32 @@
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -2312,6 +2306,12 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2324,7 +2324,7 @@
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
+      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2355,61 +2355,61 @@
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="44" t="s">
         <v>110</v>
       </c>
       <c r="D4" s="47"/>
@@ -2427,55 +2427,55 @@
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="3" t="s">
@@ -2484,16 +2484,16 @@
       <c r="C8" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
     </row>
     <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="3" t="s">
@@ -3646,7 +3646,7 @@
         <v>43</v>
       </c>
       <c r="O35" s="38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35" s="38"/>
       <c r="Q35" s="38"/>

</xml_diff>

<commit_message>
EPBDS-1332 Make failOnMiss property available at category and module levels
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -4100,29 +4100,29 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4525,52 +4525,52 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="66" t="s">
         <v>101</v>
       </c>
       <c r="D5" s="65"/>
@@ -4585,46 +4585,46 @@
       <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1">
       <c r="B9" s="3" t="s">
@@ -4633,13 +4633,13 @@
       <c r="C9" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1">
       <c r="B10" s="3" t="s">
@@ -4660,7 +4660,7 @@
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="66" t="s">
         <v>106</v>
       </c>
       <c r="D11" s="65"/>
@@ -4675,7 +4675,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="60" t="s">
         <v>120</v>
       </c>
       <c r="D12" s="65"/>
@@ -4690,7 +4690,7 @@
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="60" t="s">
         <v>107</v>
       </c>
       <c r="D13" s="65"/>
@@ -4705,32 +4705,38 @@
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -4739,12 +4745,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4754,10 +4754,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4788,61 +4788,61 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="66" t="s">
         <v>101</v>
       </c>
       <c r="D4" s="65"/>
@@ -4860,55 +4860,55 @@
       <c r="B5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="3" t="s">
@@ -4917,16 +4917,16 @@
       <c r="C8" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
     </row>
     <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="3" t="s">
@@ -6082,7 +6082,7 @@
       <c r="P35" s="36"/>
       <c r="Q35" s="36"/>
       <c r="R35" s="36" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="S35" s="36" t="s">
         <v>96</v>
@@ -11935,7 +11935,7 @@
         <v>619</v>
       </c>
       <c r="C8" s="82"/>
-      <c r="D8" s="61"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="82" t="s">
         <v>1084</v>
       </c>
@@ -11948,7 +11948,7 @@
       <c r="C9" s="40" t="s">
         <v>621</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="40" t="s">
         <v>1054</v>
       </c>
@@ -11963,7 +11963,7 @@
       <c r="C10" s="40" t="s">
         <v>623</v>
       </c>
-      <c r="D10" s="61"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="40" t="s">
         <v>620</v>
       </c>
@@ -11978,7 +11978,7 @@
       <c r="C11" s="40" t="s">
         <v>625</v>
       </c>
-      <c r="D11" s="61"/>
+      <c r="D11" s="64"/>
       <c r="E11" s="40" t="s">
         <v>622</v>
       </c>
@@ -11993,7 +11993,7 @@
       <c r="C12" s="40" t="s">
         <v>626</v>
       </c>
-      <c r="D12" s="61"/>
+      <c r="D12" s="64"/>
       <c r="E12" s="40" t="s">
         <v>636</v>
       </c>
@@ -12008,7 +12008,7 @@
       <c r="C13" s="40" t="s">
         <v>627</v>
       </c>
-      <c r="D13" s="61"/>
+      <c r="D13" s="64"/>
       <c r="E13" s="40" t="s">
         <v>668</v>
       </c>
@@ -12023,7 +12023,7 @@
       <c r="C14" s="40" t="s">
         <v>628</v>
       </c>
-      <c r="D14" s="61"/>
+      <c r="D14" s="64"/>
       <c r="E14" s="40" t="s">
         <v>630</v>
       </c>
@@ -12038,7 +12038,7 @@
       <c r="C15" s="40" t="s">
         <v>629</v>
       </c>
-      <c r="D15" s="61"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="40" t="s">
         <v>208</v>
       </c>
@@ -12053,7 +12053,7 @@
       <c r="C16" s="40" t="s">
         <v>631</v>
       </c>
-      <c r="D16" s="61"/>
+      <c r="D16" s="64"/>
       <c r="E16" s="40" t="s">
         <v>200</v>
       </c>
@@ -12068,7 +12068,7 @@
       <c r="C17" s="40" t="s">
         <v>633</v>
       </c>
-      <c r="D17" s="61"/>
+      <c r="D17" s="64"/>
       <c r="E17" s="40" t="s">
         <v>638</v>
       </c>
@@ -12083,7 +12083,7 @@
       <c r="C18" s="40" t="s">
         <v>634</v>
       </c>
-      <c r="D18" s="61"/>
+      <c r="D18" s="64"/>
       <c r="E18" s="40" t="s">
         <v>642</v>
       </c>
@@ -12098,7 +12098,7 @@
       <c r="C19" s="40" t="s">
         <v>635</v>
       </c>
-      <c r="D19" s="61"/>
+      <c r="D19" s="64"/>
       <c r="E19" s="40" t="s">
         <v>670</v>
       </c>
@@ -12113,7 +12113,7 @@
       <c r="C20" s="40" t="s">
         <v>637</v>
       </c>
-      <c r="D20" s="61"/>
+      <c r="D20" s="64"/>
       <c r="E20" s="40" t="s">
         <v>652</v>
       </c>
@@ -12128,7 +12128,7 @@
       <c r="C21" s="40" t="s">
         <v>639</v>
       </c>
-      <c r="D21" s="61"/>
+      <c r="D21" s="64"/>
       <c r="E21" s="40" t="s">
         <v>650</v>
       </c>
@@ -12143,7 +12143,7 @@
       <c r="C22" s="40" t="s">
         <v>640</v>
       </c>
-      <c r="D22" s="61"/>
+      <c r="D22" s="64"/>
       <c r="E22" s="40" t="s">
         <v>682</v>
       </c>
@@ -12158,7 +12158,7 @@
       <c r="C23" s="40" t="s">
         <v>641</v>
       </c>
-      <c r="D23" s="61"/>
+      <c r="D23" s="64"/>
       <c r="E23" s="40" t="s">
         <v>647</v>
       </c>
@@ -12173,7 +12173,7 @@
       <c r="C24" s="40" t="s">
         <v>643</v>
       </c>
-      <c r="D24" s="61"/>
+      <c r="D24" s="64"/>
       <c r="E24" s="40" t="s">
         <v>687</v>
       </c>
@@ -12188,7 +12188,7 @@
       <c r="C25" s="40" t="s">
         <v>644</v>
       </c>
-      <c r="D25" s="61"/>
+      <c r="D25" s="64"/>
       <c r="E25" s="40" t="s">
         <v>661</v>
       </c>
@@ -12203,7 +12203,7 @@
       <c r="C26" s="40" t="s">
         <v>646</v>
       </c>
-      <c r="D26" s="61"/>
+      <c r="D26" s="64"/>
       <c r="E26" s="40" t="s">
         <v>680</v>
       </c>
@@ -12218,7 +12218,7 @@
       <c r="C27" s="40" t="s">
         <v>648</v>
       </c>
-      <c r="D27" s="61"/>
+      <c r="D27" s="64"/>
       <c r="E27" s="40" t="s">
         <v>666</v>
       </c>
@@ -12233,7 +12233,7 @@
       <c r="C28" s="40" t="s">
         <v>649</v>
       </c>
-      <c r="D28" s="61"/>
+      <c r="D28" s="64"/>
       <c r="E28" s="40" t="s">
         <v>206</v>
       </c>
@@ -12248,7 +12248,7 @@
       <c r="C29" s="40" t="s">
         <v>651</v>
       </c>
-      <c r="D29" s="61"/>
+      <c r="D29" s="64"/>
       <c r="E29" s="40" t="s">
         <v>645</v>
       </c>
@@ -12263,7 +12263,7 @@
       <c r="C30" s="40" t="s">
         <v>653</v>
       </c>
-      <c r="D30" s="61"/>
+      <c r="D30" s="64"/>
       <c r="E30" s="40" t="s">
         <v>663</v>
       </c>
@@ -12278,7 +12278,7 @@
       <c r="C31" s="40" t="s">
         <v>654</v>
       </c>
-      <c r="D31" s="61"/>
+      <c r="D31" s="64"/>
       <c r="E31" s="40" t="s">
         <v>672</v>
       </c>
@@ -12293,7 +12293,7 @@
       <c r="C32" s="40" t="s">
         <v>655</v>
       </c>
-      <c r="D32" s="61"/>
+      <c r="D32" s="64"/>
       <c r="E32" s="40" t="s">
         <v>168</v>
       </c>
@@ -12308,7 +12308,7 @@
       <c r="C33" s="40" t="s">
         <v>656</v>
       </c>
-      <c r="D33" s="61"/>
+      <c r="D33" s="64"/>
       <c r="E33" s="40" t="s">
         <v>657</v>
       </c>
@@ -12323,7 +12323,7 @@
       <c r="C34" s="40" t="s">
         <v>658</v>
       </c>
-      <c r="D34" s="61"/>
+      <c r="D34" s="64"/>
       <c r="E34" s="40" t="s">
         <v>220</v>
       </c>
@@ -12338,7 +12338,7 @@
       <c r="C35" s="56" t="s">
         <v>660</v>
       </c>
-      <c r="D35" s="61"/>
+      <c r="D35" s="64"/>
       <c r="E35" s="40" t="s">
         <v>716</v>
       </c>
@@ -12353,7 +12353,7 @@
       <c r="C36" s="40" t="s">
         <v>662</v>
       </c>
-      <c r="D36" s="61"/>
+      <c r="D36" s="64"/>
       <c r="E36" s="40" t="s">
         <v>864</v>
       </c>
@@ -12368,7 +12368,7 @@
       <c r="C37" s="40" t="s">
         <v>664</v>
       </c>
-      <c r="D37" s="61"/>
+      <c r="D37" s="64"/>
       <c r="E37" s="40" t="s">
         <v>703</v>
       </c>
@@ -12383,7 +12383,7 @@
       <c r="C38" s="40" t="s">
         <v>665</v>
       </c>
-      <c r="D38" s="61"/>
+      <c r="D38" s="64"/>
       <c r="E38" s="40" t="s">
         <v>212</v>
       </c>
@@ -12398,7 +12398,7 @@
       <c r="C39" s="40" t="s">
         <v>667</v>
       </c>
-      <c r="D39" s="61"/>
+      <c r="D39" s="64"/>
       <c r="E39" s="40" t="s">
         <v>708</v>
       </c>
@@ -12413,7 +12413,7 @@
       <c r="C40" s="40" t="s">
         <v>669</v>
       </c>
-      <c r="D40" s="61"/>
+      <c r="D40" s="64"/>
       <c r="E40" s="40" t="s">
         <v>719</v>
       </c>
@@ -12428,7 +12428,7 @@
       <c r="C41" s="40" t="s">
         <v>671</v>
       </c>
-      <c r="D41" s="61"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="40" t="s">
         <v>723</v>
       </c>
@@ -12443,7 +12443,7 @@
       <c r="C42" s="40" t="s">
         <v>673</v>
       </c>
-      <c r="D42" s="61"/>
+      <c r="D42" s="64"/>
       <c r="E42" s="40" t="s">
         <v>697</v>
       </c>
@@ -12458,7 +12458,7 @@
       <c r="C43" s="40" t="s">
         <v>675</v>
       </c>
-      <c r="D43" s="61"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="40" t="s">
         <v>727</v>
       </c>
@@ -12473,7 +12473,7 @@
       <c r="C44" s="40" t="s">
         <v>676</v>
       </c>
-      <c r="D44" s="61"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="40" t="s">
         <v>729</v>
       </c>
@@ -12488,7 +12488,7 @@
       <c r="C45" s="40" t="s">
         <v>677</v>
       </c>
-      <c r="D45" s="61"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="40" t="s">
         <v>733</v>
       </c>
@@ -12503,7 +12503,7 @@
       <c r="C46" s="40" t="s">
         <v>678</v>
       </c>
-      <c r="D46" s="61"/>
+      <c r="D46" s="64"/>
       <c r="E46" s="40" t="s">
         <v>731</v>
       </c>
@@ -12518,7 +12518,7 @@
       <c r="C47" s="40" t="s">
         <v>679</v>
       </c>
-      <c r="D47" s="61"/>
+      <c r="D47" s="64"/>
       <c r="E47" s="40" t="s">
         <v>736</v>
       </c>
@@ -12533,7 +12533,7 @@
       <c r="C48" s="40" t="s">
         <v>681</v>
       </c>
-      <c r="D48" s="61"/>
+      <c r="D48" s="64"/>
       <c r="E48" s="40" t="s">
         <v>624</v>
       </c>
@@ -12548,7 +12548,7 @@
       <c r="C49" s="40" t="s">
         <v>683</v>
       </c>
-      <c r="D49" s="61"/>
+      <c r="D49" s="64"/>
       <c r="E49" s="40" t="s">
         <v>755</v>
       </c>
@@ -12563,7 +12563,7 @@
       <c r="C50" s="56" t="s">
         <v>684</v>
       </c>
-      <c r="D50" s="61"/>
+      <c r="D50" s="64"/>
       <c r="E50" s="40" t="s">
         <v>743</v>
       </c>
@@ -12578,7 +12578,7 @@
       <c r="C51" s="40" t="s">
         <v>686</v>
       </c>
-      <c r="D51" s="61"/>
+      <c r="D51" s="64"/>
       <c r="E51" s="40" t="s">
         <v>753</v>
       </c>
@@ -12593,7 +12593,7 @@
       <c r="C52" s="40" t="s">
         <v>688</v>
       </c>
-      <c r="D52" s="61"/>
+      <c r="D52" s="64"/>
       <c r="E52" s="40" t="s">
         <v>751</v>
       </c>
@@ -12608,7 +12608,7 @@
       <c r="C53" s="56" t="s">
         <v>689</v>
       </c>
-      <c r="D53" s="61"/>
+      <c r="D53" s="64"/>
       <c r="E53" s="40" t="s">
         <v>210</v>
       </c>
@@ -12623,7 +12623,7 @@
       <c r="C54" s="40" t="s">
         <v>690</v>
       </c>
-      <c r="D54" s="61"/>
+      <c r="D54" s="64"/>
       <c r="E54" s="40" t="s">
         <v>762</v>
       </c>
@@ -12638,7 +12638,7 @@
       <c r="C55" s="40" t="s">
         <v>692</v>
       </c>
-      <c r="D55" s="61"/>
+      <c r="D55" s="64"/>
       <c r="E55" s="40" t="s">
         <v>759</v>
       </c>
@@ -12653,7 +12653,7 @@
       <c r="C56" s="56" t="s">
         <v>694</v>
       </c>
-      <c r="D56" s="61"/>
+      <c r="D56" s="64"/>
       <c r="E56" s="40" t="s">
         <v>216</v>
       </c>
@@ -12668,7 +12668,7 @@
       <c r="C57" s="40" t="s">
         <v>695</v>
       </c>
-      <c r="D57" s="61"/>
+      <c r="D57" s="64"/>
       <c r="E57" s="40" t="s">
         <v>774</v>
       </c>
@@ -12683,7 +12683,7 @@
       <c r="C58" s="40" t="s">
         <v>696</v>
       </c>
-      <c r="D58" s="61"/>
+      <c r="D58" s="64"/>
       <c r="E58" s="40" t="s">
         <v>792</v>
       </c>
@@ -12698,7 +12698,7 @@
       <c r="C59" s="40" t="s">
         <v>698</v>
       </c>
-      <c r="D59" s="61"/>
+      <c r="D59" s="64"/>
       <c r="E59" s="40" t="s">
         <v>777</v>
       </c>
@@ -12713,7 +12713,7 @@
       <c r="C60" s="40" t="s">
         <v>700</v>
       </c>
-      <c r="D60" s="61"/>
+      <c r="D60" s="64"/>
       <c r="E60" s="40" t="s">
         <v>779</v>
       </c>
@@ -12728,7 +12728,7 @@
       <c r="C61" s="56" t="s">
         <v>701</v>
       </c>
-      <c r="D61" s="61"/>
+      <c r="D61" s="64"/>
       <c r="E61" s="40" t="s">
         <v>772</v>
       </c>
@@ -12743,7 +12743,7 @@
       <c r="C62" s="56" t="s">
         <v>702</v>
       </c>
-      <c r="D62" s="61"/>
+      <c r="D62" s="64"/>
       <c r="E62" s="40" t="s">
         <v>794</v>
       </c>
@@ -12758,7 +12758,7 @@
       <c r="C63" s="40" t="s">
         <v>704</v>
       </c>
-      <c r="D63" s="61"/>
+      <c r="D63" s="64"/>
       <c r="E63" s="40" t="s">
         <v>790</v>
       </c>
@@ -12773,7 +12773,7 @@
       <c r="C64" s="40" t="s">
         <v>705</v>
       </c>
-      <c r="D64" s="61"/>
+      <c r="D64" s="64"/>
       <c r="E64" s="40" t="s">
         <v>797</v>
       </c>
@@ -12788,7 +12788,7 @@
       <c r="C65" s="40" t="s">
         <v>706</v>
       </c>
-      <c r="D65" s="61"/>
+      <c r="D65" s="64"/>
       <c r="E65" s="40" t="s">
         <v>808</v>
       </c>
@@ -12803,7 +12803,7 @@
       <c r="C66" s="40" t="s">
         <v>707</v>
       </c>
-      <c r="D66" s="61"/>
+      <c r="D66" s="64"/>
       <c r="E66" s="40" t="s">
         <v>806</v>
       </c>
@@ -12818,7 +12818,7 @@
       <c r="C67" s="40" t="s">
         <v>709</v>
       </c>
-      <c r="D67" s="61"/>
+      <c r="D67" s="64"/>
       <c r="E67" s="40" t="s">
         <v>721</v>
       </c>
@@ -12833,7 +12833,7 @@
       <c r="C68" s="40" t="s">
         <v>710</v>
       </c>
-      <c r="D68" s="61"/>
+      <c r="D68" s="64"/>
       <c r="E68" s="40" t="s">
         <v>799</v>
       </c>
@@ -12848,7 +12848,7 @@
       <c r="C69" s="40" t="s">
         <v>712</v>
       </c>
-      <c r="D69" s="61"/>
+      <c r="D69" s="64"/>
       <c r="E69" s="40" t="s">
         <v>810</v>
       </c>
@@ -12863,7 +12863,7 @@
       <c r="C70" s="40" t="s">
         <v>714</v>
       </c>
-      <c r="D70" s="61"/>
+      <c r="D70" s="64"/>
       <c r="E70" s="40" t="s">
         <v>740</v>
       </c>
@@ -12878,7 +12878,7 @@
       <c r="C71" s="56" t="s">
         <v>715</v>
       </c>
-      <c r="D71" s="61"/>
+      <c r="D71" s="64"/>
       <c r="E71" s="40" t="s">
         <v>825</v>
       </c>
@@ -12893,7 +12893,7 @@
       <c r="C72" s="40" t="s">
         <v>717</v>
       </c>
-      <c r="D72" s="61"/>
+      <c r="D72" s="64"/>
       <c r="E72" s="40" t="s">
         <v>823</v>
       </c>
@@ -12908,7 +12908,7 @@
       <c r="C73" s="40" t="s">
         <v>718</v>
       </c>
-      <c r="D73" s="61"/>
+      <c r="D73" s="64"/>
       <c r="E73" s="40" t="s">
         <v>214</v>
       </c>
@@ -12923,7 +12923,7 @@
       <c r="C74" s="40" t="s">
         <v>720</v>
       </c>
-      <c r="D74" s="61"/>
+      <c r="D74" s="64"/>
       <c r="E74" s="40" t="s">
         <v>820</v>
       </c>
@@ -12938,7 +12938,7 @@
       <c r="C75" s="40" t="s">
         <v>722</v>
       </c>
-      <c r="D75" s="61"/>
+      <c r="D75" s="64"/>
       <c r="E75" s="40" t="s">
         <v>818</v>
       </c>
@@ -12953,7 +12953,7 @@
       <c r="C76" s="40" t="s">
         <v>724</v>
       </c>
-      <c r="D76" s="61"/>
+      <c r="D76" s="64"/>
       <c r="E76" s="40" t="s">
         <v>812</v>
       </c>
@@ -12968,7 +12968,7 @@
       <c r="C77" s="40" t="s">
         <v>725</v>
       </c>
-      <c r="D77" s="61"/>
+      <c r="D77" s="64"/>
       <c r="E77" s="40" t="s">
         <v>833</v>
       </c>
@@ -12983,7 +12983,7 @@
       <c r="C78" s="40" t="s">
         <v>726</v>
       </c>
-      <c r="D78" s="61"/>
+      <c r="D78" s="64"/>
       <c r="E78" s="40" t="s">
         <v>828</v>
       </c>
@@ -12998,7 +12998,7 @@
       <c r="C79" s="40" t="s">
         <v>728</v>
       </c>
-      <c r="D79" s="61"/>
+      <c r="D79" s="64"/>
       <c r="E79" s="40" t="s">
         <v>835</v>
       </c>
@@ -13013,7 +13013,7 @@
       <c r="C80" s="40" t="s">
         <v>730</v>
       </c>
-      <c r="D80" s="61"/>
+      <c r="D80" s="64"/>
       <c r="E80" s="40" t="s">
         <v>831</v>
       </c>
@@ -13028,7 +13028,7 @@
       <c r="C81" s="40" t="s">
         <v>732</v>
       </c>
-      <c r="D81" s="61"/>
+      <c r="D81" s="64"/>
       <c r="E81" s="40" t="s">
         <v>840</v>
       </c>
@@ -13043,7 +13043,7 @@
       <c r="C82" s="40" t="s">
         <v>734</v>
       </c>
-      <c r="D82" s="61"/>
+      <c r="D82" s="64"/>
       <c r="E82" s="40" t="s">
         <v>849</v>
       </c>
@@ -13058,7 +13058,7 @@
       <c r="C83" s="40" t="s">
         <v>735</v>
       </c>
-      <c r="D83" s="61"/>
+      <c r="D83" s="64"/>
       <c r="E83" s="40" t="s">
         <v>691</v>
       </c>
@@ -13073,7 +13073,7 @@
       <c r="C84" s="40" t="s">
         <v>737</v>
       </c>
-      <c r="D84" s="61"/>
+      <c r="D84" s="64"/>
       <c r="E84" s="40" t="s">
         <v>711</v>
       </c>
@@ -13088,7 +13088,7 @@
       <c r="C85" s="40" t="s">
         <v>738</v>
       </c>
-      <c r="D85" s="61"/>
+      <c r="D85" s="64"/>
       <c r="E85" s="40" t="s">
         <v>843</v>
       </c>
@@ -13103,7 +13103,7 @@
       <c r="C86" s="40" t="s">
         <v>739</v>
       </c>
-      <c r="D86" s="61"/>
+      <c r="D86" s="64"/>
       <c r="E86" s="40" t="s">
         <v>845</v>
       </c>
@@ -13118,7 +13118,7 @@
       <c r="C87" s="40" t="s">
         <v>741</v>
       </c>
-      <c r="D87" s="61"/>
+      <c r="D87" s="64"/>
       <c r="E87" s="40" t="s">
         <v>847</v>
       </c>
@@ -13133,7 +13133,7 @@
       <c r="C88" s="40" t="s">
         <v>742</v>
       </c>
-      <c r="D88" s="61"/>
+      <c r="D88" s="64"/>
       <c r="E88" s="40" t="s">
         <v>699</v>
       </c>
@@ -13148,7 +13148,7 @@
       <c r="C89" s="40" t="s">
         <v>744</v>
       </c>
-      <c r="D89" s="61"/>
+      <c r="D89" s="64"/>
       <c r="E89" s="40" t="s">
         <v>837</v>
       </c>
@@ -13163,7 +13163,7 @@
       <c r="C90" s="40" t="s">
         <v>745</v>
       </c>
-      <c r="D90" s="61"/>
+      <c r="D90" s="64"/>
       <c r="E90" s="40" t="s">
         <v>851</v>
       </c>
@@ -13178,7 +13178,7 @@
       <c r="C91" s="40" t="s">
         <v>747</v>
       </c>
-      <c r="D91" s="61"/>
+      <c r="D91" s="64"/>
       <c r="E91" s="40" t="s">
         <v>855</v>
       </c>
@@ -13193,7 +13193,7 @@
       <c r="C92" s="40" t="s">
         <v>748</v>
       </c>
-      <c r="D92" s="61"/>
+      <c r="D92" s="64"/>
       <c r="E92" s="40" t="s">
         <v>1010</v>
       </c>
@@ -13208,7 +13208,7 @@
       <c r="C93" s="40" t="s">
         <v>749</v>
       </c>
-      <c r="D93" s="61"/>
+      <c r="D93" s="64"/>
       <c r="E93" s="40" t="s">
         <v>860</v>
       </c>
@@ -13223,7 +13223,7 @@
       <c r="C94" s="56" t="s">
         <v>750</v>
       </c>
-      <c r="D94" s="61"/>
+      <c r="D94" s="64"/>
       <c r="E94" s="40" t="s">
         <v>857</v>
       </c>
@@ -13238,7 +13238,7 @@
       <c r="C95" s="40" t="s">
         <v>752</v>
       </c>
-      <c r="D95" s="61"/>
+      <c r="D95" s="64"/>
       <c r="E95" s="40" t="s">
         <v>866</v>
       </c>
@@ -13253,7 +13253,7 @@
       <c r="C96" s="40" t="s">
         <v>754</v>
       </c>
-      <c r="D96" s="61"/>
+      <c r="D96" s="64"/>
       <c r="E96" s="40" t="s">
         <v>853</v>
       </c>
@@ -13268,7 +13268,7 @@
       <c r="C97" s="40" t="s">
         <v>756</v>
       </c>
-      <c r="D97" s="61"/>
+      <c r="D97" s="64"/>
       <c r="E97" s="40" t="s">
         <v>862</v>
       </c>
@@ -13283,7 +13283,7 @@
       <c r="C98" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D98" s="61"/>
+      <c r="D98" s="64"/>
       <c r="E98" s="40" t="s">
         <v>907</v>
       </c>
@@ -13298,7 +13298,7 @@
       <c r="C99" s="56" t="s">
         <v>758</v>
       </c>
-      <c r="D99" s="61"/>
+      <c r="D99" s="64"/>
       <c r="E99" s="40" t="s">
         <v>900</v>
       </c>
@@ -13313,7 +13313,7 @@
       <c r="C100" s="40" t="s">
         <v>760</v>
       </c>
-      <c r="D100" s="61"/>
+      <c r="D100" s="64"/>
       <c r="E100" s="40" t="s">
         <v>873</v>
       </c>
@@ -13328,7 +13328,7 @@
       <c r="C101" s="40" t="s">
         <v>761</v>
       </c>
-      <c r="D101" s="61"/>
+      <c r="D101" s="64"/>
       <c r="E101" s="40" t="s">
         <v>871</v>
       </c>
@@ -13343,7 +13343,7 @@
       <c r="C102" s="40" t="s">
         <v>763</v>
       </c>
-      <c r="D102" s="61"/>
+      <c r="D102" s="64"/>
       <c r="E102" s="40" t="s">
         <v>685</v>
       </c>
@@ -13358,7 +13358,7 @@
       <c r="C103" s="40" t="s">
         <v>764</v>
       </c>
-      <c r="D103" s="61"/>
+      <c r="D103" s="64"/>
       <c r="E103" s="40" t="s">
         <v>903</v>
       </c>
@@ -13373,7 +13373,7 @@
       <c r="C104" s="40" t="s">
         <v>765</v>
       </c>
-      <c r="D104" s="61"/>
+      <c r="D104" s="64"/>
       <c r="E104" s="40" t="s">
         <v>869</v>
       </c>
@@ -13388,7 +13388,7 @@
       <c r="C105" s="40" t="s">
         <v>766</v>
       </c>
-      <c r="D105" s="61"/>
+      <c r="D105" s="64"/>
       <c r="E105" s="40" t="s">
         <v>890</v>
       </c>
@@ -13403,7 +13403,7 @@
       <c r="C106" s="40" t="s">
         <v>767</v>
       </c>
-      <c r="D106" s="61"/>
+      <c r="D106" s="64"/>
       <c r="E106" s="40" t="s">
         <v>884</v>
       </c>
@@ -13418,7 +13418,7 @@
       <c r="C107" s="40" t="s">
         <v>768</v>
       </c>
-      <c r="D107" s="61"/>
+      <c r="D107" s="64"/>
       <c r="E107" s="40" t="s">
         <v>892</v>
       </c>
@@ -13433,7 +13433,7 @@
       <c r="C108" s="40" t="s">
         <v>769</v>
       </c>
-      <c r="D108" s="61"/>
+      <c r="D108" s="64"/>
       <c r="E108" s="40" t="s">
         <v>880</v>
       </c>
@@ -13448,7 +13448,7 @@
       <c r="C109" s="40" t="s">
         <v>770</v>
       </c>
-      <c r="D109" s="61"/>
+      <c r="D109" s="64"/>
       <c r="E109" s="40" t="s">
         <v>876</v>
       </c>
@@ -13463,7 +13463,7 @@
       <c r="C110" s="56" t="s">
         <v>771</v>
       </c>
-      <c r="D110" s="61"/>
+      <c r="D110" s="64"/>
       <c r="E110" s="40" t="s">
         <v>202</v>
       </c>
@@ -13478,7 +13478,7 @@
       <c r="C111" s="40" t="s">
         <v>773</v>
       </c>
-      <c r="D111" s="61"/>
+      <c r="D111" s="64"/>
       <c r="E111" s="40" t="s">
         <v>878</v>
       </c>
@@ -13493,7 +13493,7 @@
       <c r="C112" s="40" t="s">
         <v>775</v>
       </c>
-      <c r="D112" s="61"/>
+      <c r="D112" s="64"/>
       <c r="E112" s="40" t="s">
         <v>909</v>
       </c>
@@ -13508,7 +13508,7 @@
       <c r="C113" s="40" t="s">
         <v>776</v>
       </c>
-      <c r="D113" s="61"/>
+      <c r="D113" s="64"/>
       <c r="E113" s="40" t="s">
         <v>912</v>
       </c>
@@ -13523,7 +13523,7 @@
       <c r="C114" s="40" t="s">
         <v>778</v>
       </c>
-      <c r="D114" s="61"/>
+      <c r="D114" s="64"/>
       <c r="E114" s="40" t="s">
         <v>926</v>
       </c>
@@ -13538,7 +13538,7 @@
       <c r="C115" s="40" t="s">
         <v>780</v>
       </c>
-      <c r="D115" s="61"/>
+      <c r="D115" s="64"/>
       <c r="E115" s="40" t="s">
         <v>923</v>
       </c>
@@ -13553,7 +13553,7 @@
       <c r="C116" s="40" t="s">
         <v>782</v>
       </c>
-      <c r="D116" s="61"/>
+      <c r="D116" s="64"/>
       <c r="E116" s="40" t="s">
         <v>674</v>
       </c>
@@ -13568,7 +13568,7 @@
       <c r="C117" s="40" t="s">
         <v>783</v>
       </c>
-      <c r="D117" s="61"/>
+      <c r="D117" s="64"/>
       <c r="E117" s="40" t="s">
         <v>916</v>
       </c>
@@ -13583,7 +13583,7 @@
       <c r="C118" s="40" t="s">
         <v>784</v>
       </c>
-      <c r="D118" s="61"/>
+      <c r="D118" s="64"/>
       <c r="E118" s="40" t="s">
         <v>204</v>
       </c>
@@ -13598,7 +13598,7 @@
       <c r="C119" s="40" t="s">
         <v>785</v>
       </c>
-      <c r="D119" s="61"/>
+      <c r="D119" s="64"/>
       <c r="E119" s="40" t="s">
         <v>932</v>
       </c>
@@ -13613,7 +13613,7 @@
       <c r="C120" s="40" t="s">
         <v>786</v>
       </c>
-      <c r="D120" s="61"/>
+      <c r="D120" s="64"/>
       <c r="E120" s="40" t="s">
         <v>939</v>
       </c>
@@ -13628,7 +13628,7 @@
       <c r="C121" s="40" t="s">
         <v>787</v>
       </c>
-      <c r="D121" s="61"/>
+      <c r="D121" s="64"/>
       <c r="E121" s="40" t="s">
         <v>946</v>
       </c>
@@ -13643,7 +13643,7 @@
       <c r="C122" s="40" t="s">
         <v>788</v>
       </c>
-      <c r="D122" s="61"/>
+      <c r="D122" s="64"/>
       <c r="E122" s="40" t="s">
         <v>942</v>
       </c>
@@ -13658,7 +13658,7 @@
       <c r="C123" s="40" t="s">
         <v>789</v>
       </c>
-      <c r="D123" s="61"/>
+      <c r="D123" s="64"/>
       <c r="E123" s="40" t="s">
         <v>948</v>
       </c>
@@ -13673,7 +13673,7 @@
       <c r="C124" s="40" t="s">
         <v>791</v>
       </c>
-      <c r="D124" s="61"/>
+      <c r="D124" s="64"/>
       <c r="E124" s="40" t="s">
         <v>934</v>
       </c>
@@ -13688,7 +13688,7 @@
       <c r="C125" s="40" t="s">
         <v>793</v>
       </c>
-      <c r="D125" s="61"/>
+      <c r="D125" s="64"/>
       <c r="E125" s="40" t="s">
         <v>953</v>
       </c>
@@ -13703,7 +13703,7 @@
       <c r="C126" s="40" t="s">
         <v>795</v>
       </c>
-      <c r="D126" s="61"/>
+      <c r="D126" s="64"/>
       <c r="E126" s="40" t="s">
         <v>944</v>
       </c>
@@ -13718,7 +13718,7 @@
       <c r="C127" s="56" t="s">
         <v>796</v>
       </c>
-      <c r="D127" s="61"/>
+      <c r="D127" s="64"/>
       <c r="E127" s="40" t="s">
         <v>959</v>
       </c>
@@ -13733,7 +13733,7 @@
       <c r="C128" s="40" t="s">
         <v>798</v>
       </c>
-      <c r="D128" s="61"/>
+      <c r="D128" s="64"/>
       <c r="E128" s="40" t="s">
         <v>962</v>
       </c>
@@ -13748,7 +13748,7 @@
       <c r="C129" s="40" t="s">
         <v>800</v>
       </c>
-      <c r="D129" s="61"/>
+      <c r="D129" s="64"/>
       <c r="E129" s="40" t="s">
         <v>987</v>
       </c>
@@ -13763,7 +13763,7 @@
       <c r="C130" s="40" t="s">
         <v>801</v>
       </c>
-      <c r="D130" s="61"/>
+      <c r="D130" s="64"/>
       <c r="E130" s="40" t="s">
         <v>167</v>
       </c>
@@ -13778,7 +13778,7 @@
       <c r="C131" s="40" t="s">
         <v>802</v>
       </c>
-      <c r="D131" s="61"/>
+      <c r="D131" s="64"/>
       <c r="E131" s="40" t="s">
         <v>965</v>
       </c>
@@ -13793,7 +13793,7 @@
       <c r="C132" s="40" t="s">
         <v>803</v>
       </c>
-      <c r="D132" s="61"/>
+      <c r="D132" s="64"/>
       <c r="E132" s="40" t="s">
         <v>982</v>
       </c>
@@ -13808,7 +13808,7 @@
       <c r="C133" s="40" t="s">
         <v>804</v>
       </c>
-      <c r="D133" s="61"/>
+      <c r="D133" s="64"/>
       <c r="E133" s="40" t="s">
         <v>1001</v>
       </c>
@@ -13823,7 +13823,7 @@
       <c r="C134" s="40" t="s">
         <v>805</v>
       </c>
-      <c r="D134" s="61"/>
+      <c r="D134" s="64"/>
       <c r="E134" s="40" t="s">
         <v>989</v>
       </c>
@@ -13838,7 +13838,7 @@
       <c r="C135" s="40" t="s">
         <v>807</v>
       </c>
-      <c r="D135" s="61"/>
+      <c r="D135" s="64"/>
       <c r="E135" s="40" t="s">
         <v>1012</v>
       </c>
@@ -13853,7 +13853,7 @@
       <c r="C136" s="40" t="s">
         <v>809</v>
       </c>
-      <c r="D136" s="61"/>
+      <c r="D136" s="64"/>
       <c r="E136" s="40" t="s">
         <v>1019</v>
       </c>
@@ -13868,7 +13868,7 @@
       <c r="C137" s="40" t="s">
         <v>811</v>
       </c>
-      <c r="D137" s="61"/>
+      <c r="D137" s="64"/>
       <c r="E137" s="40" t="s">
         <v>995</v>
       </c>
@@ -13883,7 +13883,7 @@
       <c r="C138" s="40" t="s">
         <v>813</v>
       </c>
-      <c r="D138" s="61"/>
+      <c r="D138" s="64"/>
       <c r="E138" s="40" t="s">
         <v>971</v>
       </c>
@@ -13898,7 +13898,7 @@
       <c r="C139" s="40" t="s">
         <v>814</v>
       </c>
-      <c r="D139" s="61"/>
+      <c r="D139" s="64"/>
       <c r="E139" s="40" t="s">
         <v>991</v>
       </c>
@@ -13913,7 +13913,7 @@
       <c r="C140" s="40" t="s">
         <v>815</v>
       </c>
-      <c r="D140" s="61"/>
+      <c r="D140" s="64"/>
       <c r="E140" s="40" t="s">
         <v>1003</v>
       </c>
@@ -13928,7 +13928,7 @@
       <c r="C141" s="40" t="s">
         <v>817</v>
       </c>
-      <c r="D141" s="61"/>
+      <c r="D141" s="64"/>
       <c r="E141" s="40" t="s">
         <v>984</v>
       </c>
@@ -13943,7 +13943,7 @@
       <c r="C142" s="40" t="s">
         <v>819</v>
       </c>
-      <c r="D142" s="61"/>
+      <c r="D142" s="64"/>
       <c r="E142" s="40" t="s">
         <v>1014</v>
       </c>
@@ -13958,7 +13958,7 @@
       <c r="C143" s="40" t="s">
         <v>821</v>
       </c>
-      <c r="D143" s="61"/>
+      <c r="D143" s="64"/>
       <c r="E143" s="40" t="s">
         <v>956</v>
       </c>
@@ -13973,7 +13973,7 @@
       <c r="C144" s="40" t="s">
         <v>822</v>
       </c>
-      <c r="D144" s="61"/>
+      <c r="D144" s="64"/>
       <c r="E144" s="40" t="s">
         <v>746</v>
       </c>
@@ -13988,7 +13988,7 @@
       <c r="C145" s="40" t="s">
         <v>824</v>
       </c>
-      <c r="D145" s="61"/>
+      <c r="D145" s="64"/>
       <c r="E145" s="40" t="s">
         <v>1022</v>
       </c>
@@ -14003,7 +14003,7 @@
       <c r="C146" s="40" t="s">
         <v>826</v>
       </c>
-      <c r="D146" s="61"/>
+      <c r="D146" s="64"/>
       <c r="E146" s="40" t="s">
         <v>1017</v>
       </c>
@@ -14018,7 +14018,7 @@
       <c r="C147" s="40" t="s">
         <v>827</v>
       </c>
-      <c r="D147" s="61"/>
+      <c r="D147" s="64"/>
       <c r="E147" s="40" t="s">
         <v>1031</v>
       </c>
@@ -14033,7 +14033,7 @@
       <c r="C148" s="40" t="s">
         <v>829</v>
       </c>
-      <c r="D148" s="61"/>
+      <c r="D148" s="64"/>
       <c r="E148" s="40" t="s">
         <v>1027</v>
       </c>
@@ -14048,7 +14048,7 @@
       <c r="C149" s="40" t="s">
         <v>830</v>
       </c>
-      <c r="D149" s="61"/>
+      <c r="D149" s="64"/>
       <c r="E149" s="40" t="s">
         <v>1045</v>
       </c>
@@ -14063,7 +14063,7 @@
       <c r="C150" s="40" t="s">
         <v>832</v>
       </c>
-      <c r="D150" s="61"/>
+      <c r="D150" s="64"/>
       <c r="E150" s="40" t="s">
         <v>1041</v>
       </c>
@@ -14078,7 +14078,7 @@
       <c r="C151" s="40" t="s">
         <v>834</v>
       </c>
-      <c r="D151" s="61"/>
+      <c r="D151" s="64"/>
       <c r="E151" s="40" t="s">
         <v>1038</v>
       </c>
@@ -14093,7 +14093,7 @@
       <c r="C152" s="40" t="s">
         <v>836</v>
       </c>
-      <c r="D152" s="61"/>
+      <c r="D152" s="64"/>
       <c r="E152" s="40" t="s">
         <v>1043</v>
       </c>
@@ -14108,7 +14108,7 @@
       <c r="C153" s="40" t="s">
         <v>838</v>
       </c>
-      <c r="D153" s="61"/>
+      <c r="D153" s="64"/>
       <c r="E153" s="40" t="s">
         <v>1034</v>
       </c>
@@ -14123,7 +14123,7 @@
       <c r="C154" s="40" t="s">
         <v>839</v>
       </c>
-      <c r="D154" s="61"/>
+      <c r="D154" s="64"/>
       <c r="E154" s="40" t="s">
         <v>1048</v>
       </c>
@@ -14138,7 +14138,7 @@
       <c r="C155" s="40" t="s">
         <v>841</v>
       </c>
-      <c r="D155" s="61"/>
+      <c r="D155" s="64"/>
       <c r="E155" s="40" t="s">
         <v>1024</v>
       </c>
@@ -14153,7 +14153,7 @@
       <c r="C156" s="40" t="s">
         <v>842</v>
       </c>
-      <c r="D156" s="61"/>
+      <c r="D156" s="64"/>
       <c r="E156" s="40" t="s">
         <v>1029</v>
       </c>
@@ -14168,7 +14168,7 @@
       <c r="C157" s="40" t="s">
         <v>844</v>
       </c>
-      <c r="D157" s="61"/>
+      <c r="D157" s="64"/>
       <c r="E157" s="40" t="s">
         <v>1052</v>
       </c>
@@ -14183,7 +14183,7 @@
       <c r="C158" s="40" t="s">
         <v>846</v>
       </c>
-      <c r="D158" s="61"/>
+      <c r="D158" s="64"/>
       <c r="E158" s="40" t="s">
         <v>1050</v>
       </c>
@@ -14198,7 +14198,7 @@
       <c r="C159" s="40" t="s">
         <v>848</v>
       </c>
-      <c r="D159" s="61"/>
+      <c r="D159" s="64"/>
       <c r="E159" s="40" t="s">
         <v>69</v>
       </c>
@@ -14213,7 +14213,7 @@
       <c r="C160" s="40" t="s">
         <v>850</v>
       </c>
-      <c r="D160" s="61"/>
+      <c r="D160" s="64"/>
       <c r="E160" s="40" t="s">
         <v>1059</v>
       </c>
@@ -14228,7 +14228,7 @@
       <c r="C161" s="40" t="s">
         <v>852</v>
       </c>
-      <c r="D161" s="61"/>
+      <c r="D161" s="64"/>
       <c r="E161" s="40" t="s">
         <v>1062</v>
       </c>
@@ -14243,7 +14243,7 @@
       <c r="C162" s="40" t="s">
         <v>854</v>
       </c>
-      <c r="D162" s="61"/>
+      <c r="D162" s="64"/>
       <c r="E162" s="40" t="s">
         <v>1067</v>
       </c>
@@ -14258,7 +14258,7 @@
       <c r="C163" s="40" t="s">
         <v>856</v>
       </c>
-      <c r="D163" s="61"/>
+      <c r="D163" s="64"/>
       <c r="E163" s="40" t="s">
         <v>1069</v>
       </c>
@@ -14273,7 +14273,7 @@
       <c r="C164" s="40" t="s">
         <v>858</v>
       </c>
-      <c r="D164" s="61"/>
+      <c r="D164" s="64"/>
       <c r="E164" s="40" t="s">
         <v>1071</v>
       </c>
@@ -14288,7 +14288,7 @@
       <c r="C165" s="40" t="s">
         <v>859</v>
       </c>
-      <c r="D165" s="61"/>
+      <c r="D165" s="64"/>
       <c r="E165" s="40" t="s">
         <v>1064</v>
       </c>
@@ -14303,7 +14303,7 @@
       <c r="C166" s="40" t="s">
         <v>861</v>
       </c>
-      <c r="D166" s="61"/>
+      <c r="D166" s="64"/>
       <c r="E166" s="40" t="s">
         <v>979</v>
       </c>
@@ -14318,7 +14318,7 @@
       <c r="C167" s="40" t="s">
         <v>863</v>
       </c>
-      <c r="D167" s="61"/>
+      <c r="D167" s="64"/>
       <c r="E167" s="40" t="s">
         <v>693</v>
       </c>
@@ -14333,7 +14333,7 @@
       <c r="C168" s="40" t="s">
         <v>865</v>
       </c>
-      <c r="D168" s="61"/>
+      <c r="D168" s="64"/>
       <c r="E168" s="40" t="s">
         <v>993</v>
       </c>
@@ -14348,7 +14348,7 @@
       <c r="C169" s="40" t="s">
         <v>867</v>
       </c>
-      <c r="D169" s="61"/>
+      <c r="D169" s="64"/>
       <c r="E169" s="40" t="s">
         <v>781</v>
       </c>
@@ -14363,7 +14363,7 @@
       <c r="C170" s="40" t="s">
         <v>868</v>
       </c>
-      <c r="D170" s="61"/>
+      <c r="D170" s="64"/>
       <c r="E170" s="40" t="s">
         <v>632</v>
       </c>
@@ -14378,7 +14378,7 @@
       <c r="C171" s="40" t="s">
         <v>870</v>
       </c>
-      <c r="D171" s="61"/>
+      <c r="D171" s="64"/>
       <c r="E171" s="40" t="s">
         <v>816</v>
       </c>
@@ -14393,7 +14393,7 @@
       <c r="C172" s="40" t="s">
         <v>872</v>
       </c>
-      <c r="D172" s="61"/>
+      <c r="D172" s="64"/>
       <c r="E172" s="40" t="s">
         <v>659</v>
       </c>
@@ -14408,7 +14408,7 @@
       <c r="C173" s="40" t="s">
         <v>874</v>
       </c>
-      <c r="D173" s="61"/>
+      <c r="D173" s="64"/>
       <c r="E173" s="40" t="s">
         <v>937</v>
       </c>
@@ -14423,7 +14423,7 @@
       <c r="C174" s="40" t="s">
         <v>875</v>
       </c>
-      <c r="D174" s="61"/>
+      <c r="D174" s="64"/>
       <c r="E174" s="40" t="s">
         <v>713</v>
       </c>
@@ -14438,7 +14438,7 @@
       <c r="C175" s="40" t="s">
         <v>877</v>
       </c>
-      <c r="D175" s="61"/>
+      <c r="D175" s="64"/>
       <c r="E175" s="40" t="s">
         <v>951</v>
       </c>
@@ -14453,7 +14453,7 @@
       <c r="C176" s="40" t="s">
         <v>879</v>
       </c>
-      <c r="D176" s="61"/>
+      <c r="D176" s="64"/>
       <c r="E176" s="40" t="s">
         <v>1078</v>
       </c>
@@ -14468,7 +14468,7 @@
       <c r="C177" s="40" t="s">
         <v>881</v>
       </c>
-      <c r="D177" s="61"/>
+      <c r="D177" s="64"/>
       <c r="E177" s="40" t="s">
         <v>218</v>
       </c>
@@ -14483,7 +14483,7 @@
       <c r="C178" s="56" t="s">
         <v>882</v>
       </c>
-      <c r="D178" s="61"/>
+      <c r="D178" s="64"/>
       <c r="E178" s="40" t="s">
         <v>1080</v>
       </c>
@@ -14498,7 +14498,7 @@
       <c r="C179" s="40" t="s">
         <v>883</v>
       </c>
-      <c r="D179" s="61"/>
+      <c r="D179" s="64"/>
       <c r="E179" s="40" t="s">
         <v>1082</v>
       </c>
@@ -14513,7 +14513,7 @@
       <c r="C180" s="40" t="s">
         <v>885</v>
       </c>
-      <c r="D180" s="61"/>
+      <c r="D180" s="64"/>
       <c r="E180" s="81"/>
       <c r="F180" s="81"/>
     </row>
@@ -14524,7 +14524,7 @@
       <c r="C181" s="40" t="s">
         <v>886</v>
       </c>
-      <c r="D181" s="61"/>
+      <c r="D181" s="64"/>
       <c r="E181" s="81"/>
       <c r="F181" s="81"/>
     </row>
@@ -14535,7 +14535,7 @@
       <c r="C182" s="40" t="s">
         <v>887</v>
       </c>
-      <c r="D182" s="61"/>
+      <c r="D182" s="64"/>
       <c r="E182" s="81"/>
       <c r="F182" s="81"/>
     </row>
@@ -14546,7 +14546,7 @@
       <c r="C183" s="40" t="s">
         <v>888</v>
       </c>
-      <c r="D183" s="61"/>
+      <c r="D183" s="64"/>
       <c r="E183" s="81"/>
       <c r="F183" s="81"/>
     </row>
@@ -14557,7 +14557,7 @@
       <c r="C184" s="40" t="s">
         <v>889</v>
       </c>
-      <c r="D184" s="61"/>
+      <c r="D184" s="64"/>
       <c r="E184" s="81"/>
       <c r="F184" s="81"/>
     </row>
@@ -14568,7 +14568,7 @@
       <c r="C185" s="40" t="s">
         <v>891</v>
       </c>
-      <c r="D185" s="61"/>
+      <c r="D185" s="64"/>
       <c r="E185" s="81"/>
       <c r="F185" s="81"/>
     </row>
@@ -14579,7 +14579,7 @@
       <c r="C186" s="40" t="s">
         <v>893</v>
       </c>
-      <c r="D186" s="61"/>
+      <c r="D186" s="64"/>
       <c r="E186" s="81"/>
       <c r="F186" s="81"/>
     </row>
@@ -14590,7 +14590,7 @@
       <c r="C187" s="40" t="s">
         <v>894</v>
       </c>
-      <c r="D187" s="61"/>
+      <c r="D187" s="64"/>
       <c r="E187" s="81"/>
       <c r="F187" s="81"/>
     </row>
@@ -14601,7 +14601,7 @@
       <c r="C188" s="40" t="s">
         <v>895</v>
       </c>
-      <c r="D188" s="61"/>
+      <c r="D188" s="64"/>
       <c r="E188" s="81"/>
       <c r="F188" s="81"/>
     </row>
@@ -14612,7 +14612,7 @@
       <c r="C189" s="40" t="s">
         <v>896</v>
       </c>
-      <c r="D189" s="61"/>
+      <c r="D189" s="64"/>
       <c r="E189" s="81"/>
       <c r="F189" s="81"/>
     </row>
@@ -14623,7 +14623,7 @@
       <c r="C190" s="40" t="s">
         <v>897</v>
       </c>
-      <c r="D190" s="61"/>
+      <c r="D190" s="64"/>
       <c r="E190" s="81"/>
       <c r="F190" s="81"/>
     </row>
@@ -14634,7 +14634,7 @@
       <c r="C191" s="40" t="s">
         <v>898</v>
       </c>
-      <c r="D191" s="61"/>
+      <c r="D191" s="64"/>
       <c r="E191" s="81"/>
       <c r="F191" s="81"/>
     </row>
@@ -14645,7 +14645,7 @@
       <c r="C192" s="40" t="s">
         <v>899</v>
       </c>
-      <c r="D192" s="61"/>
+      <c r="D192" s="64"/>
       <c r="E192" s="81"/>
       <c r="F192" s="81"/>
     </row>
@@ -14656,7 +14656,7 @@
       <c r="C193" s="40" t="s">
         <v>901</v>
       </c>
-      <c r="D193" s="61"/>
+      <c r="D193" s="64"/>
       <c r="E193" s="81"/>
       <c r="F193" s="81"/>
     </row>
@@ -14667,7 +14667,7 @@
       <c r="C194" s="40" t="s">
         <v>902</v>
       </c>
-      <c r="D194" s="61"/>
+      <c r="D194" s="64"/>
       <c r="E194" s="81"/>
       <c r="F194" s="81"/>
     </row>
@@ -14678,7 +14678,7 @@
       <c r="C195" s="40" t="s">
         <v>904</v>
       </c>
-      <c r="D195" s="61"/>
+      <c r="D195" s="64"/>
       <c r="E195" s="81"/>
       <c r="F195" s="81"/>
     </row>
@@ -14689,7 +14689,7 @@
       <c r="C196" s="40" t="s">
         <v>905</v>
       </c>
-      <c r="D196" s="61"/>
+      <c r="D196" s="64"/>
       <c r="E196" s="81"/>
       <c r="F196" s="81"/>
     </row>
@@ -14700,7 +14700,7 @@
       <c r="C197" s="40" t="s">
         <v>906</v>
       </c>
-      <c r="D197" s="61"/>
+      <c r="D197" s="64"/>
       <c r="E197" s="81"/>
       <c r="F197" s="81"/>
     </row>
@@ -14711,7 +14711,7 @@
       <c r="C198" s="40" t="s">
         <v>908</v>
       </c>
-      <c r="D198" s="61"/>
+      <c r="D198" s="64"/>
       <c r="E198" s="81"/>
       <c r="F198" s="81"/>
     </row>
@@ -14722,7 +14722,7 @@
       <c r="C199" s="40" t="s">
         <v>910</v>
       </c>
-      <c r="D199" s="61"/>
+      <c r="D199" s="64"/>
       <c r="E199" s="81"/>
       <c r="F199" s="81"/>
     </row>
@@ -14733,7 +14733,7 @@
       <c r="C200" s="40" t="s">
         <v>911</v>
       </c>
-      <c r="D200" s="61"/>
+      <c r="D200" s="64"/>
       <c r="E200" s="81"/>
       <c r="F200" s="81"/>
     </row>
@@ -14744,7 +14744,7 @@
       <c r="C201" s="40" t="s">
         <v>913</v>
       </c>
-      <c r="D201" s="61"/>
+      <c r="D201" s="64"/>
       <c r="E201" s="81"/>
       <c r="F201" s="81"/>
     </row>
@@ -14755,7 +14755,7 @@
       <c r="C202" s="40" t="s">
         <v>914</v>
       </c>
-      <c r="D202" s="61"/>
+      <c r="D202" s="64"/>
       <c r="E202" s="81"/>
       <c r="F202" s="81"/>
     </row>
@@ -14766,7 +14766,7 @@
       <c r="C203" s="40" t="s">
         <v>915</v>
       </c>
-      <c r="D203" s="61"/>
+      <c r="D203" s="64"/>
       <c r="E203" s="81"/>
       <c r="F203" s="81"/>
     </row>
@@ -14777,7 +14777,7 @@
       <c r="C204" s="40" t="s">
         <v>917</v>
       </c>
-      <c r="D204" s="61"/>
+      <c r="D204" s="64"/>
       <c r="E204" s="81"/>
       <c r="F204" s="81"/>
     </row>
@@ -14788,7 +14788,7 @@
       <c r="C205" s="40" t="s">
         <v>918</v>
       </c>
-      <c r="D205" s="61"/>
+      <c r="D205" s="64"/>
       <c r="E205" s="81"/>
       <c r="F205" s="81"/>
     </row>
@@ -14799,7 +14799,7 @@
       <c r="C206" s="40" t="s">
         <v>919</v>
       </c>
-      <c r="D206" s="61"/>
+      <c r="D206" s="64"/>
       <c r="E206" s="81"/>
       <c r="F206" s="81"/>
     </row>
@@ -14810,7 +14810,7 @@
       <c r="C207" s="40" t="s">
         <v>920</v>
       </c>
-      <c r="D207" s="61"/>
+      <c r="D207" s="64"/>
       <c r="E207" s="81"/>
       <c r="F207" s="81"/>
     </row>
@@ -14821,7 +14821,7 @@
       <c r="C208" s="40" t="s">
         <v>921</v>
       </c>
-      <c r="D208" s="61"/>
+      <c r="D208" s="64"/>
       <c r="E208" s="81"/>
       <c r="F208" s="81"/>
     </row>
@@ -14832,7 +14832,7 @@
       <c r="C209" s="40" t="s">
         <v>922</v>
       </c>
-      <c r="D209" s="61"/>
+      <c r="D209" s="64"/>
       <c r="E209" s="81"/>
       <c r="F209" s="81"/>
     </row>
@@ -14843,7 +14843,7 @@
       <c r="C210" s="40" t="s">
         <v>924</v>
       </c>
-      <c r="D210" s="61"/>
+      <c r="D210" s="64"/>
       <c r="E210" s="81"/>
       <c r="F210" s="81"/>
     </row>
@@ -14854,7 +14854,7 @@
       <c r="C211" s="56" t="s">
         <v>925</v>
       </c>
-      <c r="D211" s="61"/>
+      <c r="D211" s="64"/>
       <c r="E211" s="81"/>
       <c r="F211" s="81"/>
     </row>
@@ -14865,7 +14865,7 @@
       <c r="C212" s="40" t="s">
         <v>927</v>
       </c>
-      <c r="D212" s="61"/>
+      <c r="D212" s="64"/>
       <c r="E212" s="81"/>
       <c r="F212" s="81"/>
     </row>
@@ -14876,7 +14876,7 @@
       <c r="C213" s="40" t="s">
         <v>928</v>
       </c>
-      <c r="D213" s="61"/>
+      <c r="D213" s="64"/>
       <c r="E213" s="81"/>
       <c r="F213" s="81"/>
     </row>
@@ -14887,7 +14887,7 @@
       <c r="C214" s="40" t="s">
         <v>929</v>
       </c>
-      <c r="D214" s="61"/>
+      <c r="D214" s="64"/>
       <c r="E214" s="81"/>
       <c r="F214" s="81"/>
     </row>
@@ -14898,7 +14898,7 @@
       <c r="C215" s="40" t="s">
         <v>930</v>
       </c>
-      <c r="D215" s="61"/>
+      <c r="D215" s="64"/>
       <c r="E215" s="81"/>
       <c r="F215" s="81"/>
     </row>
@@ -14909,7 +14909,7 @@
       <c r="C216" s="40" t="s">
         <v>931</v>
       </c>
-      <c r="D216" s="61"/>
+      <c r="D216" s="64"/>
       <c r="E216" s="81"/>
       <c r="F216" s="81"/>
     </row>
@@ -14920,7 +14920,7 @@
       <c r="C217" s="40" t="s">
         <v>933</v>
       </c>
-      <c r="D217" s="61"/>
+      <c r="D217" s="64"/>
       <c r="E217" s="81"/>
       <c r="F217" s="81"/>
     </row>
@@ -14931,7 +14931,7 @@
       <c r="C218" s="40" t="s">
         <v>935</v>
       </c>
-      <c r="D218" s="61"/>
+      <c r="D218" s="64"/>
       <c r="E218" s="81"/>
       <c r="F218" s="81"/>
     </row>
@@ -14942,7 +14942,7 @@
       <c r="C219" s="40" t="s">
         <v>936</v>
       </c>
-      <c r="D219" s="61"/>
+      <c r="D219" s="64"/>
       <c r="E219" s="81"/>
       <c r="F219" s="81"/>
     </row>
@@ -14953,7 +14953,7 @@
       <c r="C220" s="40" t="s">
         <v>938</v>
       </c>
-      <c r="D220" s="61"/>
+      <c r="D220" s="64"/>
       <c r="E220" s="81"/>
       <c r="F220" s="81"/>
     </row>
@@ -14964,7 +14964,7 @@
       <c r="C221" s="40" t="s">
         <v>940</v>
       </c>
-      <c r="D221" s="61"/>
+      <c r="D221" s="64"/>
       <c r="E221" s="81"/>
       <c r="F221" s="81"/>
     </row>
@@ -14975,7 +14975,7 @@
       <c r="C222" s="40" t="s">
         <v>941</v>
       </c>
-      <c r="D222" s="61"/>
+      <c r="D222" s="64"/>
       <c r="E222" s="81"/>
       <c r="F222" s="81"/>
     </row>
@@ -14986,7 +14986,7 @@
       <c r="C223" s="40" t="s">
         <v>943</v>
       </c>
-      <c r="D223" s="61"/>
+      <c r="D223" s="64"/>
       <c r="E223" s="81"/>
       <c r="F223" s="81"/>
     </row>
@@ -14997,7 +14997,7 @@
       <c r="C224" s="40" t="s">
         <v>945</v>
       </c>
-      <c r="D224" s="61"/>
+      <c r="D224" s="64"/>
       <c r="E224" s="81"/>
       <c r="F224" s="81"/>
     </row>
@@ -15008,7 +15008,7 @@
       <c r="C225" s="40" t="s">
         <v>947</v>
       </c>
-      <c r="D225" s="61"/>
+      <c r="D225" s="64"/>
       <c r="E225" s="81"/>
       <c r="F225" s="81"/>
     </row>
@@ -15019,7 +15019,7 @@
       <c r="C226" s="40" t="s">
         <v>949</v>
       </c>
-      <c r="D226" s="61"/>
+      <c r="D226" s="64"/>
       <c r="E226" s="81"/>
       <c r="F226" s="81"/>
     </row>
@@ -15030,7 +15030,7 @@
       <c r="C227" s="40" t="s">
         <v>950</v>
       </c>
-      <c r="D227" s="61"/>
+      <c r="D227" s="64"/>
       <c r="E227" s="81"/>
       <c r="F227" s="81"/>
     </row>
@@ -15041,7 +15041,7 @@
       <c r="C228" s="40" t="s">
         <v>952</v>
       </c>
-      <c r="D228" s="61"/>
+      <c r="D228" s="64"/>
       <c r="E228" s="81"/>
       <c r="F228" s="81"/>
     </row>
@@ -15052,7 +15052,7 @@
       <c r="C229" s="40" t="s">
         <v>954</v>
       </c>
-      <c r="D229" s="61"/>
+      <c r="D229" s="64"/>
       <c r="E229" s="81"/>
       <c r="F229" s="81"/>
     </row>
@@ -15063,7 +15063,7 @@
       <c r="C230" s="40" t="s">
         <v>955</v>
       </c>
-      <c r="D230" s="61"/>
+      <c r="D230" s="64"/>
       <c r="E230" s="81"/>
       <c r="F230" s="81"/>
     </row>
@@ -15074,7 +15074,7 @@
       <c r="C231" s="40" t="s">
         <v>957</v>
       </c>
-      <c r="D231" s="61"/>
+      <c r="D231" s="64"/>
       <c r="E231" s="81"/>
       <c r="F231" s="81"/>
     </row>
@@ -15085,7 +15085,7 @@
       <c r="C232" s="40" t="s">
         <v>958</v>
       </c>
-      <c r="D232" s="61"/>
+      <c r="D232" s="64"/>
       <c r="E232" s="81"/>
       <c r="F232" s="81"/>
     </row>
@@ -15096,7 +15096,7 @@
       <c r="C233" s="40" t="s">
         <v>960</v>
       </c>
-      <c r="D233" s="61"/>
+      <c r="D233" s="64"/>
       <c r="E233" s="81"/>
       <c r="F233" s="81"/>
     </row>
@@ -15107,7 +15107,7 @@
       <c r="C234" s="40" t="s">
         <v>961</v>
       </c>
-      <c r="D234" s="61"/>
+      <c r="D234" s="64"/>
       <c r="E234" s="81"/>
       <c r="F234" s="81"/>
     </row>
@@ -15118,7 +15118,7 @@
       <c r="C235" s="40" t="s">
         <v>963</v>
       </c>
-      <c r="D235" s="61"/>
+      <c r="D235" s="64"/>
       <c r="E235" s="81"/>
       <c r="F235" s="81"/>
     </row>
@@ -15129,7 +15129,7 @@
       <c r="C236" s="40" t="s">
         <v>964</v>
       </c>
-      <c r="D236" s="61"/>
+      <c r="D236" s="64"/>
       <c r="E236" s="81"/>
       <c r="F236" s="81"/>
     </row>
@@ -15140,7 +15140,7 @@
       <c r="C237" s="40" t="s">
         <v>966</v>
       </c>
-      <c r="D237" s="61"/>
+      <c r="D237" s="64"/>
       <c r="E237" s="81"/>
       <c r="F237" s="81"/>
     </row>
@@ -15151,7 +15151,7 @@
       <c r="C238" s="40" t="s">
         <v>967</v>
       </c>
-      <c r="D238" s="61"/>
+      <c r="D238" s="64"/>
       <c r="E238" s="81"/>
       <c r="F238" s="81"/>
     </row>
@@ -15162,7 +15162,7 @@
       <c r="C239" s="40" t="s">
         <v>968</v>
       </c>
-      <c r="D239" s="61"/>
+      <c r="D239" s="64"/>
       <c r="E239" s="81"/>
       <c r="F239" s="81"/>
     </row>
@@ -15173,7 +15173,7 @@
       <c r="C240" s="40" t="s">
         <v>969</v>
       </c>
-      <c r="D240" s="61"/>
+      <c r="D240" s="64"/>
       <c r="E240" s="81"/>
       <c r="F240" s="81"/>
     </row>
@@ -15184,7 +15184,7 @@
       <c r="C241" s="40" t="s">
         <v>970</v>
       </c>
-      <c r="D241" s="61"/>
+      <c r="D241" s="64"/>
       <c r="E241" s="81"/>
       <c r="F241" s="81"/>
     </row>
@@ -15195,7 +15195,7 @@
       <c r="C242" s="40" t="s">
         <v>972</v>
       </c>
-      <c r="D242" s="61"/>
+      <c r="D242" s="64"/>
       <c r="E242" s="81"/>
       <c r="F242" s="81"/>
     </row>
@@ -15206,7 +15206,7 @@
       <c r="C243" s="40" t="s">
         <v>973</v>
       </c>
-      <c r="D243" s="61"/>
+      <c r="D243" s="64"/>
       <c r="E243" s="81"/>
       <c r="F243" s="81"/>
     </row>
@@ -15217,7 +15217,7 @@
       <c r="C244" s="40" t="s">
         <v>974</v>
       </c>
-      <c r="D244" s="61"/>
+      <c r="D244" s="64"/>
       <c r="E244" s="81"/>
       <c r="F244" s="81"/>
     </row>
@@ -15228,7 +15228,7 @@
       <c r="C245" s="40" t="s">
         <v>975</v>
       </c>
-      <c r="D245" s="61"/>
+      <c r="D245" s="64"/>
       <c r="E245" s="81"/>
       <c r="F245" s="81"/>
     </row>
@@ -15239,7 +15239,7 @@
       <c r="C246" s="40" t="s">
         <v>976</v>
       </c>
-      <c r="D246" s="61"/>
+      <c r="D246" s="64"/>
       <c r="E246" s="81"/>
       <c r="F246" s="81"/>
     </row>
@@ -15250,7 +15250,7 @@
       <c r="C247" s="40" t="s">
         <v>977</v>
       </c>
-      <c r="D247" s="61"/>
+      <c r="D247" s="64"/>
       <c r="E247" s="81"/>
       <c r="F247" s="81"/>
     </row>
@@ -15261,7 +15261,7 @@
       <c r="C248" s="40" t="s">
         <v>978</v>
       </c>
-      <c r="D248" s="61"/>
+      <c r="D248" s="64"/>
       <c r="E248" s="81"/>
       <c r="F248" s="81"/>
     </row>
@@ -15272,7 +15272,7 @@
       <c r="C249" s="40" t="s">
         <v>980</v>
       </c>
-      <c r="D249" s="61"/>
+      <c r="D249" s="64"/>
       <c r="E249" s="81"/>
       <c r="F249" s="81"/>
     </row>
@@ -15283,7 +15283,7 @@
       <c r="C250" s="40" t="s">
         <v>981</v>
       </c>
-      <c r="D250" s="61"/>
+      <c r="D250" s="64"/>
       <c r="E250" s="81"/>
       <c r="F250" s="81"/>
     </row>
@@ -15294,7 +15294,7 @@
       <c r="C251" s="40" t="s">
         <v>983</v>
       </c>
-      <c r="D251" s="61"/>
+      <c r="D251" s="64"/>
       <c r="E251" s="81"/>
       <c r="F251" s="81"/>
     </row>
@@ -15305,7 +15305,7 @@
       <c r="C252" s="40" t="s">
         <v>985</v>
       </c>
-      <c r="D252" s="61"/>
+      <c r="D252" s="64"/>
       <c r="E252" s="81"/>
       <c r="F252" s="81"/>
     </row>
@@ -15316,7 +15316,7 @@
       <c r="C253" s="56" t="s">
         <v>986</v>
       </c>
-      <c r="D253" s="61"/>
+      <c r="D253" s="64"/>
       <c r="E253" s="81"/>
       <c r="F253" s="81"/>
     </row>
@@ -15327,7 +15327,7 @@
       <c r="C254" s="40" t="s">
         <v>988</v>
       </c>
-      <c r="D254" s="61"/>
+      <c r="D254" s="64"/>
       <c r="E254" s="81"/>
       <c r="F254" s="81"/>
     </row>
@@ -15338,7 +15338,7 @@
       <c r="C255" s="40" t="s">
         <v>990</v>
       </c>
-      <c r="D255" s="61"/>
+      <c r="D255" s="64"/>
       <c r="E255" s="81"/>
       <c r="F255" s="81"/>
     </row>
@@ -15349,7 +15349,7 @@
       <c r="C256" s="40" t="s">
         <v>992</v>
       </c>
-      <c r="D256" s="61"/>
+      <c r="D256" s="64"/>
       <c r="E256" s="81"/>
       <c r="F256" s="81"/>
     </row>
@@ -15360,7 +15360,7 @@
       <c r="C257" s="40" t="s">
         <v>994</v>
       </c>
-      <c r="D257" s="61"/>
+      <c r="D257" s="64"/>
       <c r="E257" s="81"/>
       <c r="F257" s="81"/>
     </row>
@@ -15371,7 +15371,7 @@
       <c r="C258" s="40" t="s">
         <v>996</v>
       </c>
-      <c r="D258" s="61"/>
+      <c r="D258" s="64"/>
       <c r="E258" s="81"/>
       <c r="F258" s="81"/>
     </row>
@@ -15382,7 +15382,7 @@
       <c r="C259" s="40" t="s">
         <v>997</v>
       </c>
-      <c r="D259" s="61"/>
+      <c r="D259" s="64"/>
       <c r="E259" s="81"/>
       <c r="F259" s="81"/>
     </row>
@@ -15393,7 +15393,7 @@
       <c r="C260" s="40" t="s">
         <v>998</v>
       </c>
-      <c r="D260" s="61"/>
+      <c r="D260" s="64"/>
       <c r="E260" s="81"/>
       <c r="F260" s="81"/>
     </row>
@@ -15404,7 +15404,7 @@
       <c r="C261" s="40" t="s">
         <v>999</v>
       </c>
-      <c r="D261" s="61"/>
+      <c r="D261" s="64"/>
       <c r="E261" s="81"/>
       <c r="F261" s="81"/>
     </row>
@@ -15415,7 +15415,7 @@
       <c r="C262" s="40" t="s">
         <v>1000</v>
       </c>
-      <c r="D262" s="61"/>
+      <c r="D262" s="64"/>
       <c r="E262" s="81"/>
       <c r="F262" s="81"/>
     </row>
@@ -15426,7 +15426,7 @@
       <c r="C263" s="40" t="s">
         <v>1002</v>
       </c>
-      <c r="D263" s="61"/>
+      <c r="D263" s="64"/>
       <c r="E263" s="81"/>
       <c r="F263" s="81"/>
     </row>
@@ -15437,7 +15437,7 @@
       <c r="C264" s="40" t="s">
         <v>1004</v>
       </c>
-      <c r="D264" s="61"/>
+      <c r="D264" s="64"/>
       <c r="E264" s="81"/>
       <c r="F264" s="81"/>
     </row>
@@ -15448,7 +15448,7 @@
       <c r="C265" s="40" t="s">
         <v>1005</v>
       </c>
-      <c r="D265" s="61"/>
+      <c r="D265" s="64"/>
       <c r="E265" s="81"/>
       <c r="F265" s="81"/>
     </row>
@@ -15459,7 +15459,7 @@
       <c r="C266" s="40" t="s">
         <v>1006</v>
       </c>
-      <c r="D266" s="61"/>
+      <c r="D266" s="64"/>
       <c r="E266" s="81"/>
       <c r="F266" s="81"/>
     </row>
@@ -15470,7 +15470,7 @@
       <c r="C267" s="40" t="s">
         <v>1007</v>
       </c>
-      <c r="D267" s="61"/>
+      <c r="D267" s="64"/>
       <c r="E267" s="81"/>
       <c r="F267" s="81"/>
     </row>
@@ -15481,7 +15481,7 @@
       <c r="C268" s="40" t="s">
         <v>1008</v>
       </c>
-      <c r="D268" s="61"/>
+      <c r="D268" s="64"/>
       <c r="E268" s="81"/>
       <c r="F268" s="81"/>
     </row>
@@ -15492,7 +15492,7 @@
       <c r="C269" s="40" t="s">
         <v>1009</v>
       </c>
-      <c r="D269" s="61"/>
+      <c r="D269" s="64"/>
       <c r="E269" s="81"/>
       <c r="F269" s="81"/>
     </row>
@@ -15503,7 +15503,7 @@
       <c r="C270" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="D270" s="61"/>
+      <c r="D270" s="64"/>
       <c r="E270" s="81"/>
       <c r="F270" s="81"/>
     </row>
@@ -15514,7 +15514,7 @@
       <c r="C271" s="40" t="s">
         <v>1013</v>
       </c>
-      <c r="D271" s="61"/>
+      <c r="D271" s="64"/>
       <c r="E271" s="81"/>
       <c r="F271" s="81"/>
     </row>
@@ -15525,7 +15525,7 @@
       <c r="C272" s="40" t="s">
         <v>1015</v>
       </c>
-      <c r="D272" s="61"/>
+      <c r="D272" s="64"/>
       <c r="E272" s="81"/>
       <c r="F272" s="81"/>
     </row>
@@ -15536,7 +15536,7 @@
       <c r="C273" s="40" t="s">
         <v>1016</v>
       </c>
-      <c r="D273" s="61"/>
+      <c r="D273" s="64"/>
       <c r="E273" s="81"/>
       <c r="F273" s="81"/>
     </row>
@@ -15547,7 +15547,7 @@
       <c r="C274" s="40" t="s">
         <v>1018</v>
       </c>
-      <c r="D274" s="61"/>
+      <c r="D274" s="64"/>
       <c r="E274" s="81"/>
       <c r="F274" s="81"/>
     </row>
@@ -15558,7 +15558,7 @@
       <c r="C275" s="40" t="s">
         <v>1020</v>
       </c>
-      <c r="D275" s="61"/>
+      <c r="D275" s="64"/>
       <c r="E275" s="81"/>
       <c r="F275" s="81"/>
     </row>
@@ -15569,7 +15569,7 @@
       <c r="C276" s="40" t="s">
         <v>1021</v>
       </c>
-      <c r="D276" s="61"/>
+      <c r="D276" s="64"/>
       <c r="E276" s="81"/>
       <c r="F276" s="81"/>
     </row>
@@ -15580,7 +15580,7 @@
       <c r="C277" s="40" t="s">
         <v>1023</v>
       </c>
-      <c r="D277" s="61"/>
+      <c r="D277" s="64"/>
       <c r="E277" s="81"/>
       <c r="F277" s="81"/>
     </row>
@@ -15591,7 +15591,7 @@
       <c r="C278" s="40" t="s">
         <v>1025</v>
       </c>
-      <c r="D278" s="61"/>
+      <c r="D278" s="64"/>
       <c r="E278" s="81"/>
       <c r="F278" s="81"/>
     </row>
@@ -15602,7 +15602,7 @@
       <c r="C279" s="40" t="s">
         <v>1026</v>
       </c>
-      <c r="D279" s="61"/>
+      <c r="D279" s="64"/>
     </row>
     <row r="280" spans="2:6">
       <c r="B280" s="40" t="s">
@@ -15611,7 +15611,7 @@
       <c r="C280" s="40" t="s">
         <v>1028</v>
       </c>
-      <c r="D280" s="61"/>
+      <c r="D280" s="64"/>
     </row>
     <row r="281" spans="2:6">
       <c r="B281" s="40" t="s">
@@ -15620,7 +15620,7 @@
       <c r="C281" s="40" t="s">
         <v>1030</v>
       </c>
-      <c r="D281" s="61"/>
+      <c r="D281" s="64"/>
     </row>
     <row r="282" spans="2:6">
       <c r="B282" s="40" t="s">
@@ -15629,7 +15629,7 @@
       <c r="C282" s="40" t="s">
         <v>1032</v>
       </c>
-      <c r="D282" s="61"/>
+      <c r="D282" s="64"/>
     </row>
     <row r="283" spans="2:6">
       <c r="B283" s="40" t="s">
@@ -15638,7 +15638,7 @@
       <c r="C283" s="40" t="s">
         <v>1033</v>
       </c>
-      <c r="D283" s="61"/>
+      <c r="D283" s="64"/>
     </row>
     <row r="284" spans="2:6">
       <c r="B284" s="40" t="s">
@@ -15647,7 +15647,7 @@
       <c r="C284" s="40" t="s">
         <v>1035</v>
       </c>
-      <c r="D284" s="61"/>
+      <c r="D284" s="64"/>
     </row>
     <row r="285" spans="2:6" ht="30">
       <c r="B285" s="40" t="s">
@@ -15656,7 +15656,7 @@
       <c r="C285" s="56" t="s">
         <v>1036</v>
       </c>
-      <c r="D285" s="61"/>
+      <c r="D285" s="64"/>
     </row>
     <row r="286" spans="2:6">
       <c r="B286" s="40" t="s">
@@ -15665,7 +15665,7 @@
       <c r="C286" s="40" t="s">
         <v>1037</v>
       </c>
-      <c r="D286" s="61"/>
+      <c r="D286" s="64"/>
     </row>
     <row r="287" spans="2:6">
       <c r="B287" s="40" t="s">
@@ -15674,7 +15674,7 @@
       <c r="C287" s="40" t="s">
         <v>1039</v>
       </c>
-      <c r="D287" s="61"/>
+      <c r="D287" s="64"/>
     </row>
     <row r="288" spans="2:6">
       <c r="B288" s="40" t="s">
@@ -15683,7 +15683,7 @@
       <c r="C288" s="40" t="s">
         <v>1040</v>
       </c>
-      <c r="D288" s="61"/>
+      <c r="D288" s="64"/>
     </row>
     <row r="289" spans="2:4">
       <c r="B289" s="40" t="s">
@@ -15692,7 +15692,7 @@
       <c r="C289" s="40" t="s">
         <v>1042</v>
       </c>
-      <c r="D289" s="61"/>
+      <c r="D289" s="64"/>
     </row>
     <row r="290" spans="2:4">
       <c r="B290" s="40" t="s">
@@ -15701,7 +15701,7 @@
       <c r="C290" s="40" t="s">
         <v>1044</v>
       </c>
-      <c r="D290" s="61"/>
+      <c r="D290" s="64"/>
     </row>
     <row r="291" spans="2:4">
       <c r="B291" s="40" t="s">
@@ -15710,7 +15710,7 @@
       <c r="C291" s="40" t="s">
         <v>1046</v>
       </c>
-      <c r="D291" s="61"/>
+      <c r="D291" s="64"/>
     </row>
     <row r="292" spans="2:4" ht="30">
       <c r="B292" s="40" t="s">
@@ -15719,7 +15719,7 @@
       <c r="C292" s="40" t="s">
         <v>1047</v>
       </c>
-      <c r="D292" s="61"/>
+      <c r="D292" s="64"/>
     </row>
     <row r="293" spans="2:4">
       <c r="B293" s="40" t="s">
@@ -15728,7 +15728,7 @@
       <c r="C293" s="40" t="s">
         <v>1049</v>
       </c>
-      <c r="D293" s="61"/>
+      <c r="D293" s="64"/>
     </row>
     <row r="294" spans="2:4">
       <c r="B294" s="40" t="s">
@@ -15737,7 +15737,7 @@
       <c r="C294" s="40" t="s">
         <v>1051</v>
       </c>
-      <c r="D294" s="61"/>
+      <c r="D294" s="64"/>
     </row>
     <row r="295" spans="2:4">
       <c r="B295" s="40" t="s">
@@ -15746,7 +15746,7 @@
       <c r="C295" s="40" t="s">
         <v>1053</v>
       </c>
-      <c r="D295" s="61"/>
+      <c r="D295" s="64"/>
     </row>
     <row r="296" spans="2:4">
       <c r="B296" s="40" t="s">
@@ -15755,7 +15755,7 @@
       <c r="C296" s="40" t="s">
         <v>1055</v>
       </c>
-      <c r="D296" s="61"/>
+      <c r="D296" s="64"/>
     </row>
     <row r="297" spans="2:4">
       <c r="B297" s="40" t="s">
@@ -15764,7 +15764,7 @@
       <c r="C297" s="40" t="s">
         <v>1056</v>
       </c>
-      <c r="D297" s="61"/>
+      <c r="D297" s="64"/>
     </row>
     <row r="298" spans="2:4" ht="30">
       <c r="B298" s="40" t="s">
@@ -15773,7 +15773,7 @@
       <c r="C298" s="40" t="s">
         <v>1057</v>
       </c>
-      <c r="D298" s="61"/>
+      <c r="D298" s="64"/>
     </row>
     <row r="299" spans="2:4">
       <c r="B299" s="40" t="s">
@@ -15782,7 +15782,7 @@
       <c r="C299" s="40" t="s">
         <v>1058</v>
       </c>
-      <c r="D299" s="61"/>
+      <c r="D299" s="64"/>
     </row>
     <row r="300" spans="2:4">
       <c r="B300" s="40" t="s">
@@ -15791,7 +15791,7 @@
       <c r="C300" s="40" t="s">
         <v>1060</v>
       </c>
-      <c r="D300" s="61"/>
+      <c r="D300" s="64"/>
     </row>
     <row r="301" spans="2:4" ht="30">
       <c r="B301" s="40" t="s">
@@ -15800,7 +15800,7 @@
       <c r="C301" s="40" t="s">
         <v>1061</v>
       </c>
-      <c r="D301" s="61"/>
+      <c r="D301" s="64"/>
     </row>
     <row r="302" spans="2:4">
       <c r="B302" s="40" t="s">
@@ -15809,7 +15809,7 @@
       <c r="C302" s="40" t="s">
         <v>1063</v>
       </c>
-      <c r="D302" s="61"/>
+      <c r="D302" s="64"/>
     </row>
     <row r="303" spans="2:4">
       <c r="B303" s="40" t="s">
@@ -15818,7 +15818,7 @@
       <c r="C303" s="40" t="s">
         <v>1065</v>
       </c>
-      <c r="D303" s="61"/>
+      <c r="D303" s="64"/>
     </row>
     <row r="304" spans="2:4">
       <c r="B304" s="40" t="s">
@@ -15827,7 +15827,7 @@
       <c r="C304" s="40" t="s">
         <v>1066</v>
       </c>
-      <c r="D304" s="61"/>
+      <c r="D304" s="64"/>
     </row>
     <row r="305" spans="2:4" ht="30">
       <c r="B305" s="40" t="s">
@@ -15836,7 +15836,7 @@
       <c r="C305" s="40" t="s">
         <v>1068</v>
       </c>
-      <c r="D305" s="61"/>
+      <c r="D305" s="64"/>
     </row>
     <row r="306" spans="2:4">
       <c r="B306" s="40" t="s">
@@ -15845,7 +15845,7 @@
       <c r="C306" s="40" t="s">
         <v>1070</v>
       </c>
-      <c r="D306" s="61"/>
+      <c r="D306" s="64"/>
     </row>
     <row r="307" spans="2:4">
       <c r="B307" s="40" t="s">
@@ -15854,7 +15854,7 @@
       <c r="C307" s="40" t="s">
         <v>1072</v>
       </c>
-      <c r="D307" s="61"/>
+      <c r="D307" s="64"/>
     </row>
     <row r="308" spans="2:4" ht="30">
       <c r="B308" s="40" t="s">
@@ -15863,7 +15863,7 @@
       <c r="C308" s="40" t="s">
         <v>1073</v>
       </c>
-      <c r="D308" s="61"/>
+      <c r="D308" s="64"/>
     </row>
     <row r="309" spans="2:4" ht="30">
       <c r="B309" s="40" t="s">
@@ -15872,7 +15872,7 @@
       <c r="C309" s="40" t="s">
         <v>1074</v>
       </c>
-      <c r="D309" s="61"/>
+      <c r="D309" s="64"/>
     </row>
     <row r="310" spans="2:4">
       <c r="B310" s="40" t="s">
@@ -15881,7 +15881,7 @@
       <c r="C310" s="40" t="s">
         <v>1075</v>
       </c>
-      <c r="D310" s="61"/>
+      <c r="D310" s="64"/>
     </row>
     <row r="311" spans="2:4" ht="30">
       <c r="B311" s="40" t="s">
@@ -15890,7 +15890,7 @@
       <c r="C311" s="40" t="s">
         <v>1076</v>
       </c>
-      <c r="D311" s="61"/>
+      <c r="D311" s="64"/>
     </row>
     <row r="312" spans="2:4">
       <c r="B312" s="40" t="s">
@@ -15899,7 +15899,7 @@
       <c r="C312" s="40" t="s">
         <v>1077</v>
       </c>
-      <c r="D312" s="61"/>
+      <c r="D312" s="64"/>
     </row>
     <row r="313" spans="2:4">
       <c r="B313" s="40" t="s">
@@ -15908,7 +15908,7 @@
       <c r="C313" s="40" t="s">
         <v>1079</v>
       </c>
-      <c r="D313" s="61"/>
+      <c r="D313" s="64"/>
     </row>
     <row r="314" spans="2:4">
       <c r="B314" s="40" t="s">
@@ -15917,7 +15917,7 @@
       <c r="C314" s="40" t="s">
         <v>1081</v>
       </c>
-      <c r="D314" s="61"/>
+      <c r="D314" s="64"/>
     </row>
     <row r="315" spans="2:4">
       <c r="B315" s="40" t="s">
@@ -15926,10 +15926,88 @@
       <c r="C315" s="40" t="s">
         <v>1083</v>
       </c>
-      <c r="D315" s="61"/>
+      <c r="D315" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="102">
+    <mergeCell ref="E277:F277"/>
+    <mergeCell ref="E278:F278"/>
+    <mergeCell ref="E271:F271"/>
+    <mergeCell ref="E272:F272"/>
+    <mergeCell ref="E273:F273"/>
+    <mergeCell ref="E274:F274"/>
+    <mergeCell ref="E275:F275"/>
+    <mergeCell ref="E276:F276"/>
+    <mergeCell ref="E265:F265"/>
+    <mergeCell ref="E266:F266"/>
+    <mergeCell ref="E267:F267"/>
+    <mergeCell ref="E268:F268"/>
+    <mergeCell ref="E269:F269"/>
+    <mergeCell ref="E270:F270"/>
+    <mergeCell ref="E259:F259"/>
+    <mergeCell ref="E260:F260"/>
+    <mergeCell ref="E261:F261"/>
+    <mergeCell ref="E262:F262"/>
+    <mergeCell ref="E263:F263"/>
+    <mergeCell ref="E264:F264"/>
+    <mergeCell ref="E253:F253"/>
+    <mergeCell ref="E254:F254"/>
+    <mergeCell ref="E255:F255"/>
+    <mergeCell ref="E256:F256"/>
+    <mergeCell ref="E257:F257"/>
+    <mergeCell ref="E258:F258"/>
+    <mergeCell ref="E247:F247"/>
+    <mergeCell ref="E248:F248"/>
+    <mergeCell ref="E249:F249"/>
+    <mergeCell ref="E250:F250"/>
+    <mergeCell ref="E251:F251"/>
+    <mergeCell ref="E252:F252"/>
+    <mergeCell ref="E241:F241"/>
+    <mergeCell ref="E242:F242"/>
+    <mergeCell ref="E243:F243"/>
+    <mergeCell ref="E244:F244"/>
+    <mergeCell ref="E245:F245"/>
+    <mergeCell ref="E246:F246"/>
+    <mergeCell ref="E235:F235"/>
+    <mergeCell ref="E236:F236"/>
+    <mergeCell ref="E237:F237"/>
+    <mergeCell ref="E238:F238"/>
+    <mergeCell ref="E239:F239"/>
+    <mergeCell ref="E240:F240"/>
+    <mergeCell ref="E229:F229"/>
+    <mergeCell ref="E230:F230"/>
+    <mergeCell ref="E231:F231"/>
+    <mergeCell ref="E232:F232"/>
+    <mergeCell ref="E233:F233"/>
+    <mergeCell ref="E234:F234"/>
+    <mergeCell ref="E225:F225"/>
+    <mergeCell ref="E226:F226"/>
+    <mergeCell ref="E227:F227"/>
+    <mergeCell ref="E228:F228"/>
+    <mergeCell ref="E217:F217"/>
+    <mergeCell ref="E218:F218"/>
+    <mergeCell ref="E219:F219"/>
+    <mergeCell ref="E220:F220"/>
+    <mergeCell ref="E221:F221"/>
+    <mergeCell ref="E222:F222"/>
+    <mergeCell ref="E216:F216"/>
+    <mergeCell ref="E205:F205"/>
+    <mergeCell ref="E206:F206"/>
+    <mergeCell ref="E207:F207"/>
+    <mergeCell ref="E208:F208"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="E210:F210"/>
+    <mergeCell ref="E223:F223"/>
+    <mergeCell ref="E224:F224"/>
+    <mergeCell ref="E195:F195"/>
+    <mergeCell ref="E196:F196"/>
+    <mergeCell ref="E197:F197"/>
+    <mergeCell ref="E198:F198"/>
+    <mergeCell ref="E211:F211"/>
+    <mergeCell ref="E212:F212"/>
+    <mergeCell ref="E213:F213"/>
+    <mergeCell ref="E214:F214"/>
+    <mergeCell ref="E215:F215"/>
     <mergeCell ref="E187:F187"/>
     <mergeCell ref="E188:F188"/>
     <mergeCell ref="E189:F189"/>
@@ -15954,84 +16032,6 @@
     <mergeCell ref="E204:F204"/>
     <mergeCell ref="E193:F193"/>
     <mergeCell ref="E194:F194"/>
-    <mergeCell ref="E195:F195"/>
-    <mergeCell ref="E196:F196"/>
-    <mergeCell ref="E197:F197"/>
-    <mergeCell ref="E198:F198"/>
-    <mergeCell ref="E211:F211"/>
-    <mergeCell ref="E212:F212"/>
-    <mergeCell ref="E213:F213"/>
-    <mergeCell ref="E214:F214"/>
-    <mergeCell ref="E215:F215"/>
-    <mergeCell ref="E216:F216"/>
-    <mergeCell ref="E205:F205"/>
-    <mergeCell ref="E206:F206"/>
-    <mergeCell ref="E207:F207"/>
-    <mergeCell ref="E208:F208"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="E210:F210"/>
-    <mergeCell ref="E223:F223"/>
-    <mergeCell ref="E224:F224"/>
-    <mergeCell ref="E225:F225"/>
-    <mergeCell ref="E226:F226"/>
-    <mergeCell ref="E227:F227"/>
-    <mergeCell ref="E228:F228"/>
-    <mergeCell ref="E217:F217"/>
-    <mergeCell ref="E218:F218"/>
-    <mergeCell ref="E219:F219"/>
-    <mergeCell ref="E220:F220"/>
-    <mergeCell ref="E221:F221"/>
-    <mergeCell ref="E222:F222"/>
-    <mergeCell ref="E235:F235"/>
-    <mergeCell ref="E236:F236"/>
-    <mergeCell ref="E237:F237"/>
-    <mergeCell ref="E238:F238"/>
-    <mergeCell ref="E239:F239"/>
-    <mergeCell ref="E240:F240"/>
-    <mergeCell ref="E229:F229"/>
-    <mergeCell ref="E230:F230"/>
-    <mergeCell ref="E231:F231"/>
-    <mergeCell ref="E232:F232"/>
-    <mergeCell ref="E233:F233"/>
-    <mergeCell ref="E234:F234"/>
-    <mergeCell ref="E247:F247"/>
-    <mergeCell ref="E248:F248"/>
-    <mergeCell ref="E249:F249"/>
-    <mergeCell ref="E250:F250"/>
-    <mergeCell ref="E251:F251"/>
-    <mergeCell ref="E252:F252"/>
-    <mergeCell ref="E241:F241"/>
-    <mergeCell ref="E242:F242"/>
-    <mergeCell ref="E243:F243"/>
-    <mergeCell ref="E244:F244"/>
-    <mergeCell ref="E245:F245"/>
-    <mergeCell ref="E246:F246"/>
-    <mergeCell ref="E259:F259"/>
-    <mergeCell ref="E260:F260"/>
-    <mergeCell ref="E261:F261"/>
-    <mergeCell ref="E262:F262"/>
-    <mergeCell ref="E263:F263"/>
-    <mergeCell ref="E264:F264"/>
-    <mergeCell ref="E253:F253"/>
-    <mergeCell ref="E254:F254"/>
-    <mergeCell ref="E255:F255"/>
-    <mergeCell ref="E256:F256"/>
-    <mergeCell ref="E257:F257"/>
-    <mergeCell ref="E258:F258"/>
-    <mergeCell ref="E277:F277"/>
-    <mergeCell ref="E278:F278"/>
-    <mergeCell ref="E271:F271"/>
-    <mergeCell ref="E272:F272"/>
-    <mergeCell ref="E273:F273"/>
-    <mergeCell ref="E274:F274"/>
-    <mergeCell ref="E275:F275"/>
-    <mergeCell ref="E276:F276"/>
-    <mergeCell ref="E265:F265"/>
-    <mergeCell ref="E266:F266"/>
-    <mergeCell ref="E267:F267"/>
-    <mergeCell ref="E268:F268"/>
-    <mergeCell ref="E269:F269"/>
-    <mergeCell ref="E270:F270"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C35" r:id="rId1" location="cfa" display="http://www.xe.com/iso4217.php - cfa"/>

</xml_diff>

<commit_message>
EPBDS-1682 EPBDS regex constraint for datatypePackage property.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -13,12 +13,12 @@
     <sheet name="Runtime Scope" sheetId="3" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="705">
   <si>
     <t>name</t>
   </si>
@@ -2157,12 +2157,15 @@
   <si>
     <t>Yemen</t>
   </si>
+  <si>
+    <t>regexp:([a-z_]{1}[a-z0-9_]*(\\.[a-z_]{1}[a-z0-9_]*)*)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2596,29 +2599,29 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2661,17 +2664,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2709,7 +2717,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2743,6 +2751,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2777,9 +2786,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2952,69 +2962,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="74.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-    </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+    </row>
+    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1">
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="38" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="37"/>
@@ -3025,67 +3035,67 @@
       <c r="I5" s="37"/>
       <c r="J5" s="37"/>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-    </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+    </row>
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1">
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+    </row>
+    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1">
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-    </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1">
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+    </row>
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
@@ -3100,11 +3110,11 @@
       <c r="I10" s="37"/>
       <c r="J10" s="37"/>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1">
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="38" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="37"/>
@@ -3115,11 +3125,11 @@
       <c r="I11" s="37"/>
       <c r="J11" s="37"/>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="32" t="s">
         <v>119</v>
       </c>
       <c r="D12" s="37"/>
@@ -3130,11 +3140,11 @@
       <c r="I12" s="37"/>
       <c r="J12" s="37"/>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1">
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D13" s="37"/>
@@ -3145,36 +3155,42 @@
       <c r="I13" s="37"/>
       <c r="J13" s="37"/>
     </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1">
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1">
-      <c r="B15" s="39" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3183,28 +3199,22 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
@@ -3228,65 +3238,65 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
+    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-    </row>
-    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+    </row>
+    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-    </row>
-    <row r="3" spans="2:19" ht="57.75" customHeight="1">
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+    </row>
+    <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-    </row>
-    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="37"/>
@@ -3300,79 +3310,79 @@
       <c r="L4" s="37"/>
       <c r="M4" s="37"/>
     </row>
-    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
+    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-    </row>
-    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+    </row>
+    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-    </row>
-    <row r="7" spans="2:19" ht="42.75" customHeight="1">
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+    </row>
+    <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-    </row>
-    <row r="8" spans="2:19" ht="33" customHeight="1">
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+    </row>
+    <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-    </row>
-    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+    </row>
+    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
@@ -3390,7 +3400,7 @@
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
     </row>
-    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3402,7 +3412,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="2:19" ht="15" customHeight="1">
+    <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="40" t="s">
         <v>28</v>
       </c>
@@ -3424,7 +3434,7 @@
       <c r="R11" s="40"/>
       <c r="S11" s="40"/>
     </row>
-    <row r="12" spans="2:19" ht="30">
+    <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
@@ -3480,7 +3490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:19" ht="60">
+    <row r="13" spans="2:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>29</v>
       </c>
@@ -3536,7 +3546,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:19">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>11</v>
       </c>
@@ -3580,7 +3590,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="105">
+    <row r="15" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
@@ -3624,7 +3634,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="2:19" s="4" customFormat="1">
+    <row r="16" spans="2:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>35</v>
       </c>
@@ -3668,7 +3678,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="30">
+    <row r="17" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>21</v>
       </c>
@@ -3712,7 +3722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="90">
+    <row r="18" spans="2:19" ht="90" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>316</v>
       </c>
@@ -3760,7 +3770,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="75">
+    <row r="19" spans="2:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>315</v>
       </c>
@@ -3808,7 +3818,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="20" spans="2:19">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
         <v>22</v>
       </c>
@@ -3856,7 +3866,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:19">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>23</v>
       </c>
@@ -3906,7 +3916,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:19">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
         <v>24</v>
       </c>
@@ -3954,7 +3964,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:19">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>25</v>
       </c>
@@ -4004,7 +4014,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:19" ht="45">
+    <row r="24" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>26</v>
       </c>
@@ -4048,7 +4058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="30">
+    <row r="25" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
         <v>45</v>
       </c>
@@ -4094,7 +4104,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="26" spans="2:19" ht="105">
+    <row r="26" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
         <v>49</v>
       </c>
@@ -4140,7 +4150,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="105">
+    <row r="27" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
         <v>54</v>
       </c>
@@ -4186,7 +4196,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="105">
+    <row r="28" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
         <v>466</v>
       </c>
@@ -4232,7 +4242,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="30">
+    <row r="29" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
         <v>56</v>
       </c>
@@ -4278,7 +4288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="30">
+    <row r="30" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
         <v>57</v>
       </c>
@@ -4324,7 +4334,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="105">
+    <row r="31" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
         <v>467</v>
       </c>
@@ -4370,7 +4380,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="2:19" ht="105">
+    <row r="32" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
         <v>53</v>
       </c>
@@ -4416,7 +4426,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="2:19" ht="78.75" customHeight="1">
+    <row r="33" spans="2:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>83</v>
       </c>
@@ -4456,7 +4466,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="75">
+    <row r="34" spans="2:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
         <v>85</v>
       </c>
@@ -4498,7 +4508,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="2:19" ht="45">
+    <row r="35" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
         <v>90</v>
       </c>
@@ -4538,7 +4548,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="2:19" ht="30">
+    <row r="36" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="25" t="s">
         <v>126</v>
       </c>
@@ -4580,7 +4590,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="37" spans="2:19" ht="45">
+    <row r="37" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
         <v>468</v>
       </c>
@@ -4614,7 +4624,7 @@
         <v>471</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>129</v>
+        <v>704</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="25" t="s">
@@ -4624,7 +4634,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="38" spans="2:19" ht="30">
+    <row r="38" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
         <v>484</v>
       </c>
@@ -4662,7 +4672,7 @@
       </c>
       <c r="S38" s="25"/>
     </row>
-    <row r="39" spans="2:19">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" s="25" t="s">
         <v>485</v>
       </c>
@@ -4700,7 +4710,7 @@
       </c>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="2:19">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B40" s="25" t="s">
         <v>486</v>
       </c>
@@ -4738,7 +4748,7 @@
       </c>
       <c r="S40" s="25"/>
     </row>
-    <row r="42" spans="2:19" ht="45">
+    <row r="42" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
         <v>91</v>
       </c>
@@ -4795,16 +4805,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
         <v>109</v>
       </c>
@@ -4813,7 +4823,7 @@
       <c r="E5" s="46"/>
       <c r="F5" s="47"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="41" t="s">
         <v>110</v>
       </c>
@@ -4824,7 +4834,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="41"/>
       <c r="C7" s="24" t="s">
         <v>113</v>
@@ -4833,7 +4843,7 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="41"/>
       <c r="C8" s="24" t="s">
         <v>134</v>
@@ -4842,7 +4852,7 @@
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="41"/>
       <c r="C9" s="24" t="s">
         <v>135</v>
@@ -4851,7 +4861,7 @@
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="41"/>
       <c r="C10" s="42" t="s">
         <v>158</v>
@@ -4871,14 +4881,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
@@ -4886,7 +4896,7 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" customHeight="1">
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="48" t="s">
         <v>111</v>
       </c>
@@ -4894,7 +4904,7 @@
       <c r="D2" s="49"/>
       <c r="E2" s="50"/>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -4908,7 +4918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
@@ -4922,7 +4932,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>112</v>
       </c>
@@ -4934,7 +4944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>50</v>
       </c>
@@ -4946,7 +4956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>125</v>
       </c>
@@ -4960,7 +4970,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>60</v>
       </c>
@@ -4974,7 +4984,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>123</v>
       </c>
@@ -4988,7 +4998,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>64</v>
       </c>
@@ -5012,14 +5022,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K216"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
@@ -5030,7 +5040,7 @@
     <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
         <v>130</v>
       </c>
@@ -5044,7 +5054,7 @@
       </c>
       <c r="K3" s="52"/>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -5064,7 +5074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>131</v>
       </c>
@@ -5084,7 +5094,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>203</v>
       </c>
@@ -5104,7 +5114,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>498</v>
       </c>
@@ -5124,7 +5134,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>168</v>
       </c>
@@ -5144,7 +5154,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>163</v>
       </c>
@@ -5164,7 +5174,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>499</v>
       </c>
@@ -5178,7 +5188,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>500</v>
       </c>
@@ -5192,7 +5202,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>452</v>
       </c>
@@ -5206,7 +5216,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>501</v>
       </c>
@@ -5220,7 +5230,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>502</v>
       </c>
@@ -5238,7 +5248,7 @@
       </c>
       <c r="K14" s="52"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>503</v>
       </c>
@@ -5258,7 +5268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>167</v>
       </c>
@@ -5278,7 +5288,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>504</v>
       </c>
@@ -5298,7 +5308,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>166</v>
       </c>
@@ -5318,7 +5328,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>505</v>
       </c>
@@ -5338,7 +5348,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>449</v>
       </c>
@@ -5358,7 +5368,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>211</v>
       </c>
@@ -5378,7 +5388,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>506</v>
       </c>
@@ -5392,7 +5402,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>507</v>
       </c>
@@ -5406,7 +5416,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>508</v>
       </c>
@@ -5420,7 +5430,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>509</v>
       </c>
@@ -5434,7 +5444,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>510</v>
       </c>
@@ -5448,7 +5458,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>511</v>
       </c>
@@ -5462,7 +5472,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>512</v>
       </c>
@@ -5476,7 +5486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>513</v>
       </c>
@@ -5490,7 +5500,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>514</v>
       </c>
@@ -5504,7 +5514,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>515</v>
       </c>
@@ -5518,7 +5528,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>516</v>
       </c>
@@ -5532,7 +5542,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>170</v>
       </c>
@@ -5546,7 +5556,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>171</v>
       </c>
@@ -5560,7 +5570,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>517</v>
       </c>
@@ -5574,7 +5584,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>518</v>
       </c>
@@ -5588,7 +5598,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="14.25" customHeight="1">
+    <row r="37" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>519</v>
       </c>
@@ -5602,7 +5612,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>520</v>
       </c>
@@ -5616,7 +5626,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>451</v>
       </c>
@@ -5630,7 +5640,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>521</v>
       </c>
@@ -5644,7 +5654,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>172</v>
       </c>
@@ -5658,7 +5668,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>222</v>
       </c>
@@ -5672,7 +5682,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>522</v>
       </c>
@@ -5686,7 +5696,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="44" spans="2:7">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>523</v>
       </c>
@@ -5700,7 +5710,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="2:7">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>224</v>
       </c>
@@ -5714,7 +5724,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="2:7">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>174</v>
       </c>
@@ -5728,7 +5738,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>321</v>
       </c>
@@ -5742,7 +5752,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>524</v>
       </c>
@@ -5756,7 +5766,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>525</v>
       </c>
@@ -5770,7 +5780,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>453</v>
       </c>
@@ -5784,7 +5794,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>526</v>
       </c>
@@ -5798,7 +5808,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>454</v>
       </c>
@@ -5812,7 +5822,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>527</v>
       </c>
@@ -5826,7 +5836,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>528</v>
       </c>
@@ -5840,7 +5850,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>529</v>
       </c>
@@ -5854,7 +5864,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="8" t="s">
         <v>249</v>
       </c>
@@ -5868,7 +5878,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="8" t="s">
         <v>164</v>
       </c>
@@ -5882,7 +5892,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="8" t="s">
         <v>239</v>
       </c>
@@ -5890,7 +5900,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="8" t="s">
         <v>530</v>
       </c>
@@ -5898,7 +5908,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="8" t="s">
         <v>165</v>
       </c>
@@ -5906,7 +5916,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="61" spans="2:7">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="8" t="s">
         <v>531</v>
       </c>
@@ -5914,7 +5924,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="8" t="s">
         <v>532</v>
       </c>
@@ -5922,7 +5932,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="8" t="s">
         <v>533</v>
       </c>
@@ -5930,7 +5940,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="64" spans="2:7">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="s">
         <v>273</v>
       </c>
@@ -5938,7 +5948,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="65" spans="2:3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="s">
         <v>534</v>
       </c>
@@ -5946,7 +5956,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="66" spans="2:3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="s">
         <v>535</v>
       </c>
@@ -5954,7 +5964,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="67" spans="2:3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>536</v>
       </c>
@@ -5962,7 +5972,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>537</v>
       </c>
@@ -5970,7 +5980,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="s">
         <v>538</v>
       </c>
@@ -5978,7 +5988,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="70" spans="2:3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
         <v>481</v>
       </c>
@@ -5986,7 +5996,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="71" spans="2:3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="s">
         <v>539</v>
       </c>
@@ -5994,7 +6004,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="72" spans="2:3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
         <v>540</v>
       </c>
@@ -6002,7 +6012,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="73" spans="2:3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="s">
         <v>133</v>
       </c>
@@ -6010,7 +6020,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="74" spans="2:3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="8" t="s">
         <v>541</v>
       </c>
@@ -6018,7 +6028,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="75" spans="2:3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="8" t="s">
         <v>542</v>
       </c>
@@ -6026,7 +6036,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="2:3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="8" t="s">
         <v>543</v>
       </c>
@@ -6034,7 +6044,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="77" spans="2:3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="8" t="s">
         <v>544</v>
       </c>
@@ -6042,7 +6052,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="78" spans="2:3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
         <v>545</v>
       </c>
@@ -6050,7 +6060,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="79" spans="2:3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="s">
         <v>175</v>
       </c>
@@ -6058,7 +6068,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="80" spans="2:3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>546</v>
       </c>
@@ -6066,7 +6076,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>279</v>
       </c>
@@ -6074,7 +6084,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="82" spans="2:3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="s">
         <v>304</v>
       </c>
@@ -6082,7 +6092,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="83" spans="2:3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="8" t="s">
         <v>173</v>
       </c>
@@ -6090,7 +6100,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="2:3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>491</v>
       </c>
@@ -6098,7 +6108,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="2:3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="s">
         <v>448</v>
       </c>
@@ -6106,7 +6116,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="86" spans="2:3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>492</v>
       </c>
@@ -6114,7 +6124,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="8" t="s">
         <v>281</v>
       </c>
@@ -6122,7 +6132,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="88" spans="2:3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="s">
         <v>450</v>
       </c>
@@ -6130,7 +6140,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="89" spans="2:3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
         <v>320</v>
       </c>
@@ -6138,7 +6148,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="90" spans="2:3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>493</v>
       </c>
@@ -6146,7 +6156,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="91" spans="2:3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
         <v>169</v>
       </c>
@@ -6154,7 +6164,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="92" spans="2:3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="8" t="s">
         <v>69</v>
       </c>
@@ -6162,7 +6172,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="s">
         <v>494</v>
       </c>
@@ -6170,7 +6180,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="8" t="s">
         <v>495</v>
       </c>
@@ -6178,7 +6188,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="95" spans="2:3">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="s">
         <v>496</v>
       </c>
@@ -6186,7 +6196,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="96" spans="2:3">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="8" t="s">
         <v>497</v>
       </c>
@@ -6194,13 +6204,13 @@
         <v>703</v>
       </c>
     </row>
-    <row r="100" spans="2:3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="51" t="s">
         <v>187</v>
       </c>
       <c r="C100" s="52"/>
     </row>
-    <row r="101" spans="2:3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
         <v>0</v>
       </c>
@@ -6208,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="2:3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
         <v>131</v>
       </c>
@@ -6216,7 +6226,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="2:3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="8" t="s">
         <v>606</v>
       </c>
@@ -6224,7 +6234,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="104" spans="2:3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="8" t="s">
         <v>575</v>
       </c>
@@ -6232,7 +6242,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="105" spans="2:3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="8" t="s">
         <v>576</v>
       </c>
@@ -6240,7 +6250,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="106" spans="2:3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="8" t="s">
         <v>578</v>
       </c>
@@ -6248,7 +6258,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="107" spans="2:3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="8" t="s">
         <v>579</v>
       </c>
@@ -6256,7 +6266,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="108" spans="2:3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="8" t="s">
         <v>196</v>
       </c>
@@ -6264,7 +6274,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="2:3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="8" t="s">
         <v>417</v>
       </c>
@@ -6272,7 +6282,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="110" spans="2:3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="8" t="s">
         <v>580</v>
       </c>
@@ -6280,7 +6290,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="111" spans="2:3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="8" t="s">
         <v>581</v>
       </c>
@@ -6288,7 +6298,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="112" spans="2:3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="8" t="s">
         <v>600</v>
       </c>
@@ -6296,7 +6306,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="113" spans="2:3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="8" t="s">
         <v>583</v>
       </c>
@@ -6304,7 +6314,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="114" spans="2:3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="8" t="s">
         <v>584</v>
       </c>
@@ -6312,7 +6322,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="115" spans="2:3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="8" t="s">
         <v>585</v>
       </c>
@@ -6320,7 +6330,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="2:3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="8" t="s">
         <v>198</v>
       </c>
@@ -6328,7 +6338,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="2:3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="8" t="s">
         <v>582</v>
       </c>
@@ -6336,7 +6346,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="118" spans="2:3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="8" t="s">
         <v>587</v>
       </c>
@@ -6344,7 +6354,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="119" spans="2:3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="8" t="s">
         <v>589</v>
       </c>
@@ -6352,7 +6362,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="120" spans="2:3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="8" t="s">
         <v>590</v>
       </c>
@@ -6360,7 +6370,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="121" spans="2:3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="8" t="s">
         <v>591</v>
       </c>
@@ -6368,7 +6378,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="122" spans="2:3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="8" t="s">
         <v>586</v>
       </c>
@@ -6376,7 +6386,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="123" spans="2:3">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="8" t="s">
         <v>194</v>
       </c>
@@ -6384,7 +6394,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="2:3">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="8" t="s">
         <v>593</v>
       </c>
@@ -6392,7 +6402,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="125" spans="2:3">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="8" t="s">
         <v>594</v>
       </c>
@@ -6400,7 +6410,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="126" spans="2:3">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="8" t="s">
         <v>596</v>
       </c>
@@ -6408,7 +6418,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="127" spans="2:3">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="8" t="s">
         <v>597</v>
       </c>
@@ -6416,7 +6426,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="128" spans="2:3">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="8" t="s">
         <v>599</v>
       </c>
@@ -6424,7 +6434,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="129" spans="2:3">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="8" t="s">
         <v>598</v>
       </c>
@@ -6432,7 +6442,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="130" spans="2:3">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="8" t="s">
         <v>601</v>
       </c>
@@ -6440,7 +6450,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="131" spans="2:3">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="8" t="s">
         <v>602</v>
       </c>
@@ -6448,7 +6458,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="132" spans="2:3">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="8" t="s">
         <v>189</v>
       </c>
@@ -6456,7 +6466,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="133" spans="2:3">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="8" t="s">
         <v>603</v>
       </c>
@@ -6464,7 +6474,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="134" spans="2:3">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="8" t="s">
         <v>191</v>
       </c>
@@ -6472,7 +6482,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:3">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="8" t="s">
         <v>607</v>
       </c>
@@ -6480,7 +6490,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="136" spans="2:3">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="8" t="s">
         <v>604</v>
       </c>
@@ -6488,7 +6498,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="137" spans="2:3">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="8" t="s">
         <v>605</v>
       </c>
@@ -6496,7 +6506,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="138" spans="2:3">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="8" t="s">
         <v>608</v>
       </c>
@@ -6504,7 +6514,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="139" spans="2:3">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="8" t="s">
         <v>609</v>
       </c>
@@ -6512,7 +6522,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="140" spans="2:3">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="8" t="s">
         <v>610</v>
       </c>
@@ -6520,7 +6530,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="141" spans="2:3">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="8" t="s">
         <v>611</v>
       </c>
@@ -6528,13 +6538,13 @@
         <v>574</v>
       </c>
     </row>
-    <row r="144" spans="2:3">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="51" t="s">
         <v>613</v>
       </c>
       <c r="C144" s="52"/>
     </row>
-    <row r="145" spans="2:3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">
         <v>0</v>
       </c>
@@ -6542,7 +6552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="2:3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="6" t="s">
         <v>131</v>
       </c>
@@ -6550,7 +6560,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="2:3">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="8" t="s">
         <v>322</v>
       </c>
@@ -6558,7 +6568,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="148" spans="2:3">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="8" t="s">
         <v>324</v>
       </c>
@@ -6566,7 +6576,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="149" spans="2:3">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="8" t="s">
         <v>180</v>
       </c>
@@ -6574,7 +6584,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="150" spans="2:3">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="8" t="s">
         <v>176</v>
       </c>
@@ -6582,7 +6592,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="151" spans="2:3">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="8" t="s">
         <v>328</v>
       </c>
@@ -6590,7 +6600,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="152" spans="2:3">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="8" t="s">
         <v>162</v>
       </c>
@@ -6598,7 +6608,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="153" spans="2:3">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="8" t="s">
         <v>331</v>
       </c>
@@ -6606,7 +6616,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="154" spans="2:3">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="8" t="s">
         <v>333</v>
       </c>
@@ -6614,7 +6624,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="155" spans="2:3">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="8" t="s">
         <v>179</v>
       </c>
@@ -6622,7 +6632,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="156" spans="2:3">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="8" t="s">
         <v>186</v>
       </c>
@@ -6630,7 +6640,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="157" spans="2:3">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="8" t="s">
         <v>338</v>
       </c>
@@ -6638,7 +6648,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="158" spans="2:3">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="8" t="s">
         <v>182</v>
       </c>
@@ -6646,7 +6656,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="159" spans="2:3">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="8" t="s">
         <v>341</v>
       </c>
@@ -6654,7 +6664,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="160" spans="2:3">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="8" t="s">
         <v>343</v>
       </c>
@@ -6662,7 +6672,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="161" spans="2:3">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="8" t="s">
         <v>345</v>
       </c>
@@ -6670,7 +6680,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="162" spans="2:3">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="8" t="s">
         <v>347</v>
       </c>
@@ -6678,7 +6688,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="163" spans="2:3">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="8" t="s">
         <v>349</v>
       </c>
@@ -6686,7 +6696,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="164" spans="2:3">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="8" t="s">
         <v>351</v>
       </c>
@@ -6694,7 +6704,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="165" spans="2:3">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="8" t="s">
         <v>354</v>
       </c>
@@ -6702,7 +6712,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="166" spans="2:3">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="8" t="s">
         <v>181</v>
       </c>
@@ -6710,7 +6720,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="167" spans="2:3">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="8" t="s">
         <v>356</v>
       </c>
@@ -6718,7 +6728,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="168" spans="2:3">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="8" t="s">
         <v>358</v>
       </c>
@@ -6726,7 +6736,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="169" spans="2:3">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="8" t="s">
         <v>360</v>
       </c>
@@ -6734,7 +6744,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="170" spans="2:3">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="8" t="s">
         <v>362</v>
       </c>
@@ -6742,7 +6752,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="171" spans="2:3">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="8" t="s">
         <v>364</v>
       </c>
@@ -6750,7 +6760,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="172" spans="2:3">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="8" t="s">
         <v>183</v>
       </c>
@@ -6758,7 +6768,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="173" spans="2:3">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="8" t="s">
         <v>353</v>
       </c>
@@ -6766,7 +6776,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="174" spans="2:3">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="8" t="s">
         <v>368</v>
       </c>
@@ -6774,7 +6784,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="175" spans="2:3">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="8" t="s">
         <v>370</v>
       </c>
@@ -6782,7 +6792,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="176" spans="2:3">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="8" t="s">
         <v>372</v>
       </c>
@@ -6790,7 +6800,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="177" spans="2:3">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="8" t="s">
         <v>374</v>
       </c>
@@ -6798,7 +6808,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="178" spans="2:3">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="8" t="s">
         <v>376</v>
       </c>
@@ -6806,7 +6816,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="179" spans="2:3">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="8" t="s">
         <v>378</v>
       </c>
@@ -6814,7 +6824,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="180" spans="2:3">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="8" t="s">
         <v>380</v>
       </c>
@@ -6822,7 +6832,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="181" spans="2:3">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="8" t="s">
         <v>383</v>
       </c>
@@ -6830,7 +6840,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="182" spans="2:3">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="8" t="s">
         <v>385</v>
       </c>
@@ -6838,7 +6848,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="183" spans="2:3">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="8" t="s">
         <v>387</v>
       </c>
@@ -6846,7 +6856,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="184" spans="2:3">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="8" t="s">
         <v>177</v>
       </c>
@@ -6854,7 +6864,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="185" spans="2:3">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="8" t="s">
         <v>390</v>
       </c>
@@ -6862,7 +6872,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="186" spans="2:3">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="8" t="s">
         <v>178</v>
       </c>
@@ -6870,7 +6880,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="187" spans="2:3">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="8" t="s">
         <v>393</v>
       </c>
@@ -6878,7 +6888,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="188" spans="2:3">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="8" t="s">
         <v>335</v>
       </c>
@@ -6886,7 +6896,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="189" spans="2:3">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="8" t="s">
         <v>396</v>
       </c>
@@ -6894,7 +6904,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="190" spans="2:3">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="8" t="s">
         <v>398</v>
       </c>
@@ -6902,7 +6912,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="191" spans="2:3">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="8" t="s">
         <v>400</v>
       </c>
@@ -6910,7 +6920,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="192" spans="2:3">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="8" t="s">
         <v>402</v>
       </c>
@@ -6918,7 +6928,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="193" spans="2:3">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="8" t="s">
         <v>404</v>
       </c>
@@ -6926,7 +6936,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="194" spans="2:3">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="8" t="s">
         <v>406</v>
       </c>
@@ -6934,7 +6944,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="195" spans="2:3">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="8" t="s">
         <v>408</v>
       </c>
@@ -6942,7 +6952,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="196" spans="2:3">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="8" t="s">
         <v>410</v>
       </c>
@@ -6950,7 +6960,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="197" spans="2:3">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="8" t="s">
         <v>161</v>
       </c>
@@ -6958,7 +6968,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="198" spans="2:3">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="8" t="s">
         <v>413</v>
       </c>
@@ -6966,7 +6976,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="199" spans="2:3">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="8" t="s">
         <v>415</v>
       </c>
@@ -6974,7 +6984,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="200" spans="2:3">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="8" t="s">
         <v>418</v>
       </c>
@@ -6982,7 +6992,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="201" spans="2:3">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" s="8" t="s">
         <v>185</v>
       </c>
@@ -6990,7 +7000,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="202" spans="2:3">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="8" t="s">
         <v>421</v>
       </c>
@@ -6998,7 +7008,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="203" spans="2:3">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" s="8" t="s">
         <v>423</v>
       </c>
@@ -7006,7 +7016,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="204" spans="2:3">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="8" t="s">
         <v>382</v>
       </c>
@@ -7014,7 +7024,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="205" spans="2:3">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="8" t="s">
         <v>426</v>
       </c>
@@ -7022,7 +7032,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="206" spans="2:3">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="8" t="s">
         <v>428</v>
       </c>
@@ -7030,7 +7040,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="207" spans="2:3">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="8" t="s">
         <v>430</v>
       </c>
@@ -7038,7 +7048,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="208" spans="2:3">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="8" t="s">
         <v>432</v>
       </c>
@@ -7046,7 +7056,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="209" spans="2:3">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="8" t="s">
         <v>434</v>
       </c>
@@ -7054,7 +7064,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="210" spans="2:3">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" s="8" t="s">
         <v>436</v>
       </c>
@@ -7062,7 +7072,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="211" spans="2:3">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" s="8" t="s">
         <v>184</v>
       </c>
@@ -7070,7 +7080,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="212" spans="2:3">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" s="8" t="s">
         <v>68</v>
       </c>
@@ -7078,7 +7088,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="213" spans="2:3">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" s="8" t="s">
         <v>440</v>
       </c>
@@ -7086,7 +7096,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="214" spans="2:3">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" s="8" t="s">
         <v>442</v>
       </c>
@@ -7094,7 +7104,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="215" spans="2:3">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="8" t="s">
         <v>444</v>
       </c>
@@ -7102,7 +7112,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="216" spans="2:3">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" s="8" t="s">
         <v>446</v>
       </c>

</xml_diff>

<commit_message>
Start request date was added.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -13,12 +13,12 @@
     <sheet name="Runtime Scope" sheetId="3" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="712">
   <si>
     <t>name</t>
   </si>
@@ -2160,17 +2160,46 @@
   <si>
     <t>regexp:([a-z_]{1}[a-z0-9_]*(\\.[a-z_]{1}[a-z0-9_]*)*)</t>
   </si>
+  <si>
+    <t>requestDate</t>
+  </si>
+  <si>
+    <t>contains(currency)</t>
+  </si>
+  <si>
+    <t>Start Request Date</t>
+  </si>
+  <si>
+    <t>startRequestDate</t>
+  </si>
+  <si>
+    <t>Start request date</t>
+  </si>
+  <si>
+    <t>contains(lang)</t>
+  </si>
+  <si>
+    <t>max(le(requestDate))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2518,21 +2547,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2544,10 +2573,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2562,51 +2591,48 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2614,16 +2640,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2638,33 +2673,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2677,9 +2712,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2717,7 +2752,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2751,7 +2786,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2786,10 +2820,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2962,235 +2995,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="74.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="30" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="2:10" ht="30" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-    </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+    </row>
+    <row r="6" spans="2:10" ht="15" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-    </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+    </row>
+    <row r="7" spans="2:10" ht="30" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-    </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="2:10" ht="51.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-    </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="2:10" ht="30" customHeight="1">
       <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-    </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+    </row>
+    <row r="11" spans="2:10" ht="30" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-    </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+    </row>
+    <row r="13" spans="2:10" ht="30" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+    </row>
+    <row r="14" spans="2:10" ht="30" customHeight="1">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1">
+      <c r="B15" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3199,22 +3226,28 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
@@ -3238,169 +3271,169 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-    </row>
-    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-    </row>
-    <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+    </row>
+    <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-    </row>
-    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+    </row>
+    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-    </row>
-    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+    </row>
+    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-    </row>
-    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+    </row>
+    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-    </row>
-    <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+    </row>
+    <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-    </row>
-    <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+    </row>
+    <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-    </row>
-    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-    </row>
-    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3412,29 +3445,29 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+    <row r="11" spans="2:19" ht="15" customHeight="1">
+      <c r="B11" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="40"/>
-    </row>
-    <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+    </row>
+    <row r="12" spans="2:19" ht="30">
       <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
@@ -3490,7 +3523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" ht="60">
       <c r="B13" s="14" t="s">
         <v>29</v>
       </c>
@@ -3546,7 +3579,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19">
       <c r="B14" s="25" t="s">
         <v>11</v>
       </c>
@@ -3590,7 +3623,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" ht="105">
       <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
@@ -3634,7 +3667,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="2:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" s="4" customFormat="1">
       <c r="B16" s="25" t="s">
         <v>35</v>
       </c>
@@ -3678,7 +3711,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" ht="30">
       <c r="B17" s="25" t="s">
         <v>21</v>
       </c>
@@ -3722,7 +3755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" ht="90">
       <c r="B18" s="25" t="s">
         <v>316</v>
       </c>
@@ -3770,21 +3803,21 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" s="32" customFormat="1" ht="30">
       <c r="B19" s="25" t="s">
-        <v>315</v>
+        <v>707</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>3</v>
+        <v>708</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>474</v>
+        <v>711</v>
       </c>
       <c r="G19" s="25" t="s">
         <v>73</v>
@@ -3806,7 +3839,7 @@
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>118</v>
@@ -3815,40 +3848,38 @@
         <v>150</v>
       </c>
       <c r="S19" s="25" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" ht="75">
       <c r="B20" s="25" t="s">
-        <v>22</v>
+        <v>315</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>474</v>
+      </c>
       <c r="G20" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I20" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>142</v>
-      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
       <c r="L20" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="M20" s="25" t="s">
         <v>3</v>
@@ -3856,28 +3887,30 @@
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="25"/>
+        <v>137</v>
+      </c>
+      <c r="Q20" s="25" t="s">
+        <v>118</v>
+      </c>
       <c r="R20" s="25" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="S20" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19">
       <c r="B21" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="25" t="s">
@@ -3890,7 +3923,7 @@
         <v>73</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="K21" s="25" t="s">
         <v>142</v>
@@ -3906,28 +3939,26 @@
       <c r="P21" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q21" s="25" t="s">
-        <v>118</v>
-      </c>
+      <c r="Q21" s="25"/>
       <c r="R21" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S21" s="25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19">
       <c r="B22" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="25" t="s">
@@ -3937,13 +3968,13 @@
         <v>41</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L22" s="25" t="s">
         <v>73</v>
@@ -3956,26 +3987,28 @@
       <c r="P22" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q22" s="25"/>
+      <c r="Q22" s="25" t="s">
+        <v>118</v>
+      </c>
       <c r="R22" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S22" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19">
       <c r="B23" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>459</v>
+        <v>17</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="25" t="s">
@@ -3988,7 +4021,7 @@
         <v>3</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="K23" s="25" t="s">
         <v>143</v>
@@ -4004,43 +4037,45 @@
       <c r="P23" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q23" s="25" t="s">
-        <v>118</v>
-      </c>
+      <c r="Q23" s="25"/>
       <c r="R23" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S23" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19">
       <c r="B24" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>14</v>
+        <v>459</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="25" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
+      <c r="J24" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>143</v>
+      </c>
       <c r="L24" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="M24" s="25" t="s">
         <v>3</v>
@@ -4048,22 +4083,24 @@
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
       <c r="P24" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q24" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="Q24" s="25" t="s">
+        <v>118</v>
+      </c>
       <c r="R24" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S24" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" ht="45">
       <c r="B25" s="25" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>3</v>
@@ -4089,27 +4126,25 @@
       <c r="M25" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="N25" s="25" t="s">
-        <v>475</v>
-      </c>
+      <c r="N25" s="25"/>
       <c r="O25" s="25"/>
       <c r="P25" s="25" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S25" s="25" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="30">
       <c r="B26" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>3</v>
@@ -4117,17 +4152,15 @@
       <c r="E26" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="25" t="s">
-        <v>122</v>
-      </c>
+      <c r="F26" s="25"/>
       <c r="G26" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -4135,36 +4168,38 @@
         <v>3</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="N26" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="N26" s="25" t="s">
+        <v>475</v>
+      </c>
       <c r="O26" s="25"/>
       <c r="P26" s="25" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" ht="105">
       <c r="B27" s="25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>154</v>
+        <v>1</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>489</v>
+        <v>122</v>
       </c>
       <c r="G27" s="25" t="s">
         <v>73</v>
@@ -4186,22 +4221,22 @@
       <c r="N27" s="25"/>
       <c r="O27" s="25"/>
       <c r="P27" s="25" t="s">
-        <v>464</v>
+        <v>51</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S27" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" ht="105">
+      <c r="B28" s="25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="2:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
-        <v>466</v>
-      </c>
       <c r="C28" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>3</v>
@@ -4210,7 +4245,7 @@
         <v>154</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>155</v>
+        <v>489</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>73</v>
@@ -4219,7 +4254,7 @@
         <v>42</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
@@ -4232,22 +4267,22 @@
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25" t="s">
-        <v>156</v>
+        <v>464</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S28" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" ht="105">
       <c r="B29" s="25" t="s">
-        <v>56</v>
+        <v>466</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>3</v>
@@ -4255,12 +4290,14 @@
       <c r="E29" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="25" t="s">
+        <v>155</v>
+      </c>
       <c r="G29" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I29" s="25" t="s">
         <v>3</v>
@@ -4271,29 +4308,27 @@
         <v>3</v>
       </c>
       <c r="M29" s="25" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="N29" s="25"/>
-      <c r="O29" s="25" t="s">
-        <v>68</v>
-      </c>
+      <c r="O29" s="25"/>
       <c r="P29" s="25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S29" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" ht="105">
+      <c r="B30" s="25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="25" t="s">
-        <v>57</v>
-      </c>
       <c r="C30" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>3</v>
@@ -4301,12 +4336,14 @@
       <c r="E30" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="25"/>
+      <c r="F30" s="25" t="s">
+        <v>706</v>
+      </c>
       <c r="G30" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I30" s="25" t="s">
         <v>3</v>
@@ -4317,29 +4354,29 @@
         <v>3</v>
       </c>
       <c r="M30" s="25" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="N30" s="25"/>
       <c r="O30" s="25" t="s">
-        <v>583</v>
+        <v>68</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S30" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" ht="105">
+      <c r="B31" s="25" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="2:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
-        <v>467</v>
-      </c>
       <c r="C31" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>3</v>
@@ -4348,7 +4385,7 @@
         <v>154</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>317</v>
+        <v>710</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>73</v>
@@ -4357,7 +4394,7 @@
         <v>42</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
@@ -4368,24 +4405,26 @@
         <v>77</v>
       </c>
       <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
+      <c r="O31" s="25" t="s">
+        <v>583</v>
+      </c>
       <c r="P31" s="25" t="s">
-        <v>463</v>
+        <v>200</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" ht="105">
       <c r="B32" s="25" t="s">
-        <v>53</v>
+        <v>467</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>3</v>
@@ -4394,7 +4433,7 @@
         <v>154</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>490</v>
+        <v>317</v>
       </c>
       <c r="G32" s="25" t="s">
         <v>73</v>
@@ -4416,66 +4455,72 @@
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25" t="s">
-        <v>201</v>
+        <v>463</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S32" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="2:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" ht="105">
       <c r="B33" s="25" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="E33" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="25"/>
+        <v>154</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>490</v>
+      </c>
       <c r="G33" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="25"/>
+        <v>42</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
       <c r="L33" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25" t="s">
-        <v>478</v>
-      </c>
+      <c r="M33" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="N33" s="25"/>
       <c r="O33" s="25"/>
       <c r="P33" s="25" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="25" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" ht="78.75" customHeight="1">
       <c r="B34" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="25" t="s">
@@ -4494,26 +4539,24 @@
       <c r="N34" s="25" t="s">
         <v>478</v>
       </c>
-      <c r="O34" s="25" t="b">
-        <v>1</v>
-      </c>
+      <c r="O34" s="25"/>
       <c r="P34" s="25" t="s">
-        <v>314</v>
+        <v>87</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S34" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" ht="75">
       <c r="B35" s="25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
@@ -4524,7 +4567,7 @@
         <v>3</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25"/>
@@ -4534,30 +4577,32 @@
       </c>
       <c r="M35" s="25"/>
       <c r="N35" s="25" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="O35" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="P35" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="P35" s="25" t="s">
+        <v>314</v>
+      </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S35" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" ht="45">
       <c r="B36" s="25" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="25" t="s">
@@ -4566,9 +4611,7 @@
       <c r="H36" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="25" t="s">
-        <v>128</v>
-      </c>
+      <c r="I36" s="25"/>
       <c r="J36" s="25"/>
       <c r="K36" s="25"/>
       <c r="L36" s="25" t="s">
@@ -4576,26 +4619,26 @@
       </c>
       <c r="M36" s="25"/>
       <c r="N36" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25" t="s">
-        <v>129</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="O36" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="P36" s="25"/>
       <c r="Q36" s="25"/>
       <c r="R36" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" ht="30">
       <c r="B37" s="25" t="s">
-        <v>468</v>
+        <v>126</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>469</v>
+        <v>127</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
@@ -4609,7 +4652,7 @@
         <v>43</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>470</v>
+        <v>128</v>
       </c>
       <c r="J37" s="25"/>
       <c r="K37" s="25"/>
@@ -4618,32 +4661,30 @@
       </c>
       <c r="M37" s="25"/>
       <c r="N37" s="25" t="s">
-        <v>477</v>
-      </c>
-      <c r="O37" s="25" t="s">
-        <v>471</v>
-      </c>
+        <v>476</v>
+      </c>
+      <c r="O37" s="25"/>
       <c r="P37" s="25" t="s">
-        <v>704</v>
+        <v>129</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="25" t="s">
-        <v>472</v>
+        <v>152</v>
       </c>
       <c r="S37" s="25" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="38" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" ht="45">
       <c r="B38" s="25" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
-        <v>159</v>
+        <v>1</v>
       </c>
       <c r="F38" s="25"/>
       <c r="G38" s="25" t="s">
@@ -4661,23 +4702,29 @@
         <v>3</v>
       </c>
       <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
+      <c r="N38" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="O38" s="25" t="s">
+        <v>471</v>
+      </c>
       <c r="P38" s="25" t="s">
-        <v>3</v>
+        <v>704</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="S38" s="25"/>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+      <c r="S38" s="25" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" ht="30">
       <c r="B39" s="25" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="25" t="s">
@@ -4710,12 +4757,12 @@
       </c>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19">
       <c r="B40" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25" t="s">
@@ -4748,41 +4795,79 @@
       </c>
       <c r="S40" s="25"/>
     </row>
-    <row r="42" spans="2:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
+    <row r="41" spans="2:19">
+      <c r="B41" s="25" t="s">
+        <v>486</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>488</v>
+      </c>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I41" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="S41" s="25"/>
+    </row>
+    <row r="43" spans="2:19" ht="45">
+      <c r="B43" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C43" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25" t="s">
+      <c r="D43" s="25"/>
+      <c r="E43" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H42" s="25" t="s">
+      <c r="F43" s="25"/>
+      <c r="G43" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H43" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25" t="s">
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25" t="s">
         <v>475</v>
       </c>
-      <c r="O42" s="25"/>
-      <c r="P42" s="25"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="25" t="s">
+      <c r="O43" s="25"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S42" s="25" t="s">
+      <c r="S43" s="25" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4805,26 +4890,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+    <row r="5" spans="2:6">
+      <c r="B5" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="43" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -4834,8 +4919,8 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
+    <row r="7" spans="2:6">
+      <c r="B7" s="43"/>
       <c r="C7" s="24" t="s">
         <v>113</v>
       </c>
@@ -4843,8 +4928,8 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
+    <row r="8" spans="2:6">
+      <c r="B8" s="43"/>
       <c r="C8" s="24" t="s">
         <v>134</v>
       </c>
@@ -4852,8 +4937,8 @@
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+    <row r="9" spans="2:6">
+      <c r="B9" s="43"/>
       <c r="C9" s="24" t="s">
         <v>135</v>
       </c>
@@ -4861,14 +4946,14 @@
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="42" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" s="43"/>
+      <c r="C10" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4881,14 +4966,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
@@ -4896,15 +4981,15 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+    <row r="2" spans="2:5" ht="15" customHeight="1">
+      <c r="B2" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="52"/>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -4918,7 +5003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
@@ -4932,7 +5017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="15" t="s">
         <v>112</v>
       </c>
@@ -4944,71 +5029,111 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="2:5">
+      <c r="B6" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+    <row r="8" spans="2:5">
+      <c r="B8" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>463</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>157</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>156</v>
+        <v>463</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
       <c r="B9" s="19" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>157</v>
       </c>
       <c r="D9" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E10" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+    <row r="11" spans="2:5">
+      <c r="B11" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C13" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D13" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E13" s="31" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5022,14 +5147,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:K216"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
@@ -5040,21 +5165,21 @@
     <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+    <row r="3" spans="2:11">
+      <c r="B3" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="F3" s="51" t="s">
+      <c r="C3" s="54"/>
+      <c r="F3" s="53" t="s">
         <v>462</v>
       </c>
-      <c r="G3" s="52"/>
-      <c r="J3" s="51" t="s">
+      <c r="G3" s="54"/>
+      <c r="J3" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="52"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="54"/>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -5074,7 +5199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" s="6" t="s">
         <v>131</v>
       </c>
@@ -5094,7 +5219,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="8" t="s">
         <v>203</v>
       </c>
@@ -5114,7 +5239,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="8" t="s">
         <v>498</v>
       </c>
@@ -5134,7 +5259,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="8" t="s">
         <v>168</v>
       </c>
@@ -5154,7 +5279,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="8" t="s">
         <v>163</v>
       </c>
@@ -5174,7 +5299,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="8" t="s">
         <v>499</v>
       </c>
@@ -5188,7 +5313,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="8" t="s">
         <v>500</v>
       </c>
@@ -5202,7 +5327,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="8" t="s">
         <v>452</v>
       </c>
@@ -5216,7 +5341,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="8" t="s">
         <v>501</v>
       </c>
@@ -5230,7 +5355,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="8" t="s">
         <v>502</v>
       </c>
@@ -5243,12 +5368,12 @@
       <c r="G14" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="J14" s="51" t="s">
+      <c r="J14" s="53" t="s">
         <v>461</v>
       </c>
-      <c r="K14" s="52"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="54"/>
+    </row>
+    <row r="15" spans="2:11">
       <c r="B15" s="8" t="s">
         <v>503</v>
       </c>
@@ -5268,7 +5393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="8" t="s">
         <v>167</v>
       </c>
@@ -5288,7 +5413,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="B17" s="8" t="s">
         <v>504</v>
       </c>
@@ -5308,7 +5433,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="8" t="s">
         <v>166</v>
       </c>
@@ -5328,7 +5453,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="8" t="s">
         <v>505</v>
       </c>
@@ -5348,7 +5473,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="8" t="s">
         <v>449</v>
       </c>
@@ -5368,7 +5493,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="B21" s="8" t="s">
         <v>211</v>
       </c>
@@ -5388,7 +5513,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="8" t="s">
         <v>506</v>
       </c>
@@ -5402,7 +5527,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="B23" s="8" t="s">
         <v>507</v>
       </c>
@@ -5416,7 +5541,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="8" t="s">
         <v>508</v>
       </c>
@@ -5430,7 +5555,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="8" t="s">
         <v>509</v>
       </c>
@@ -5444,7 +5569,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="8" t="s">
         <v>510</v>
       </c>
@@ -5458,7 +5583,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="8" t="s">
         <v>511</v>
       </c>
@@ -5472,7 +5597,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="8" t="s">
         <v>512</v>
       </c>
@@ -5486,7 +5611,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="B29" s="8" t="s">
         <v>513</v>
       </c>
@@ -5500,7 +5625,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="B30" s="8" t="s">
         <v>514</v>
       </c>
@@ -5514,7 +5639,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="B31" s="8" t="s">
         <v>515</v>
       </c>
@@ -5528,7 +5653,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="B32" s="8" t="s">
         <v>516</v>
       </c>
@@ -5542,7 +5667,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="B33" s="8" t="s">
         <v>170</v>
       </c>
@@ -5556,7 +5681,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7">
       <c r="B34" s="8" t="s">
         <v>171</v>
       </c>
@@ -5570,7 +5695,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7">
       <c r="B35" s="8" t="s">
         <v>517</v>
       </c>
@@ -5584,7 +5709,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7">
       <c r="B36" s="8" t="s">
         <v>518</v>
       </c>
@@ -5598,7 +5723,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="14.25" customHeight="1">
       <c r="B37" s="8" t="s">
         <v>519</v>
       </c>
@@ -5612,7 +5737,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7">
       <c r="B38" s="8" t="s">
         <v>520</v>
       </c>
@@ -5626,7 +5751,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7">
       <c r="B39" s="8" t="s">
         <v>451</v>
       </c>
@@ -5640,7 +5765,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7">
       <c r="B40" s="8" t="s">
         <v>521</v>
       </c>
@@ -5654,7 +5779,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7">
       <c r="B41" s="8" t="s">
         <v>172</v>
       </c>
@@ -5668,7 +5793,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7">
       <c r="B42" s="8" t="s">
         <v>222</v>
       </c>
@@ -5682,7 +5807,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7">
       <c r="B43" s="8" t="s">
         <v>522</v>
       </c>
@@ -5696,7 +5821,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7">
       <c r="B44" s="8" t="s">
         <v>523</v>
       </c>
@@ -5710,7 +5835,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7">
       <c r="B45" s="8" t="s">
         <v>224</v>
       </c>
@@ -5724,7 +5849,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7">
       <c r="B46" s="8" t="s">
         <v>174</v>
       </c>
@@ -5738,7 +5863,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7">
       <c r="B47" s="8" t="s">
         <v>321</v>
       </c>
@@ -5752,7 +5877,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7">
       <c r="B48" s="8" t="s">
         <v>524</v>
       </c>
@@ -5766,7 +5891,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7">
       <c r="B49" s="8" t="s">
         <v>525</v>
       </c>
@@ -5780,7 +5905,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7">
       <c r="B50" s="8" t="s">
         <v>453</v>
       </c>
@@ -5794,7 +5919,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7">
       <c r="B51" s="8" t="s">
         <v>526</v>
       </c>
@@ -5808,7 +5933,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7">
       <c r="B52" s="8" t="s">
         <v>454</v>
       </c>
@@ -5822,7 +5947,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7">
       <c r="B53" s="8" t="s">
         <v>527</v>
       </c>
@@ -5836,7 +5961,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7">
       <c r="B54" s="8" t="s">
         <v>528</v>
       </c>
@@ -5850,7 +5975,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7">
       <c r="B55" s="8" t="s">
         <v>529</v>
       </c>
@@ -5864,7 +5989,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7">
       <c r="B56" s="8" t="s">
         <v>249</v>
       </c>
@@ -5878,7 +6003,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7">
       <c r="B57" s="8" t="s">
         <v>164</v>
       </c>
@@ -5892,7 +6017,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7">
       <c r="B58" s="8" t="s">
         <v>239</v>
       </c>
@@ -5900,7 +6025,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7">
       <c r="B59" s="8" t="s">
         <v>530</v>
       </c>
@@ -5908,7 +6033,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7">
       <c r="B60" s="8" t="s">
         <v>165</v>
       </c>
@@ -5916,7 +6041,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7">
       <c r="B61" s="8" t="s">
         <v>531</v>
       </c>
@@ -5924,7 +6049,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7">
       <c r="B62" s="8" t="s">
         <v>532</v>
       </c>
@@ -5932,7 +6057,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7">
       <c r="B63" s="8" t="s">
         <v>533</v>
       </c>
@@ -5940,7 +6065,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7">
       <c r="B64" s="8" t="s">
         <v>273</v>
       </c>
@@ -5948,7 +6073,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3">
       <c r="B65" s="8" t="s">
         <v>534</v>
       </c>
@@ -5956,7 +6081,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3">
       <c r="B66" s="8" t="s">
         <v>535</v>
       </c>
@@ -5964,7 +6089,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3">
       <c r="B67" s="8" t="s">
         <v>536</v>
       </c>
@@ -5972,7 +6097,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" s="8" t="s">
         <v>537</v>
       </c>
@@ -5980,7 +6105,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" s="8" t="s">
         <v>538</v>
       </c>
@@ -5988,7 +6113,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3">
       <c r="B70" s="8" t="s">
         <v>481</v>
       </c>
@@ -5996,7 +6121,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3">
       <c r="B71" s="8" t="s">
         <v>539</v>
       </c>
@@ -6004,7 +6129,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3">
       <c r="B72" s="8" t="s">
         <v>540</v>
       </c>
@@ -6012,7 +6137,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3">
       <c r="B73" s="8" t="s">
         <v>133</v>
       </c>
@@ -6020,7 +6145,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3">
       <c r="B74" s="8" t="s">
         <v>541</v>
       </c>
@@ -6028,7 +6153,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3">
       <c r="B75" s="8" t="s">
         <v>542</v>
       </c>
@@ -6036,7 +6161,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3">
       <c r="B76" s="8" t="s">
         <v>543</v>
       </c>
@@ -6044,7 +6169,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3">
       <c r="B77" s="8" t="s">
         <v>544</v>
       </c>
@@ -6052,7 +6177,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3">
       <c r="B78" s="8" t="s">
         <v>545</v>
       </c>
@@ -6060,7 +6185,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3">
       <c r="B79" s="8" t="s">
         <v>175</v>
       </c>
@@ -6068,7 +6193,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3">
       <c r="B80" s="8" t="s">
         <v>546</v>
       </c>
@@ -6076,7 +6201,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3">
       <c r="B81" s="8" t="s">
         <v>279</v>
       </c>
@@ -6084,7 +6209,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3">
       <c r="B82" s="8" t="s">
         <v>304</v>
       </c>
@@ -6092,7 +6217,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3">
       <c r="B83" s="8" t="s">
         <v>173</v>
       </c>
@@ -6100,7 +6225,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3">
       <c r="B84" s="8" t="s">
         <v>491</v>
       </c>
@@ -6108,7 +6233,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3">
       <c r="B85" s="8" t="s">
         <v>448</v>
       </c>
@@ -6116,7 +6241,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3">
       <c r="B86" s="8" t="s">
         <v>492</v>
       </c>
@@ -6124,7 +6249,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3">
       <c r="B87" s="8" t="s">
         <v>281</v>
       </c>
@@ -6132,7 +6257,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3">
       <c r="B88" s="8" t="s">
         <v>450</v>
       </c>
@@ -6140,7 +6265,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3">
       <c r="B89" s="8" t="s">
         <v>320</v>
       </c>
@@ -6148,7 +6273,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3">
       <c r="B90" s="8" t="s">
         <v>493</v>
       </c>
@@ -6156,7 +6281,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3">
       <c r="B91" s="8" t="s">
         <v>169</v>
       </c>
@@ -6164,7 +6289,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3">
       <c r="B92" s="8" t="s">
         <v>69</v>
       </c>
@@ -6172,7 +6297,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3">
       <c r="B93" s="8" t="s">
         <v>494</v>
       </c>
@@ -6180,7 +6305,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3">
       <c r="B94" s="8" t="s">
         <v>495</v>
       </c>
@@ -6188,7 +6313,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3">
       <c r="B95" s="8" t="s">
         <v>496</v>
       </c>
@@ -6196,7 +6321,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3">
       <c r="B96" s="8" t="s">
         <v>497</v>
       </c>
@@ -6204,13 +6329,13 @@
         <v>703</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="51" t="s">
+    <row r="100" spans="2:3">
+      <c r="B100" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="C100" s="52"/>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="54"/>
+    </row>
+    <row r="101" spans="2:3">
       <c r="B101" s="6" t="s">
         <v>0</v>
       </c>
@@ -6218,7 +6343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3">
       <c r="B102" s="6" t="s">
         <v>131</v>
       </c>
@@ -6226,7 +6351,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3">
       <c r="B103" s="8" t="s">
         <v>606</v>
       </c>
@@ -6234,7 +6359,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3">
       <c r="B104" s="8" t="s">
         <v>575</v>
       </c>
@@ -6242,7 +6367,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3">
       <c r="B105" s="8" t="s">
         <v>576</v>
       </c>
@@ -6250,7 +6375,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3">
       <c r="B106" s="8" t="s">
         <v>578</v>
       </c>
@@ -6258,7 +6383,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3">
       <c r="B107" s="8" t="s">
         <v>579</v>
       </c>
@@ -6266,7 +6391,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3">
       <c r="B108" s="8" t="s">
         <v>196</v>
       </c>
@@ -6274,7 +6399,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3">
       <c r="B109" s="8" t="s">
         <v>417</v>
       </c>
@@ -6282,7 +6407,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3">
       <c r="B110" s="8" t="s">
         <v>580</v>
       </c>
@@ -6290,7 +6415,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3">
       <c r="B111" s="8" t="s">
         <v>581</v>
       </c>
@@ -6298,7 +6423,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3">
       <c r="B112" s="8" t="s">
         <v>600</v>
       </c>
@@ -6306,7 +6431,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3">
       <c r="B113" s="8" t="s">
         <v>583</v>
       </c>
@@ -6314,7 +6439,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3">
       <c r="B114" s="8" t="s">
         <v>584</v>
       </c>
@@ -6322,7 +6447,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3">
       <c r="B115" s="8" t="s">
         <v>585</v>
       </c>
@@ -6330,7 +6455,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3">
       <c r="B116" s="8" t="s">
         <v>198</v>
       </c>
@@ -6338,7 +6463,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3">
       <c r="B117" s="8" t="s">
         <v>582</v>
       </c>
@@ -6346,7 +6471,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3">
       <c r="B118" s="8" t="s">
         <v>587</v>
       </c>
@@ -6354,7 +6479,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3">
       <c r="B119" s="8" t="s">
         <v>589</v>
       </c>
@@ -6362,7 +6487,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3">
       <c r="B120" s="8" t="s">
         <v>590</v>
       </c>
@@ -6370,7 +6495,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3">
       <c r="B121" s="8" t="s">
         <v>591</v>
       </c>
@@ -6378,7 +6503,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3">
       <c r="B122" s="8" t="s">
         <v>586</v>
       </c>
@@ -6386,7 +6511,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3">
       <c r="B123" s="8" t="s">
         <v>194</v>
       </c>
@@ -6394,7 +6519,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3">
       <c r="B124" s="8" t="s">
         <v>593</v>
       </c>
@@ -6402,7 +6527,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3">
       <c r="B125" s="8" t="s">
         <v>594</v>
       </c>
@@ -6410,7 +6535,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3">
       <c r="B126" s="8" t="s">
         <v>596</v>
       </c>
@@ -6418,7 +6543,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3">
       <c r="B127" s="8" t="s">
         <v>597</v>
       </c>
@@ -6426,7 +6551,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3">
       <c r="B128" s="8" t="s">
         <v>599</v>
       </c>
@@ -6434,7 +6559,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3">
       <c r="B129" s="8" t="s">
         <v>598</v>
       </c>
@@ -6442,7 +6567,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3">
       <c r="B130" s="8" t="s">
         <v>601</v>
       </c>
@@ -6450,7 +6575,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3">
       <c r="B131" s="8" t="s">
         <v>602</v>
       </c>
@@ -6458,7 +6583,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3">
       <c r="B132" s="8" t="s">
         <v>189</v>
       </c>
@@ -6466,7 +6591,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3">
       <c r="B133" s="8" t="s">
         <v>603</v>
       </c>
@@ -6474,7 +6599,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3">
       <c r="B134" s="8" t="s">
         <v>191</v>
       </c>
@@ -6482,7 +6607,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3">
       <c r="B135" s="8" t="s">
         <v>607</v>
       </c>
@@ -6490,7 +6615,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3">
       <c r="B136" s="8" t="s">
         <v>604</v>
       </c>
@@ -6498,7 +6623,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3">
       <c r="B137" s="8" t="s">
         <v>605</v>
       </c>
@@ -6506,7 +6631,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3">
       <c r="B138" s="8" t="s">
         <v>608</v>
       </c>
@@ -6514,7 +6639,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3">
       <c r="B139" s="8" t="s">
         <v>609</v>
       </c>
@@ -6522,7 +6647,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3">
       <c r="B140" s="8" t="s">
         <v>610</v>
       </c>
@@ -6530,7 +6655,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3">
       <c r="B141" s="8" t="s">
         <v>611</v>
       </c>
@@ -6538,13 +6663,13 @@
         <v>574</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="51" t="s">
+    <row r="144" spans="2:3">
+      <c r="B144" s="53" t="s">
         <v>613</v>
       </c>
-      <c r="C144" s="52"/>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="54"/>
+    </row>
+    <row r="145" spans="2:3">
       <c r="B145" s="6" t="s">
         <v>0</v>
       </c>
@@ -6552,7 +6677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3">
       <c r="B146" s="6" t="s">
         <v>131</v>
       </c>
@@ -6560,7 +6685,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3">
       <c r="B147" s="8" t="s">
         <v>322</v>
       </c>
@@ -6568,7 +6693,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3">
       <c r="B148" s="8" t="s">
         <v>324</v>
       </c>
@@ -6576,7 +6701,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3">
       <c r="B149" s="8" t="s">
         <v>180</v>
       </c>
@@ -6584,7 +6709,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3">
       <c r="B150" s="8" t="s">
         <v>176</v>
       </c>
@@ -6592,7 +6717,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3">
       <c r="B151" s="8" t="s">
         <v>328</v>
       </c>
@@ -6600,7 +6725,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3">
       <c r="B152" s="8" t="s">
         <v>162</v>
       </c>
@@ -6608,7 +6733,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3">
       <c r="B153" s="8" t="s">
         <v>331</v>
       </c>
@@ -6616,7 +6741,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3">
       <c r="B154" s="8" t="s">
         <v>333</v>
       </c>
@@ -6624,7 +6749,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3">
       <c r="B155" s="8" t="s">
         <v>179</v>
       </c>
@@ -6632,7 +6757,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3">
       <c r="B156" s="8" t="s">
         <v>186</v>
       </c>
@@ -6640,7 +6765,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3">
       <c r="B157" s="8" t="s">
         <v>338</v>
       </c>
@@ -6648,7 +6773,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3">
       <c r="B158" s="8" t="s">
         <v>182</v>
       </c>
@@ -6656,7 +6781,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3">
       <c r="B159" s="8" t="s">
         <v>341</v>
       </c>
@@ -6664,7 +6789,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3">
       <c r="B160" s="8" t="s">
         <v>343</v>
       </c>
@@ -6672,7 +6797,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3">
       <c r="B161" s="8" t="s">
         <v>345</v>
       </c>
@@ -6680,7 +6805,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3">
       <c r="B162" s="8" t="s">
         <v>347</v>
       </c>
@@ -6688,7 +6813,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:3">
       <c r="B163" s="8" t="s">
         <v>349</v>
       </c>
@@ -6696,7 +6821,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:3">
       <c r="B164" s="8" t="s">
         <v>351</v>
       </c>
@@ -6704,7 +6829,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:3">
       <c r="B165" s="8" t="s">
         <v>354</v>
       </c>
@@ -6712,7 +6837,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:3">
       <c r="B166" s="8" t="s">
         <v>181</v>
       </c>
@@ -6720,7 +6845,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:3">
       <c r="B167" s="8" t="s">
         <v>356</v>
       </c>
@@ -6728,7 +6853,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:3">
       <c r="B168" s="8" t="s">
         <v>358</v>
       </c>
@@ -6736,7 +6861,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:3">
       <c r="B169" s="8" t="s">
         <v>360</v>
       </c>
@@ -6744,7 +6869,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:3">
       <c r="B170" s="8" t="s">
         <v>362</v>
       </c>
@@ -6752,7 +6877,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:3">
       <c r="B171" s="8" t="s">
         <v>364</v>
       </c>
@@ -6760,7 +6885,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:3">
       <c r="B172" s="8" t="s">
         <v>183</v>
       </c>
@@ -6768,7 +6893,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3">
       <c r="B173" s="8" t="s">
         <v>353</v>
       </c>
@@ -6776,7 +6901,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:3">
       <c r="B174" s="8" t="s">
         <v>368</v>
       </c>
@@ -6784,7 +6909,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:3">
       <c r="B175" s="8" t="s">
         <v>370</v>
       </c>
@@ -6792,7 +6917,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:3">
       <c r="B176" s="8" t="s">
         <v>372</v>
       </c>
@@ -6800,7 +6925,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3">
       <c r="B177" s="8" t="s">
         <v>374</v>
       </c>
@@ -6808,7 +6933,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3">
       <c r="B178" s="8" t="s">
         <v>376</v>
       </c>
@@ -6816,7 +6941,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3">
       <c r="B179" s="8" t="s">
         <v>378</v>
       </c>
@@ -6824,7 +6949,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:3">
       <c r="B180" s="8" t="s">
         <v>380</v>
       </c>
@@ -6832,7 +6957,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:3">
       <c r="B181" s="8" t="s">
         <v>383</v>
       </c>
@@ -6840,7 +6965,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:3">
       <c r="B182" s="8" t="s">
         <v>385</v>
       </c>
@@ -6848,7 +6973,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:3">
       <c r="B183" s="8" t="s">
         <v>387</v>
       </c>
@@ -6856,7 +6981,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:3">
       <c r="B184" s="8" t="s">
         <v>177</v>
       </c>
@@ -6864,7 +6989,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:3">
       <c r="B185" s="8" t="s">
         <v>390</v>
       </c>
@@ -6872,7 +6997,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:3">
       <c r="B186" s="8" t="s">
         <v>178</v>
       </c>
@@ -6880,7 +7005,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:3">
       <c r="B187" s="8" t="s">
         <v>393</v>
       </c>
@@ -6888,7 +7013,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:3">
       <c r="B188" s="8" t="s">
         <v>335</v>
       </c>
@@ -6896,7 +7021,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:3">
       <c r="B189" s="8" t="s">
         <v>396</v>
       </c>
@@ -6904,7 +7029,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:3">
       <c r="B190" s="8" t="s">
         <v>398</v>
       </c>
@@ -6912,7 +7037,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:3">
       <c r="B191" s="8" t="s">
         <v>400</v>
       </c>
@@ -6920,7 +7045,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:3">
       <c r="B192" s="8" t="s">
         <v>402</v>
       </c>
@@ -6928,7 +7053,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:3">
       <c r="B193" s="8" t="s">
         <v>404</v>
       </c>
@@ -6936,7 +7061,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:3">
       <c r="B194" s="8" t="s">
         <v>406</v>
       </c>
@@ -6944,7 +7069,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:3">
       <c r="B195" s="8" t="s">
         <v>408</v>
       </c>
@@ -6952,7 +7077,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:3">
       <c r="B196" s="8" t="s">
         <v>410</v>
       </c>
@@ -6960,7 +7085,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:3">
       <c r="B197" s="8" t="s">
         <v>161</v>
       </c>
@@ -6968,7 +7093,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:3">
       <c r="B198" s="8" t="s">
         <v>413</v>
       </c>
@@ -6976,7 +7101,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:3">
       <c r="B199" s="8" t="s">
         <v>415</v>
       </c>
@@ -6984,7 +7109,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:3">
       <c r="B200" s="8" t="s">
         <v>418</v>
       </c>
@@ -6992,7 +7117,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:3">
       <c r="B201" s="8" t="s">
         <v>185</v>
       </c>
@@ -7000,7 +7125,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:3">
       <c r="B202" s="8" t="s">
         <v>421</v>
       </c>
@@ -7008,7 +7133,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:3">
       <c r="B203" s="8" t="s">
         <v>423</v>
       </c>
@@ -7016,7 +7141,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:3">
       <c r="B204" s="8" t="s">
         <v>382</v>
       </c>
@@ -7024,7 +7149,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:3">
       <c r="B205" s="8" t="s">
         <v>426</v>
       </c>
@@ -7032,7 +7157,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:3">
       <c r="B206" s="8" t="s">
         <v>428</v>
       </c>
@@ -7040,7 +7165,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:3">
       <c r="B207" s="8" t="s">
         <v>430</v>
       </c>
@@ -7048,7 +7173,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:3">
       <c r="B208" s="8" t="s">
         <v>432</v>
       </c>
@@ -7056,7 +7181,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:3">
       <c r="B209" s="8" t="s">
         <v>434</v>
       </c>
@@ -7064,7 +7189,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:3">
       <c r="B210" s="8" t="s">
         <v>436</v>
       </c>
@@ -7072,7 +7197,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:3">
       <c r="B211" s="8" t="s">
         <v>184</v>
       </c>
@@ -7080,7 +7205,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:3">
       <c r="B212" s="8" t="s">
         <v>68</v>
       </c>
@@ -7088,7 +7213,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:3">
       <c r="B213" s="8" t="s">
         <v>440</v>
       </c>
@@ -7096,7 +7221,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:3">
       <c r="B214" s="8" t="s">
         <v>442</v>
       </c>
@@ -7104,7 +7229,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:3">
       <c r="B215" s="8" t="s">
         <v>444</v>
       </c>
@@ -7112,7 +7237,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:3">
       <c r="B216" s="8" t="s">
         <v>446</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-2774 Place property 'StartRequestdate' after effective and expiration date
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -2185,8 +2185,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2628,11 +2628,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2640,23 +2649,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2699,7 +2699,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2712,9 +2712,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2752,7 +2752,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2786,6 +2786,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2820,9 +2821,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2995,69 +2997,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="74.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-    </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="40" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="39"/>
@@ -3068,67 +3070,67 @@
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+    </row>
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-    </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-    </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1">
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-    </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
@@ -3143,11 +3145,11 @@
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1">
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="40" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="39"/>
@@ -3158,11 +3160,11 @@
       <c r="I11" s="39"/>
       <c r="J11" s="39"/>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="34" t="s">
         <v>119</v>
       </c>
       <c r="D12" s="39"/>
@@ -3173,11 +3175,11 @@
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1">
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="34" t="s">
         <v>106</v>
       </c>
       <c r="D13" s="39"/>
@@ -3188,36 +3190,42 @@
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
     </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1">
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1">
-      <c r="B15" s="41" t="s">
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3226,28 +3234,22 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
@@ -3271,65 +3273,65 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
+    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-    </row>
-    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-    </row>
-    <row r="3" spans="2:19" ht="57.75" customHeight="1">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-    </row>
-    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="40" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="39"/>
@@ -3343,79 +3345,79 @@
       <c r="L4" s="39"/>
       <c r="M4" s="39"/>
     </row>
-    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
+    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-    </row>
-    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+    </row>
+    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-    </row>
-    <row r="7" spans="2:19" ht="42.75" customHeight="1">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+    </row>
+    <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-    </row>
-    <row r="8" spans="2:19" ht="33" customHeight="1">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+    </row>
+    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
@@ -3433,7 +3435,7 @@
       <c r="L9" s="39"/>
       <c r="M9" s="39"/>
     </row>
-    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3445,7 +3447,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="2:19" ht="15" customHeight="1">
+    <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="42" t="s">
         <v>28</v>
       </c>
@@ -3467,7 +3469,7 @@
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
     </row>
-    <row r="12" spans="2:19" ht="30">
+    <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
@@ -3523,7 +3525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:19" ht="60">
+    <row r="13" spans="2:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>29</v>
       </c>
@@ -3579,7 +3581,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:19">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>11</v>
       </c>
@@ -3623,7 +3625,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="105">
+    <row r="15" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
@@ -3667,7 +3669,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="2:19" s="4" customFormat="1">
+    <row r="16" spans="2:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>35</v>
       </c>
@@ -3711,7 +3713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="30">
+    <row r="17" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>21</v>
       </c>
@@ -3755,7 +3757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="90">
+    <row r="18" spans="2:19" ht="90" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>316</v>
       </c>
@@ -3803,21 +3805,21 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="2:19" s="32" customFormat="1" ht="30">
+    <row r="19" spans="2:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>707</v>
+        <v>315</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>708</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>3</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>711</v>
+        <v>474</v>
       </c>
       <c r="G19" s="25" t="s">
         <v>73</v>
@@ -3839,7 +3841,7 @@
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>118</v>
@@ -3848,24 +3850,24 @@
         <v>150</v>
       </c>
       <c r="S19" s="25" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" ht="75">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>315</v>
+        <v>707</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>3</v>
+        <v>708</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>474</v>
+        <v>711</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>73</v>
@@ -3887,7 +3889,7 @@
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q20" s="25" t="s">
         <v>118</v>
@@ -3896,10 +3898,10 @@
         <v>150</v>
       </c>
       <c r="S20" s="25" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>22</v>
       </c>
@@ -3947,7 +3949,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:19">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
         <v>23</v>
       </c>
@@ -3997,7 +3999,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:19">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>24</v>
       </c>
@@ -4045,7 +4047,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="2:19">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>25</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="45">
+    <row r="25" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
         <v>26</v>
       </c>
@@ -4139,7 +4141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:19" ht="30">
+    <row r="26" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
         <v>45</v>
       </c>
@@ -4185,7 +4187,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="105">
+    <row r="27" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
         <v>49</v>
       </c>
@@ -4231,7 +4233,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="105">
+    <row r="28" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
         <v>54</v>
       </c>
@@ -4277,7 +4279,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="105">
+    <row r="29" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
         <v>466</v>
       </c>
@@ -4323,7 +4325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="105">
+    <row r="30" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
         <v>56</v>
       </c>
@@ -4371,7 +4373,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="105">
+    <row r="31" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
         <v>57</v>
       </c>
@@ -4419,7 +4421,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="2:19" ht="105">
+    <row r="32" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
         <v>467</v>
       </c>
@@ -4465,7 +4467,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:19" ht="105">
+    <row r="33" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>53</v>
       </c>
@@ -4511,7 +4513,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="78.75" customHeight="1">
+    <row r="34" spans="2:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
         <v>83</v>
       </c>
@@ -4551,7 +4553,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="2:19" ht="75">
+    <row r="35" spans="2:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
         <v>85</v>
       </c>
@@ -4593,7 +4595,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="2:19" ht="45">
+    <row r="36" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="25" t="s">
         <v>90</v>
       </c>
@@ -4633,7 +4635,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="2:19" ht="30">
+    <row r="37" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
         <v>126</v>
       </c>
@@ -4675,7 +4677,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="38" spans="2:19" ht="45">
+    <row r="38" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
         <v>468</v>
       </c>
@@ -4719,7 +4721,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="39" spans="2:19" ht="30">
+    <row r="39" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="25" t="s">
         <v>484</v>
       </c>
@@ -4757,7 +4759,7 @@
       </c>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="2:19">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B40" s="25" t="s">
         <v>485</v>
       </c>
@@ -4795,7 +4797,7 @@
       </c>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="2:19">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
         <v>486</v>
       </c>
@@ -4833,7 +4835,7 @@
       </c>
       <c r="S41" s="25"/>
     </row>
-    <row r="43" spans="2:19" ht="45">
+    <row r="43" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B43" s="25" t="s">
         <v>91</v>
       </c>
@@ -4890,16 +4892,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="47" t="s">
         <v>109</v>
       </c>
@@ -4908,7 +4910,7 @@
       <c r="E5" s="48"/>
       <c r="F5" s="49"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="43" t="s">
         <v>110</v>
       </c>
@@ -4919,7 +4921,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="43"/>
       <c r="C7" s="24" t="s">
         <v>113</v>
@@ -4928,7 +4930,7 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="43"/>
       <c r="C8" s="24" t="s">
         <v>134</v>
@@ -4937,7 +4939,7 @@
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="43"/>
       <c r="C9" s="24" t="s">
         <v>135</v>
@@ -4946,7 +4948,7 @@
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="43"/>
       <c r="C10" s="44" t="s">
         <v>158</v>
@@ -4966,14 +4968,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
@@ -4981,7 +4983,7 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" customHeight="1">
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="50" t="s">
         <v>111</v>
       </c>
@@ -4989,7 +4991,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52"/>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -5003,7 +5005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
@@ -5017,7 +5019,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>112</v>
       </c>
@@ -5029,7 +5031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>705</v>
       </c>
@@ -5041,7 +5043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>50</v>
       </c>
@@ -5053,7 +5055,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>125</v>
       </c>
@@ -5067,7 +5069,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>60</v>
       </c>
@@ -5081,7 +5083,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
         <v>123</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>61</v>
       </c>
@@ -5105,11 +5107,11 @@
       <c r="D11" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>62</v>
       </c>
@@ -5123,7 +5125,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>64</v>
       </c>
@@ -5147,14 +5149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K216"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
@@ -5165,7 +5167,7 @@
     <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="53" t="s">
         <v>130</v>
       </c>
@@ -5179,7 +5181,7 @@
       </c>
       <c r="K3" s="54"/>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -5199,7 +5201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>131</v>
       </c>
@@ -5219,7 +5221,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>203</v>
       </c>
@@ -5239,7 +5241,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>498</v>
       </c>
@@ -5259,7 +5261,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>168</v>
       </c>
@@ -5279,7 +5281,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>163</v>
       </c>
@@ -5299,7 +5301,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>499</v>
       </c>
@@ -5313,7 +5315,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>500</v>
       </c>
@@ -5327,7 +5329,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>452</v>
       </c>
@@ -5341,7 +5343,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>501</v>
       </c>
@@ -5355,7 +5357,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>502</v>
       </c>
@@ -5373,7 +5375,7 @@
       </c>
       <c r="K14" s="54"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>503</v>
       </c>
@@ -5393,7 +5395,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>167</v>
       </c>
@@ -5413,7 +5415,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>504</v>
       </c>
@@ -5433,7 +5435,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>166</v>
       </c>
@@ -5453,7 +5455,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>505</v>
       </c>
@@ -5473,7 +5475,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>449</v>
       </c>
@@ -5493,7 +5495,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>211</v>
       </c>
@@ -5513,7 +5515,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>506</v>
       </c>
@@ -5527,7 +5529,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>507</v>
       </c>
@@ -5541,7 +5543,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>508</v>
       </c>
@@ -5555,7 +5557,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>509</v>
       </c>
@@ -5569,7 +5571,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>510</v>
       </c>
@@ -5583,7 +5585,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>511</v>
       </c>
@@ -5597,7 +5599,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>512</v>
       </c>
@@ -5611,7 +5613,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>513</v>
       </c>
@@ -5625,7 +5627,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>514</v>
       </c>
@@ -5639,7 +5641,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>515</v>
       </c>
@@ -5653,7 +5655,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>516</v>
       </c>
@@ -5667,7 +5669,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>170</v>
       </c>
@@ -5681,7 +5683,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>171</v>
       </c>
@@ -5695,7 +5697,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>517</v>
       </c>
@@ -5709,7 +5711,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>518</v>
       </c>
@@ -5723,7 +5725,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="14.25" customHeight="1">
+    <row r="37" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>519</v>
       </c>
@@ -5737,7 +5739,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>520</v>
       </c>
@@ -5751,7 +5753,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>451</v>
       </c>
@@ -5765,7 +5767,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>521</v>
       </c>
@@ -5779,7 +5781,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>172</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>222</v>
       </c>
@@ -5807,7 +5809,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>522</v>
       </c>
@@ -5821,7 +5823,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="44" spans="2:7">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>523</v>
       </c>
@@ -5835,7 +5837,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="2:7">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>224</v>
       </c>
@@ -5849,7 +5851,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="2:7">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>174</v>
       </c>
@@ -5863,7 +5865,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>321</v>
       </c>
@@ -5877,7 +5879,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>524</v>
       </c>
@@ -5891,7 +5893,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>525</v>
       </c>
@@ -5905,7 +5907,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>453</v>
       </c>
@@ -5919,7 +5921,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>526</v>
       </c>
@@ -5933,7 +5935,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>454</v>
       </c>
@@ -5947,7 +5949,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>527</v>
       </c>
@@ -5961,7 +5963,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>528</v>
       </c>
@@ -5975,7 +5977,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>529</v>
       </c>
@@ -5989,7 +5991,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="8" t="s">
         <v>249</v>
       </c>
@@ -6003,7 +6005,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="8" t="s">
         <v>164</v>
       </c>
@@ -6017,7 +6019,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="8" t="s">
         <v>239</v>
       </c>
@@ -6025,7 +6027,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="8" t="s">
         <v>530</v>
       </c>
@@ -6033,7 +6035,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="8" t="s">
         <v>165</v>
       </c>
@@ -6041,7 +6043,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="61" spans="2:7">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="8" t="s">
         <v>531</v>
       </c>
@@ -6049,7 +6051,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="8" t="s">
         <v>532</v>
       </c>
@@ -6057,7 +6059,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="8" t="s">
         <v>533</v>
       </c>
@@ -6065,7 +6067,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="64" spans="2:7">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="s">
         <v>273</v>
       </c>
@@ -6073,7 +6075,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="65" spans="2:3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="s">
         <v>534</v>
       </c>
@@ -6081,7 +6083,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="66" spans="2:3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="s">
         <v>535</v>
       </c>
@@ -6089,7 +6091,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="67" spans="2:3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>536</v>
       </c>
@@ -6097,7 +6099,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>537</v>
       </c>
@@ -6105,7 +6107,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="s">
         <v>538</v>
       </c>
@@ -6113,7 +6115,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="70" spans="2:3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
         <v>481</v>
       </c>
@@ -6121,7 +6123,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="71" spans="2:3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="s">
         <v>539</v>
       </c>
@@ -6129,7 +6131,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="72" spans="2:3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
         <v>540</v>
       </c>
@@ -6137,7 +6139,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="73" spans="2:3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="s">
         <v>133</v>
       </c>
@@ -6145,7 +6147,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="74" spans="2:3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="8" t="s">
         <v>541</v>
       </c>
@@ -6153,7 +6155,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="75" spans="2:3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="8" t="s">
         <v>542</v>
       </c>
@@ -6161,7 +6163,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="2:3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="8" t="s">
         <v>543</v>
       </c>
@@ -6169,7 +6171,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="77" spans="2:3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="8" t="s">
         <v>544</v>
       </c>
@@ -6177,7 +6179,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="78" spans="2:3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
         <v>545</v>
       </c>
@@ -6185,7 +6187,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="79" spans="2:3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="s">
         <v>175</v>
       </c>
@@ -6193,7 +6195,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="80" spans="2:3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>546</v>
       </c>
@@ -6201,7 +6203,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>279</v>
       </c>
@@ -6209,7 +6211,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="82" spans="2:3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="s">
         <v>304</v>
       </c>
@@ -6217,7 +6219,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="83" spans="2:3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="8" t="s">
         <v>173</v>
       </c>
@@ -6225,7 +6227,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="2:3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>491</v>
       </c>
@@ -6233,7 +6235,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="2:3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="s">
         <v>448</v>
       </c>
@@ -6241,7 +6243,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="86" spans="2:3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>492</v>
       </c>
@@ -6249,7 +6251,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="8" t="s">
         <v>281</v>
       </c>
@@ -6257,7 +6259,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="88" spans="2:3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="s">
         <v>450</v>
       </c>
@@ -6265,7 +6267,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="89" spans="2:3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
         <v>320</v>
       </c>
@@ -6273,7 +6275,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="90" spans="2:3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>493</v>
       </c>
@@ -6281,7 +6283,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="91" spans="2:3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
         <v>169</v>
       </c>
@@ -6289,7 +6291,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="92" spans="2:3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="8" t="s">
         <v>69</v>
       </c>
@@ -6297,7 +6299,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="s">
         <v>494</v>
       </c>
@@ -6305,7 +6307,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="8" t="s">
         <v>495</v>
       </c>
@@ -6313,7 +6315,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="95" spans="2:3">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="s">
         <v>496</v>
       </c>
@@ -6321,7 +6323,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="96" spans="2:3">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="8" t="s">
         <v>497</v>
       </c>
@@ -6329,13 +6331,13 @@
         <v>703</v>
       </c>
     </row>
-    <row r="100" spans="2:3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="53" t="s">
         <v>187</v>
       </c>
       <c r="C100" s="54"/>
     </row>
-    <row r="101" spans="2:3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
         <v>0</v>
       </c>
@@ -6343,7 +6345,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="2:3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
         <v>131</v>
       </c>
@@ -6351,7 +6353,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="2:3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="8" t="s">
         <v>606</v>
       </c>
@@ -6359,7 +6361,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="104" spans="2:3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="8" t="s">
         <v>575</v>
       </c>
@@ -6367,7 +6369,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="105" spans="2:3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="8" t="s">
         <v>576</v>
       </c>
@@ -6375,7 +6377,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="106" spans="2:3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="8" t="s">
         <v>578</v>
       </c>
@@ -6383,7 +6385,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="107" spans="2:3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="8" t="s">
         <v>579</v>
       </c>
@@ -6391,7 +6393,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="108" spans="2:3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="8" t="s">
         <v>196</v>
       </c>
@@ -6399,7 +6401,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="2:3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="8" t="s">
         <v>417</v>
       </c>
@@ -6407,7 +6409,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="110" spans="2:3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="8" t="s">
         <v>580</v>
       </c>
@@ -6415,7 +6417,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="111" spans="2:3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="8" t="s">
         <v>581</v>
       </c>
@@ -6423,7 +6425,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="112" spans="2:3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="8" t="s">
         <v>600</v>
       </c>
@@ -6431,7 +6433,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="113" spans="2:3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="8" t="s">
         <v>583</v>
       </c>
@@ -6439,7 +6441,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="114" spans="2:3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="8" t="s">
         <v>584</v>
       </c>
@@ -6447,7 +6449,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="115" spans="2:3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="8" t="s">
         <v>585</v>
       </c>
@@ -6455,7 +6457,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="2:3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="8" t="s">
         <v>198</v>
       </c>
@@ -6463,7 +6465,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="2:3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="8" t="s">
         <v>582</v>
       </c>
@@ -6471,7 +6473,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="118" spans="2:3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="8" t="s">
         <v>587</v>
       </c>
@@ -6479,7 +6481,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="119" spans="2:3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="8" t="s">
         <v>589</v>
       </c>
@@ -6487,7 +6489,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="120" spans="2:3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="8" t="s">
         <v>590</v>
       </c>
@@ -6495,7 +6497,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="121" spans="2:3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="8" t="s">
         <v>591</v>
       </c>
@@ -6503,7 +6505,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="122" spans="2:3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="8" t="s">
         <v>586</v>
       </c>
@@ -6511,7 +6513,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="123" spans="2:3">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="8" t="s">
         <v>194</v>
       </c>
@@ -6519,7 +6521,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="2:3">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="8" t="s">
         <v>593</v>
       </c>
@@ -6527,7 +6529,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="125" spans="2:3">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="8" t="s">
         <v>594</v>
       </c>
@@ -6535,7 +6537,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="126" spans="2:3">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="8" t="s">
         <v>596</v>
       </c>
@@ -6543,7 +6545,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="127" spans="2:3">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="8" t="s">
         <v>597</v>
       </c>
@@ -6551,7 +6553,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="128" spans="2:3">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="8" t="s">
         <v>599</v>
       </c>
@@ -6559,7 +6561,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="129" spans="2:3">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="8" t="s">
         <v>598</v>
       </c>
@@ -6567,7 +6569,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="130" spans="2:3">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="8" t="s">
         <v>601</v>
       </c>
@@ -6575,7 +6577,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="131" spans="2:3">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="8" t="s">
         <v>602</v>
       </c>
@@ -6583,7 +6585,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="132" spans="2:3">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="8" t="s">
         <v>189</v>
       </c>
@@ -6591,7 +6593,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="133" spans="2:3">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="8" t="s">
         <v>603</v>
       </c>
@@ -6599,7 +6601,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="134" spans="2:3">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="8" t="s">
         <v>191</v>
       </c>
@@ -6607,7 +6609,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="2:3">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="8" t="s">
         <v>607</v>
       </c>
@@ -6615,7 +6617,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="136" spans="2:3">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="8" t="s">
         <v>604</v>
       </c>
@@ -6623,7 +6625,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="137" spans="2:3">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="8" t="s">
         <v>605</v>
       </c>
@@ -6631,7 +6633,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="138" spans="2:3">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="8" t="s">
         <v>608</v>
       </c>
@@ -6639,7 +6641,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="139" spans="2:3">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="8" t="s">
         <v>609</v>
       </c>
@@ -6647,7 +6649,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="140" spans="2:3">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="8" t="s">
         <v>610</v>
       </c>
@@ -6655,7 +6657,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="141" spans="2:3">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="8" t="s">
         <v>611</v>
       </c>
@@ -6663,13 +6665,13 @@
         <v>574</v>
       </c>
     </row>
-    <row r="144" spans="2:3">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="53" t="s">
         <v>613</v>
       </c>
       <c r="C144" s="54"/>
     </row>
-    <row r="145" spans="2:3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">
         <v>0</v>
       </c>
@@ -6677,7 +6679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="2:3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="6" t="s">
         <v>131</v>
       </c>
@@ -6685,7 +6687,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="2:3">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="8" t="s">
         <v>322</v>
       </c>
@@ -6693,7 +6695,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="148" spans="2:3">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="8" t="s">
         <v>324</v>
       </c>
@@ -6701,7 +6703,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="149" spans="2:3">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="8" t="s">
         <v>180</v>
       </c>
@@ -6709,7 +6711,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="150" spans="2:3">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="8" t="s">
         <v>176</v>
       </c>
@@ -6717,7 +6719,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="151" spans="2:3">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="8" t="s">
         <v>328</v>
       </c>
@@ -6725,7 +6727,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="152" spans="2:3">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="8" t="s">
         <v>162</v>
       </c>
@@ -6733,7 +6735,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="153" spans="2:3">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="8" t="s">
         <v>331</v>
       </c>
@@ -6741,7 +6743,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="154" spans="2:3">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="8" t="s">
         <v>333</v>
       </c>
@@ -6749,7 +6751,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="155" spans="2:3">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="8" t="s">
         <v>179</v>
       </c>
@@ -6757,7 +6759,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="156" spans="2:3">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="8" t="s">
         <v>186</v>
       </c>
@@ -6765,7 +6767,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="157" spans="2:3">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="8" t="s">
         <v>338</v>
       </c>
@@ -6773,7 +6775,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="158" spans="2:3">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="8" t="s">
         <v>182</v>
       </c>
@@ -6781,7 +6783,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="159" spans="2:3">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="8" t="s">
         <v>341</v>
       </c>
@@ -6789,7 +6791,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="160" spans="2:3">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="8" t="s">
         <v>343</v>
       </c>
@@ -6797,7 +6799,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="161" spans="2:3">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="8" t="s">
         <v>345</v>
       </c>
@@ -6805,7 +6807,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="162" spans="2:3">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="8" t="s">
         <v>347</v>
       </c>
@@ -6813,7 +6815,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="163" spans="2:3">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="8" t="s">
         <v>349</v>
       </c>
@@ -6821,7 +6823,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="164" spans="2:3">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="8" t="s">
         <v>351</v>
       </c>
@@ -6829,7 +6831,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="165" spans="2:3">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="8" t="s">
         <v>354</v>
       </c>
@@ -6837,7 +6839,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="166" spans="2:3">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="8" t="s">
         <v>181</v>
       </c>
@@ -6845,7 +6847,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="167" spans="2:3">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="8" t="s">
         <v>356</v>
       </c>
@@ -6853,7 +6855,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="168" spans="2:3">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="8" t="s">
         <v>358</v>
       </c>
@@ -6861,7 +6863,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="169" spans="2:3">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="8" t="s">
         <v>360</v>
       </c>
@@ -6869,7 +6871,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="170" spans="2:3">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="8" t="s">
         <v>362</v>
       </c>
@@ -6877,7 +6879,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="171" spans="2:3">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="8" t="s">
         <v>364</v>
       </c>
@@ -6885,7 +6887,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="172" spans="2:3">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="8" t="s">
         <v>183</v>
       </c>
@@ -6893,7 +6895,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="173" spans="2:3">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="8" t="s">
         <v>353</v>
       </c>
@@ -6901,7 +6903,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="174" spans="2:3">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="8" t="s">
         <v>368</v>
       </c>
@@ -6909,7 +6911,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="175" spans="2:3">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="8" t="s">
         <v>370</v>
       </c>
@@ -6917,7 +6919,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="176" spans="2:3">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="8" t="s">
         <v>372</v>
       </c>
@@ -6925,7 +6927,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="177" spans="2:3">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="8" t="s">
         <v>374</v>
       </c>
@@ -6933,7 +6935,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="178" spans="2:3">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="8" t="s">
         <v>376</v>
       </c>
@@ -6941,7 +6943,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="179" spans="2:3">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="8" t="s">
         <v>378</v>
       </c>
@@ -6949,7 +6951,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="180" spans="2:3">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="8" t="s">
         <v>380</v>
       </c>
@@ -6957,7 +6959,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="181" spans="2:3">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="8" t="s">
         <v>383</v>
       </c>
@@ -6965,7 +6967,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="182" spans="2:3">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="8" t="s">
         <v>385</v>
       </c>
@@ -6973,7 +6975,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="183" spans="2:3">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="8" t="s">
         <v>387</v>
       </c>
@@ -6981,7 +6983,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="184" spans="2:3">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="8" t="s">
         <v>177</v>
       </c>
@@ -6989,7 +6991,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="185" spans="2:3">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="8" t="s">
         <v>390</v>
       </c>
@@ -6997,7 +6999,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="186" spans="2:3">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="8" t="s">
         <v>178</v>
       </c>
@@ -7005,7 +7007,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="187" spans="2:3">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="8" t="s">
         <v>393</v>
       </c>
@@ -7013,7 +7015,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="188" spans="2:3">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="8" t="s">
         <v>335</v>
       </c>
@@ -7021,7 +7023,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="189" spans="2:3">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="8" t="s">
         <v>396</v>
       </c>
@@ -7029,7 +7031,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="190" spans="2:3">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="8" t="s">
         <v>398</v>
       </c>
@@ -7037,7 +7039,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="191" spans="2:3">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="8" t="s">
         <v>400</v>
       </c>
@@ -7045,7 +7047,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="192" spans="2:3">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="8" t="s">
         <v>402</v>
       </c>
@@ -7053,7 +7055,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="193" spans="2:3">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="8" t="s">
         <v>404</v>
       </c>
@@ -7061,7 +7063,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="194" spans="2:3">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="8" t="s">
         <v>406</v>
       </c>
@@ -7069,7 +7071,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="195" spans="2:3">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="8" t="s">
         <v>408</v>
       </c>
@@ -7077,7 +7079,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="196" spans="2:3">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="8" t="s">
         <v>410</v>
       </c>
@@ -7085,7 +7087,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="197" spans="2:3">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="8" t="s">
         <v>161</v>
       </c>
@@ -7093,7 +7095,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="198" spans="2:3">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="8" t="s">
         <v>413</v>
       </c>
@@ -7101,7 +7103,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="199" spans="2:3">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="8" t="s">
         <v>415</v>
       </c>
@@ -7109,7 +7111,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="200" spans="2:3">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="8" t="s">
         <v>418</v>
       </c>
@@ -7117,7 +7119,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="201" spans="2:3">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" s="8" t="s">
         <v>185</v>
       </c>
@@ -7125,7 +7127,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="202" spans="2:3">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="8" t="s">
         <v>421</v>
       </c>
@@ -7133,7 +7135,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="203" spans="2:3">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" s="8" t="s">
         <v>423</v>
       </c>
@@ -7141,7 +7143,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="204" spans="2:3">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="8" t="s">
         <v>382</v>
       </c>
@@ -7149,7 +7151,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="205" spans="2:3">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="8" t="s">
         <v>426</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="206" spans="2:3">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="8" t="s">
         <v>428</v>
       </c>
@@ -7165,7 +7167,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="207" spans="2:3">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="8" t="s">
         <v>430</v>
       </c>
@@ -7173,7 +7175,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="208" spans="2:3">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="8" t="s">
         <v>432</v>
       </c>
@@ -7181,7 +7183,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="209" spans="2:3">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="8" t="s">
         <v>434</v>
       </c>
@@ -7189,7 +7191,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="210" spans="2:3">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" s="8" t="s">
         <v>436</v>
       </c>
@@ -7197,7 +7199,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="211" spans="2:3">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" s="8" t="s">
         <v>184</v>
       </c>
@@ -7205,7 +7207,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="212" spans="2:3">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" s="8" t="s">
         <v>68</v>
       </c>
@@ -7213,7 +7215,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="213" spans="2:3">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" s="8" t="s">
         <v>440</v>
       </c>
@@ -7221,7 +7223,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="214" spans="2:3">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" s="8" t="s">
         <v>442</v>
       </c>
@@ -7229,7 +7231,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="215" spans="2:3">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="8" t="s">
         <v>444</v>
       </c>
@@ -7237,7 +7239,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="216" spans="2:3">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" s="8" t="s">
         <v>446</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-2776 Add End Request date
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="718">
   <si>
     <t>name</t>
   </si>
@@ -2173,25 +2173,51 @@
     <t>startRequestDate</t>
   </si>
   <si>
-    <t>Start request date</t>
-  </si>
-  <si>
     <t>contains(lang)</t>
   </si>
   <si>
     <t>max(le(requestDate))</t>
+  </si>
+  <si>
+    <t>&lt; endRequestDate</t>
+  </si>
+  <si>
+    <t>The date when rules become available in production, so the requests may be processed by these rules</t>
+  </si>
+  <si>
+    <t>End Request Date</t>
+  </si>
+  <si>
+    <t>endRequestDate</t>
+  </si>
+  <si>
+    <t>min(ge(requestDate))</t>
+  </si>
+  <si>
+    <t>&gt; startRequestDate</t>
+  </si>
+  <si>
+    <t>The last date when rules are available in production, so the requests can't be processed by these rules</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2251,6 +2277,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2544,24 +2577,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2573,10 +2607,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2591,57 +2625,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2649,16 +2671,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2673,33 +2704,40 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3014,218 +3052,212 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3234,6 +3266,12 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3241,12 +3279,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S43"/>
+  <dimension ref="B1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3277,163 +3315,163 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
     </row>
     <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
     </row>
     <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
     </row>
     <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
@@ -3448,26 +3486,26 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
     </row>
     <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
@@ -3853,114 +3891,114 @@
         <v>458</v>
       </c>
     </row>
-    <row r="20" spans="2:19" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
+    <row r="20" spans="2:19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="54" t="s">
         <v>707</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="54" t="s">
         <v>708</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="54" t="s">
+        <v>710</v>
+      </c>
+      <c r="G20" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54" t="s">
         <v>711</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="Q20" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="R20" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="S20" s="54" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="54" t="s">
+        <v>713</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>714</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="54" t="s">
+        <v>715</v>
+      </c>
+      <c r="G21" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H21" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="25" t="s">
+      <c r="I21" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q20" s="25" t="s">
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q21" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="R20" s="25" t="s">
+      <c r="R21" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="S20" s="25" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="S21" s="25" t="s">
-        <v>47</v>
+      <c r="S21" s="54" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="25" t="s">
@@ -3973,7 +4011,7 @@
         <v>73</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>142</v>
@@ -3989,28 +4027,26 @@
       <c r="P22" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q22" s="25" t="s">
-        <v>118</v>
-      </c>
+      <c r="Q22" s="25"/>
       <c r="R22" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S22" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="25" t="s">
@@ -4020,13 +4056,13 @@
         <v>41</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L23" s="25" t="s">
         <v>73</v>
@@ -4039,26 +4075,28 @@
       <c r="P23" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q23" s="25"/>
+      <c r="Q23" s="25" t="s">
+        <v>118</v>
+      </c>
       <c r="R23" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S23" s="25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>459</v>
+        <v>17</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="25" t="s">
@@ -4071,7 +4109,7 @@
         <v>3</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>143</v>
@@ -4087,43 +4125,45 @@
       <c r="P24" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q24" s="25" t="s">
-        <v>118</v>
-      </c>
+      <c r="Q24" s="25"/>
       <c r="R24" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S24" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>14</v>
+        <v>459</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="25" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I25" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
+      <c r="J25" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>143</v>
+      </c>
       <c r="L25" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="M25" s="25" t="s">
         <v>3</v>
@@ -4131,22 +4171,24 @@
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
       <c r="P25" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q25" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="Q25" s="25" t="s">
+        <v>118</v>
+      </c>
       <c r="R25" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S25" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>3</v>
@@ -4172,27 +4214,25 @@
       <c r="M26" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="N26" s="25" t="s">
-        <v>475</v>
-      </c>
+      <c r="N26" s="25"/>
       <c r="O26" s="25"/>
       <c r="P26" s="25" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>3</v>
@@ -4200,17 +4240,15 @@
       <c r="E27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="25" t="s">
-        <v>122</v>
-      </c>
+      <c r="F27" s="25"/>
       <c r="G27" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
@@ -4218,36 +4256,38 @@
         <v>3</v>
       </c>
       <c r="M27" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="N27" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="N27" s="25" t="s">
+        <v>475</v>
+      </c>
       <c r="O27" s="25"/>
       <c r="P27" s="25" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>52</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>154</v>
+        <v>1</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>489</v>
+        <v>122</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>73</v>
@@ -4269,22 +4309,22 @@
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25" t="s">
-        <v>464</v>
+        <v>51</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S28" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
-        <v>466</v>
+        <v>54</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>3</v>
@@ -4293,7 +4333,7 @@
         <v>154</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>155</v>
+        <v>489</v>
       </c>
       <c r="G29" s="25" t="s">
         <v>73</v>
@@ -4302,7 +4342,7 @@
         <v>42</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="J29" s="25"/>
       <c r="K29" s="25"/>
@@ -4315,22 +4355,22 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="P29" s="25" t="s">
-        <v>156</v>
+        <v>464</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S29" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>56</v>
+        <v>466</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>3</v>
@@ -4339,7 +4379,7 @@
         <v>154</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>706</v>
+        <v>155</v>
       </c>
       <c r="G30" s="25" t="s">
         <v>73</v>
@@ -4359,26 +4399,24 @@
         <v>77</v>
       </c>
       <c r="N30" s="25"/>
-      <c r="O30" s="25" t="s">
-        <v>68</v>
-      </c>
+      <c r="O30" s="25"/>
       <c r="P30" s="25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S30" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>3</v>
@@ -4387,7 +4425,7 @@
         <v>154</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>73</v>
@@ -4408,25 +4446,25 @@
       </c>
       <c r="N31" s="25"/>
       <c r="O31" s="25" t="s">
-        <v>583</v>
+        <v>68</v>
       </c>
       <c r="P31" s="25" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
-        <v>467</v>
+        <v>57</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>3</v>
@@ -4435,7 +4473,7 @@
         <v>154</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>317</v>
+        <v>709</v>
       </c>
       <c r="G32" s="25" t="s">
         <v>73</v>
@@ -4444,7 +4482,7 @@
         <v>42</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
@@ -4455,24 +4493,26 @@
         <v>77</v>
       </c>
       <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
+      <c r="O32" s="25" t="s">
+        <v>583</v>
+      </c>
       <c r="P32" s="25" t="s">
-        <v>463</v>
+        <v>200</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25" t="s">
         <v>150</v>
       </c>
       <c r="S32" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
-        <v>53</v>
+        <v>467</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>3</v>
@@ -4481,7 +4521,7 @@
         <v>154</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>490</v>
+        <v>317</v>
       </c>
       <c r="G33" s="25" t="s">
         <v>73</v>
@@ -4503,66 +4543,72 @@
       <c r="N33" s="25"/>
       <c r="O33" s="25"/>
       <c r="P33" s="25" t="s">
-        <v>201</v>
+        <v>463</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="2:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="E34" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="25"/>
+        <v>154</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>490</v>
+      </c>
       <c r="G34" s="25" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="I34" s="25"/>
+        <v>42</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
       <c r="L34" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25" t="s">
-        <v>478</v>
-      </c>
+      <c r="M34" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="N34" s="25"/>
       <c r="O34" s="25"/>
       <c r="P34" s="25" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="25" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="S34" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="25" t="s">
@@ -4581,26 +4627,24 @@
       <c r="N35" s="25" t="s">
         <v>478</v>
       </c>
-      <c r="O35" s="25" t="b">
-        <v>1</v>
-      </c>
+      <c r="O35" s="25"/>
       <c r="P35" s="25" t="s">
-        <v>314</v>
+        <v>87</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="25" t="s">
         <v>148</v>
       </c>
       <c r="S35" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B36" s="25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
@@ -4611,7 +4655,7 @@
         <v>3</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="I36" s="25"/>
       <c r="J36" s="25"/>
@@ -4621,30 +4665,32 @@
       </c>
       <c r="M36" s="25"/>
       <c r="N36" s="25" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="O36" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="P36" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="P36" s="25" t="s">
+        <v>314</v>
+      </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="25" t="s">
@@ -4653,9 +4699,7 @@
       <c r="H37" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I37" s="25" t="s">
-        <v>128</v>
-      </c>
+      <c r="I37" s="25"/>
       <c r="J37" s="25"/>
       <c r="K37" s="25"/>
       <c r="L37" s="25" t="s">
@@ -4663,26 +4707,26 @@
       </c>
       <c r="M37" s="25"/>
       <c r="N37" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25" t="s">
-        <v>129</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="O37" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="P37" s="25"/>
       <c r="Q37" s="25"/>
       <c r="R37" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S37" s="25" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="38" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
-        <v>468</v>
+        <v>126</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>469</v>
+        <v>127</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
@@ -4696,7 +4740,7 @@
         <v>43</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>470</v>
+        <v>128</v>
       </c>
       <c r="J38" s="25"/>
       <c r="K38" s="25"/>
@@ -4705,32 +4749,30 @@
       </c>
       <c r="M38" s="25"/>
       <c r="N38" s="25" t="s">
-        <v>477</v>
-      </c>
-      <c r="O38" s="25" t="s">
-        <v>471</v>
-      </c>
+        <v>476</v>
+      </c>
+      <c r="O38" s="25"/>
       <c r="P38" s="25" t="s">
-        <v>704</v>
+        <v>129</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="25" t="s">
-        <v>472</v>
+        <v>152</v>
       </c>
       <c r="S38" s="25" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="39" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="25" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="25" t="s">
-        <v>159</v>
+        <v>1</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25" t="s">
@@ -4748,23 +4790,29 @@
         <v>3</v>
       </c>
       <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="25"/>
+      <c r="N39" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="O39" s="25" t="s">
+        <v>471</v>
+      </c>
       <c r="P39" s="25" t="s">
-        <v>3</v>
+        <v>704</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="S39" s="25"/>
-    </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+      <c r="S39" s="25" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="25" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25" t="s">
@@ -4799,10 +4847,10 @@
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="25" t="s">
@@ -4835,41 +4883,79 @@
       </c>
       <c r="S41" s="25"/>
     </row>
-    <row r="43" spans="2:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
+        <v>486</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>488</v>
+      </c>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="S42" s="25"/>
+    </row>
+    <row r="44" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="B44" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C44" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25" t="s">
+      <c r="D44" s="25"/>
+      <c r="E44" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H43" s="25" t="s">
+      <c r="F44" s="25"/>
+      <c r="G44" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H44" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25" t="s">
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25" t="s">
         <v>475</v>
       </c>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25" t="s">
+      <c r="O44" s="25"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S43" s="25" t="s">
+      <c r="S44" s="25" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4902,16 +4988,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="42" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -4922,7 +5008,7 @@
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="24" t="s">
         <v>113</v>
       </c>
@@ -4931,7 +5017,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="24" t="s">
         <v>134</v>
       </c>
@@ -4940,7 +5026,7 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="24" t="s">
         <v>135</v>
       </c>
@@ -4949,13 +5035,13 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4984,12 +5070,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -5168,18 +5254,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="F3" s="53" t="s">
+      <c r="C3" s="53"/>
+      <c r="F3" s="52" t="s">
         <v>462</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="J3" s="53" t="s">
+      <c r="G3" s="53"/>
+      <c r="J3" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="54"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -5370,10 +5456,10 @@
       <c r="G14" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="J14" s="53" t="s">
+      <c r="J14" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="K14" s="54"/>
+      <c r="K14" s="53"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -6332,10 +6418,10 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="53" t="s">
+      <c r="B100" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="C100" s="54"/>
+      <c r="C100" s="53"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
@@ -6666,10 +6752,10 @@
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="53" t="s">
+      <c r="B144" s="52" t="s">
         <v>613</v>
       </c>
-      <c r="C144" s="54"/>
+      <c r="C144" s="53"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">

</xml_diff>

<commit_message>
EPBDS-2784 Fix endRequestDate description
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -2197,7 +2197,7 @@
     <t>&gt; startRequestDate</t>
   </si>
   <si>
-    <t>The last date when rules are available in production, so the requests can't be processed by these rules</t>
+    <t>The last date when rules are available in production, so the requests can not be processed by these rules</t>
   </si>
 </sst>
 </file>
@@ -2581,7 +2581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2665,29 +2665,35 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2728,10 +2734,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3052,7 +3055,7 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="41" t="s">
         <v>97</v>
       </c>
       <c r="D2" s="36"/>
@@ -3067,97 +3070,97 @@
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>104</v>
       </c>
       <c r="D9" s="36"/>
@@ -3172,67 +3175,67 @@
       <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="35" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="36"/>
@@ -3244,20 +3247,26 @@
       <c r="J14" s="36"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3266,12 +3275,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3281,10 +3284,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3315,7 +3318,7 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="41" t="s">
         <v>97</v>
       </c>
       <c r="D1" s="36"/>
@@ -3333,115 +3336,115 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
     </row>
     <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="40" t="s">
         <v>104</v>
       </c>
       <c r="D8" s="36"/>
@@ -3459,19 +3462,19 @@
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
     </row>
     <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
@@ -3486,26 +3489,26 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
     </row>
     <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
@@ -3892,98 +3895,98 @@
       </c>
     </row>
     <row r="20" spans="2:19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="33" t="s">
         <v>707</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="33" t="s">
         <v>708</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="54" t="s">
+      <c r="F20" s="33" t="s">
         <v>710</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="54" t="s">
+      <c r="H20" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="54" t="s">
+      <c r="I20" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="M20" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="54" t="s">
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33" t="s">
         <v>711</v>
       </c>
-      <c r="Q20" s="54" t="s">
+      <c r="Q20" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R20" s="54" t="s">
+      <c r="R20" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="S20" s="54" t="s">
+      <c r="S20" s="33" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="21" spans="2:19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="33" t="s">
         <v>713</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="33" t="s">
         <v>714</v>
       </c>
-      <c r="D21" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="54" t="s">
+      <c r="D21" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="33" t="s">
         <v>715</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="54" t="s">
+      <c r="H21" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="54" t="s">
+      <c r="I21" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="M21" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54" t="s">
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33" t="s">
         <v>716</v>
       </c>
-      <c r="Q21" s="54" t="s">
+      <c r="Q21" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R21" s="54" t="s">
+      <c r="R21" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="S21" s="54" t="s">
+      <c r="S21" s="56" t="s">
         <v>717</v>
       </c>
     </row>
@@ -4988,16 +4991,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="44" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5008,7 +5011,7 @@
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="24" t="s">
         <v>113</v>
       </c>
@@ -5017,7 +5020,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="24" t="s">
         <v>134</v>
       </c>
@@ -5026,7 +5029,7 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="24" t="s">
         <v>135</v>
       </c>
@@ -5035,13 +5038,13 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="43" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5070,12 +5073,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -5254,18 +5257,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="F3" s="52" t="s">
+      <c r="C3" s="55"/>
+      <c r="F3" s="54" t="s">
         <v>462</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="J3" s="52" t="s">
+      <c r="G3" s="55"/>
+      <c r="J3" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="53"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -5456,10 +5459,10 @@
       <c r="G14" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="J14" s="52" t="s">
+      <c r="J14" s="54" t="s">
         <v>461</v>
       </c>
-      <c r="K14" s="53"/>
+      <c r="K14" s="55"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -6418,10 +6421,10 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="52" t="s">
+      <c r="B100" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="C100" s="53"/>
+      <c r="C100" s="55"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
@@ -6752,10 +6755,10 @@
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="52" t="s">
+      <c r="B144" s="54" t="s">
         <v>613</v>
       </c>
-      <c r="C144" s="53"/>
+      <c r="C144" s="55"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">

</xml_diff>

<commit_message>
EPBDS-2781 Remove default values for Currency and Language properties
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="718">
   <si>
     <t>name</t>
   </si>
@@ -2671,14 +2671,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2686,14 +2680,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2733,9 +2736,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3055,218 +3055,212 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3275,6 +3269,12 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3284,10 +3284,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="S22" sqref="S22"/>
+      <selection pane="bottomLeft" activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,163 +3318,163 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
     </row>
     <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
     </row>
     <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
     </row>
     <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
@@ -3489,26 +3489,26 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
     </row>
     <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
@@ -3986,7 +3986,7 @@
       <c r="R21" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="S21" s="56" t="s">
+      <c r="S21" s="35" t="s">
         <v>717</v>
       </c>
     </row>
@@ -4448,9 +4448,7 @@
         <v>77</v>
       </c>
       <c r="N31" s="25"/>
-      <c r="O31" s="25" t="s">
-        <v>68</v>
-      </c>
+      <c r="O31" s="25"/>
       <c r="P31" s="25" t="s">
         <v>160</v>
       </c>
@@ -4496,9 +4494,7 @@
         <v>77</v>
       </c>
       <c r="N32" s="25"/>
-      <c r="O32" s="25" t="s">
-        <v>583</v>
-      </c>
+      <c r="O32" s="25"/>
       <c r="P32" s="25" t="s">
         <v>200</v>
       </c>
@@ -4991,16 +4987,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="45" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5011,7 +5007,7 @@
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="24" t="s">
         <v>113</v>
       </c>
@@ -5020,7 +5016,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="24" t="s">
         <v>134</v>
       </c>
@@ -5029,7 +5025,7 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="24" t="s">
         <v>135</v>
       </c>
@@ -5038,13 +5034,13 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
-      <c r="C10" s="45" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5073,12 +5069,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -5257,18 +5253,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="F3" s="54" t="s">
+      <c r="C3" s="56"/>
+      <c r="F3" s="55" t="s">
         <v>462</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="56"/>
+      <c r="J3" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -5459,10 +5455,10 @@
       <c r="G14" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="J14" s="54" t="s">
+      <c r="J14" s="55" t="s">
         <v>461</v>
       </c>
-      <c r="K14" s="55"/>
+      <c r="K14" s="56"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -6421,10 +6417,10 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="54" t="s">
+      <c r="B100" s="55" t="s">
         <v>187</v>
       </c>
-      <c r="C100" s="55"/>
+      <c r="C100" s="56"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
@@ -6755,10 +6751,10 @@
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="54" t="s">
+      <c r="B144" s="55" t="s">
         <v>613</v>
       </c>
-      <c r="C144" s="55"/>
+      <c r="C144" s="56"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">

</xml_diff>

<commit_message>
EPBDS Property "id" is moved from Info to Dev section.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="5" r:id="rId1"/>
@@ -2686,29 +2686,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3051,9 +3051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:J12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3065,52 +3063,52 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="43" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="42"/>
@@ -3125,46 +3123,46 @@
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1">
       <c r="B9" s="3" t="s">
@@ -3173,13 +3171,13 @@
       <c r="C9" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1">
       <c r="B10" s="3" t="s">
@@ -3200,7 +3198,7 @@
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="43" t="s">
         <v>719</v>
       </c>
       <c r="D11" s="42"/>
@@ -3215,7 +3213,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="37" t="s">
         <v>118</v>
       </c>
       <c r="D12" s="42"/>
@@ -3230,7 +3228,7 @@
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="37" t="s">
         <v>105</v>
       </c>
       <c r="D13" s="42"/>
@@ -3245,32 +3243,38 @@
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3279,12 +3283,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3294,10 +3292,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3328,61 +3326,61 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
     </row>
     <row r="3" spans="2:19" ht="57.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="43" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="42"/>
@@ -3400,55 +3398,55 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
     </row>
     <row r="7" spans="2:19" ht="42.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1">
       <c r="B8" s="3" t="s">
@@ -3457,16 +3455,16 @@
       <c r="C8" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
     </row>
     <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="B9" s="3" t="s">
@@ -3650,7 +3648,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I14" s="25" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
EPBDS-2984 Added attribute 'errorSeverity' to TablePropertyDefinitions. Update UniquePropertyValueValidator to create errors according to errorSeverity.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="730">
   <si>
     <t>name</t>
   </si>
@@ -2222,6 +2222,18 @@
   </si>
   <si>
     <t>min(endRequestDate)</t>
+  </si>
+  <si>
+    <t>errorSeverity</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Error Severity</t>
+  </si>
+  <si>
+    <t>WARN</t>
   </si>
 </sst>
 </file>
@@ -2605,7 +2617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2704,14 +2716,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2719,14 +2725,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3097,218 +3112,212 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="41" t="s">
         <v>715</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3317,6 +3326,12 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3324,12 +3339,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S53"/>
+  <dimension ref="B1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomLeft" activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3350,175 +3365,182 @@
     <col min="14" max="14" width="22" style="1" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" style="1" customWidth="1"/>
     <col min="16" max="16" width="19.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="38" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="17" width="19.140625" style="38" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="38" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-    </row>
-    <row r="2" spans="2:19" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="Q1" s="38"/>
+    </row>
+    <row r="2" spans="2:20" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-    </row>
-    <row r="3" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="Q2" s="38"/>
+    </row>
+    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-    </row>
-    <row r="4" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+    </row>
+    <row r="4" spans="2:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-    </row>
-    <row r="5" spans="2:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="Q4" s="38"/>
+    </row>
+    <row r="5" spans="2:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-    </row>
-    <row r="6" spans="2:19" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="Q5" s="38"/>
+    </row>
+    <row r="6" spans="2:20" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-    </row>
-    <row r="7" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="Q6" s="38"/>
+    </row>
+    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-    </row>
-    <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+    </row>
+    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-    </row>
-    <row r="9" spans="2:19" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+    </row>
+    <row r="9" spans="2:20" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-    </row>
-    <row r="10" spans="2:19" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="Q9" s="38"/>
+    </row>
+    <row r="10" spans="2:20" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3529,30 +3551,32 @@
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="Q10" s="38"/>
+    </row>
+    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-    </row>
-    <row r="12" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+    </row>
+    <row r="12" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
@@ -3599,16 +3623,19 @@
         <v>13</v>
       </c>
       <c r="Q12" s="14" t="s">
+        <v>726</v>
+      </c>
+      <c r="R12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="14" t="s">
+      <c r="S12" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="S12" s="14" t="s">
+      <c r="T12" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>29</v>
       </c>
@@ -3655,16 +3682,19 @@
         <v>31</v>
       </c>
       <c r="Q13" s="14" t="s">
+        <v>728</v>
+      </c>
+      <c r="R13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R13" s="14" t="s">
+      <c r="S13" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="S13" s="14" t="s">
+      <c r="T13" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>11</v>
       </c>
@@ -3700,15 +3730,18 @@
       <c r="P14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25" t="s">
+      <c r="Q14" s="25" t="s">
+        <v>729</v>
+      </c>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S14" s="25" t="s">
+      <c r="T14" s="25" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
@@ -3745,14 +3778,15 @@
         <v>3</v>
       </c>
       <c r="Q15" s="25"/>
-      <c r="R15" s="25" t="s">
+      <c r="R15" s="25"/>
+      <c r="S15" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="S15" s="25" t="s">
+      <c r="T15" s="25" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="2:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>35</v>
       </c>
@@ -3789,14 +3823,15 @@
         <v>3</v>
       </c>
       <c r="Q16" s="25"/>
-      <c r="R16" s="25" t="s">
+      <c r="R16" s="25"/>
+      <c r="S16" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S16" s="25" t="s">
+      <c r="T16" s="25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>21</v>
       </c>
@@ -3833,14 +3868,15 @@
         <v>3</v>
       </c>
       <c r="Q17" s="25"/>
-      <c r="R17" s="25" t="s">
+      <c r="R17" s="25"/>
+      <c r="S17" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S17" s="25" t="s">
+      <c r="T17" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" ht="90" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>314</v>
       </c>
@@ -3878,17 +3914,18 @@
       <c r="P18" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="R18" s="25" t="s">
+      <c r="S18" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S18" s="25" t="s">
+      <c r="T18" s="25" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>313</v>
       </c>
@@ -3926,17 +3963,18 @@
       <c r="P19" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="Q19" s="25" t="s">
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="R19" s="25" t="s">
+      <c r="S19" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S19" s="25" t="s">
+      <c r="T19" s="25" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="2:19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
         <v>704</v>
       </c>
@@ -3974,17 +4012,18 @@
       <c r="P20" s="33" t="s">
         <v>707</v>
       </c>
-      <c r="Q20" s="33" t="s">
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="R20" s="33" t="s">
+      <c r="S20" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="S20" s="33" t="s">
+      <c r="T20" s="33" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="21" spans="2:19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="33" t="s">
         <v>709</v>
       </c>
@@ -4022,17 +4061,18 @@
       <c r="P21" s="33" t="s">
         <v>711</v>
       </c>
-      <c r="Q21" s="33" t="s">
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="R21" s="33" t="s">
+      <c r="S21" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="S21" s="35" t="s">
+      <c r="T21" s="35" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
         <v>22</v>
       </c>
@@ -4073,14 +4113,15 @@
         <v>3</v>
       </c>
       <c r="Q22" s="25"/>
-      <c r="R22" s="25" t="s">
+      <c r="R22" s="25"/>
+      <c r="S22" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S22" s="25" t="s">
+      <c r="T22" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>23</v>
       </c>
@@ -4120,17 +4161,18 @@
       <c r="P23" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q23" s="25" t="s">
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="R23" s="25" t="s">
+      <c r="S23" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S23" s="25" t="s">
+      <c r="T23" s="25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
@@ -4171,14 +4213,15 @@
         <v>3</v>
       </c>
       <c r="Q24" s="25"/>
-      <c r="R24" s="25" t="s">
+      <c r="R24" s="25"/>
+      <c r="S24" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S24" s="25" t="s">
+      <c r="T24" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
         <v>25</v>
       </c>
@@ -4218,17 +4261,18 @@
       <c r="P25" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="R25" s="25" t="s">
+      <c r="S25" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S25" s="25" t="s">
+      <c r="T25" s="25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:19" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
         <v>220</v>
       </c>
@@ -4266,15 +4310,18 @@
       <c r="P26" s="25" t="s">
         <v>716</v>
       </c>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25" t="s">
+      <c r="Q26" s="25" t="s">
+        <v>727</v>
+      </c>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S26" s="25" t="s">
+      <c r="T26" s="25" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
         <v>26</v>
       </c>
@@ -4311,14 +4358,15 @@
         <v>27</v>
       </c>
       <c r="Q27" s="25"/>
-      <c r="R27" s="25" t="s">
+      <c r="R27" s="25"/>
+      <c r="S27" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S27" s="25" t="s">
+      <c r="T27" s="25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
         <v>722</v>
       </c>
@@ -4357,14 +4405,15 @@
         <v>44</v>
       </c>
       <c r="Q28" s="25"/>
-      <c r="R28" s="25" t="s">
+      <c r="R28" s="25"/>
+      <c r="S28" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S28" s="25" t="s">
+      <c r="T28" s="25" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
         <v>48</v>
       </c>
@@ -4403,14 +4452,15 @@
         <v>50</v>
       </c>
       <c r="Q29" s="25"/>
-      <c r="R29" s="25" t="s">
+      <c r="R29" s="25"/>
+      <c r="S29" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S29" s="25" t="s">
+      <c r="T29" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
         <v>53</v>
       </c>
@@ -4449,14 +4499,15 @@
         <v>462</v>
       </c>
       <c r="Q30" s="25"/>
-      <c r="R30" s="25" t="s">
+      <c r="R30" s="25"/>
+      <c r="S30" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S30" s="25" t="s">
+      <c r="T30" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
         <v>464</v>
       </c>
@@ -4495,14 +4546,15 @@
         <v>154</v>
       </c>
       <c r="Q31" s="25"/>
-      <c r="R31" s="25" t="s">
+      <c r="R31" s="25"/>
+      <c r="S31" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S31" s="25" t="s">
+      <c r="T31" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
         <v>55</v>
       </c>
@@ -4541,14 +4593,15 @@
         <v>158</v>
       </c>
       <c r="Q32" s="25"/>
-      <c r="R32" s="25" t="s">
+      <c r="R32" s="25"/>
+      <c r="S32" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S32" s="25" t="s">
+      <c r="T32" s="25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>56</v>
       </c>
@@ -4587,14 +4640,15 @@
         <v>198</v>
       </c>
       <c r="Q33" s="25"/>
-      <c r="R33" s="25" t="s">
+      <c r="R33" s="25"/>
+      <c r="S33" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S33" s="25" t="s">
+      <c r="T33" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
         <v>465</v>
       </c>
@@ -4633,14 +4687,15 @@
         <v>461</v>
       </c>
       <c r="Q34" s="25"/>
-      <c r="R34" s="25" t="s">
+      <c r="R34" s="25"/>
+      <c r="S34" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S34" s="25" t="s">
+      <c r="T34" s="25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="2:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" ht="105" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
         <v>52</v>
       </c>
@@ -4679,14 +4734,15 @@
         <v>199</v>
       </c>
       <c r="Q35" s="25"/>
-      <c r="R35" s="25" t="s">
+      <c r="R35" s="25"/>
+      <c r="S35" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="S35" s="25" t="s">
+      <c r="T35" s="25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="2:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="25" t="s">
         <v>82</v>
       </c>
@@ -4719,14 +4775,15 @@
         <v>86</v>
       </c>
       <c r="Q36" s="25"/>
-      <c r="R36" s="25" t="s">
+      <c r="R36" s="25"/>
+      <c r="S36" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S36" s="25" t="s">
+      <c r="T36" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" ht="75" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
         <v>84</v>
       </c>
@@ -4761,14 +4818,15 @@
         <v>312</v>
       </c>
       <c r="Q37" s="25"/>
-      <c r="R37" s="25" t="s">
+      <c r="R37" s="25"/>
+      <c r="S37" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S37" s="25" t="s">
+      <c r="T37" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
         <v>89</v>
       </c>
@@ -4801,14 +4859,15 @@
       </c>
       <c r="P38" s="25"/>
       <c r="Q38" s="25"/>
-      <c r="R38" s="25" t="s">
+      <c r="R38" s="25"/>
+      <c r="S38" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="S38" s="25" t="s">
+      <c r="T38" s="25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="25" t="s">
         <v>124</v>
       </c>
@@ -4843,14 +4902,15 @@
         <v>127</v>
       </c>
       <c r="Q39" s="25"/>
-      <c r="R39" s="25" t="s">
+      <c r="R39" s="25"/>
+      <c r="S39" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="S39" s="25" t="s">
+      <c r="T39" s="25" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="40" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="25" t="s">
         <v>723</v>
       </c>
@@ -4887,14 +4947,15 @@
         <v>701</v>
       </c>
       <c r="Q40" s="25"/>
-      <c r="R40" s="25" t="s">
+      <c r="R40" s="25"/>
+      <c r="S40" s="25" t="s">
         <v>469</v>
       </c>
-      <c r="S40" s="25" t="s">
+      <c r="T40" s="25" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="41" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
         <v>481</v>
       </c>
@@ -4927,12 +4988,13 @@
         <v>3</v>
       </c>
       <c r="Q41" s="25"/>
-      <c r="R41" s="25" t="s">
+      <c r="R41" s="25"/>
+      <c r="S41" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S41" s="25"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T41" s="25"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
         <v>482</v>
       </c>
@@ -4965,12 +5027,13 @@
         <v>3</v>
       </c>
       <c r="Q42" s="25"/>
-      <c r="R42" s="25" t="s">
+      <c r="R42" s="25"/>
+      <c r="S42" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S42" s="25"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T42" s="25"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="25" t="s">
         <v>483</v>
       </c>
@@ -5003,12 +5066,13 @@
         <v>3</v>
       </c>
       <c r="Q43" s="25"/>
-      <c r="R43" s="25" t="s">
+      <c r="R43" s="25"/>
+      <c r="S43" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S43" s="25"/>
-    </row>
-    <row r="45" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="T43" s="25"/>
+    </row>
+    <row r="45" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
         <v>90</v>
       </c>
@@ -5039,60 +5103,63 @@
       <c r="O45" s="25"/>
       <c r="P45" s="25"/>
       <c r="Q45" s="25"/>
-      <c r="R45" s="25" t="s">
+      <c r="R45" s="25"/>
+      <c r="S45" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="S45" s="25" t="s">
+      <c r="T45" s="25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="46" t="s">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="47" t="s">
         <v>718</v>
       </c>
-      <c r="C49" s="46"/>
-    </row>
-    <row r="50" spans="2:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="49" t="s">
+      <c r="C49" s="47"/>
+    </row>
+    <row r="50" spans="2:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="50" t="s">
         <v>719</v>
       </c>
-      <c r="C50" s="50"/>
-    </row>
-    <row r="51" spans="2:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="49" t="s">
+      <c r="C50" s="51"/>
+      <c r="Q50" s="38"/>
+    </row>
+    <row r="51" spans="2:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="50" t="s">
         <v>717</v>
       </c>
-      <c r="C51" s="50"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="47" t="s">
+      <c r="C51" s="51"/>
+      <c r="Q51" s="38"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" s="48" t="s">
         <v>724</v>
       </c>
-      <c r="C52" s="48"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="47" t="s">
+      <c r="C52" s="49"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="48" t="s">
         <v>725</v>
       </c>
-      <c r="C53" s="48"/>
+      <c r="C53" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
     <mergeCell ref="C1:M1"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="C4:M4"/>
     <mergeCell ref="C5:M5"/>
-    <mergeCell ref="B11:S11"/>
+    <mergeCell ref="B11:T11"/>
     <mergeCell ref="C8:M8"/>
     <mergeCell ref="C9:M9"/>
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="C6:M6"/>
     <mergeCell ref="C7:M7"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -5110,16 +5177,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="58"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>108</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5130,7 +5197,7 @@
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="51"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="24" t="s">
         <v>111</v>
       </c>
@@ -5139,7 +5206,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="24" t="s">
         <v>132</v>
       </c>
@@ -5148,7 +5215,7 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="51"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="24" t="s">
         <v>133</v>
       </c>
@@ -5157,13 +5224,13 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="52" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5192,12 +5259,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -5377,18 +5444,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="F3" s="61" t="s">
+      <c r="C3" s="63"/>
+      <c r="F3" s="62" t="s">
         <v>460</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="J3" s="61" t="s">
+      <c r="G3" s="63"/>
+      <c r="J3" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="K3" s="62"/>
+      <c r="K3" s="63"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -5579,10 +5646,10 @@
       <c r="G14" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="J14" s="61" t="s">
+      <c r="J14" s="62" t="s">
         <v>459</v>
       </c>
-      <c r="K14" s="62"/>
+      <c r="K14" s="63"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -6541,10 +6608,10 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="61" t="s">
+      <c r="B100" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="C100" s="62"/>
+      <c r="C100" s="63"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
@@ -6875,10 +6942,10 @@
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="61" t="s">
+      <c r="B144" s="62" t="s">
         <v>610</v>
       </c>
-      <c r="C144" s="62"/>
+      <c r="C144" s="63"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">

</xml_diff>

<commit_message>
fix bug: Property 'failOnMiss' can`t be defined in table of type 'xls.properties' (Hollard_Motor_Test fails)
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -2725,29 +2725,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2802,7 +2802,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2816,9 +2816,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2856,7 +2856,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2928,7 +2928,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3118,52 +3118,52 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>99</v>
       </c>
       <c r="D5" s="44"/>
@@ -3178,46 +3178,46 @@
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -3226,13 +3226,13 @@
       <c r="C9" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -3253,7 +3253,7 @@
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="45" t="s">
         <v>712</v>
       </c>
       <c r="D11" s="44"/>
@@ -3268,7 +3268,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="39" t="s">
         <v>117</v>
       </c>
       <c r="D12" s="44"/>
@@ -3283,7 +3283,7 @@
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="39" t="s">
         <v>104</v>
       </c>
       <c r="D13" s="44"/>
@@ -3298,32 +3298,38 @@
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3332,12 +3338,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3347,10 +3347,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="S35" sqref="S35"/>
+      <selection pane="bottomLeft" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,63 +3382,63 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
       <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="2:20" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
       <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
     </row>
     <row r="4" spans="2:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="45" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="44"/>
@@ -3457,57 +3457,57 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
       <c r="Q5" s="38"/>
     </row>
     <row r="6" spans="2:20" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -3516,16 +3516,16 @@
       <c r="C8" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
     </row>
     <row r="9" spans="2:20" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="M38" s="25"/>
       <c r="N38" s="25" t="s">
-        <v>471</v>
+        <v>729</v>
       </c>
       <c r="O38" s="25" t="b">
         <v>0</v>
@@ -5151,11 +5151,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
     <mergeCell ref="C1:M1"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="C4:M4"/>
@@ -5166,6 +5161,11 @@
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="C6:M6"/>
     <mergeCell ref="C7:M7"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Cache method invocation funtionality with tests.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="15270" windowHeight="8145" activeTab="1"/>
@@ -13,12 +13,12 @@
     <sheet name="Runtime Scope" sheetId="3" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcMode="manual" iterate="1" iterateCount="1000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="734">
   <si>
     <t>name</t>
   </si>
@@ -2237,6 +2237,15 @@
   </si>
   <si>
     <t>removed</t>
+  </si>
+  <si>
+    <t>cacheable</t>
+  </si>
+  <si>
+    <t>Cacheable</t>
+  </si>
+  <si>
+    <t>Is method use cache by input arguments, if cache is enabled.</t>
   </si>
 </sst>
 </file>
@@ -2620,7 +2629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2725,29 +2734,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3118,212 +3130,218 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="47" t="s">
         <v>708</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3332,12 +3350,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3345,12 +3357,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T53"/>
+  <dimension ref="B1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomLeft" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,18 +3394,18 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
       <c r="P1" s="38"/>
       <c r="R1" s="39"/>
     </row>
@@ -3401,18 +3413,18 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
       <c r="P2" s="38"/>
       <c r="R2" s="39"/>
     </row>
@@ -3420,35 +3432,35 @@
       <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="2:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="P4" s="38"/>
       <c r="R4" s="39"/>
     </row>
@@ -3456,18 +3468,18 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
       <c r="P5" s="38"/>
       <c r="R5" s="39"/>
     </row>
@@ -3475,18 +3487,18 @@
       <c r="B6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
       <c r="P6" s="38"/>
       <c r="R6" s="39"/>
     </row>
@@ -3494,52 +3506,52 @@
       <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="2:20" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
       <c r="P9" s="38"/>
       <c r="R9" s="39"/>
     </row>
@@ -3558,27 +3570,27 @@
       <c r="R10" s="39"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
     </row>
     <row r="12" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
@@ -5024,86 +5036,120 @@
       </c>
       <c r="T43" s="25"/>
     </row>
-    <row r="45" spans="2:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="B45" s="25" t="s">
+    <row r="44" spans="2:20" s="40" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="25" t="s">
+        <v>732</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H44" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="T44" s="25" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C46" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25" t="s">
+      <c r="D46" s="25"/>
+      <c r="E46" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" s="25" t="s">
+      <c r="F46" s="25"/>
+      <c r="G46" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H46" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25" t="s">
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25" t="s">
         <v>467</v>
       </c>
-      <c r="N45" s="25"/>
-      <c r="O45" s="25"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25" t="s">
+      <c r="N46" s="25"/>
+      <c r="O46" s="25"/>
+      <c r="P46" s="25"/>
+      <c r="Q46" s="25"/>
+      <c r="R46" s="25"/>
+      <c r="S46" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="T45" s="25" t="s">
+      <c r="T46" s="25" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B49" s="48" t="s">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" s="49" t="s">
         <v>711</v>
       </c>
-      <c r="C49" s="48"/>
-    </row>
-    <row r="50" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="51" t="s">
+      <c r="C50" s="49"/>
+    </row>
+    <row r="51" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="52" t="s">
         <v>712</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="P50" s="38"/>
-      <c r="R50" s="39"/>
-    </row>
-    <row r="51" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="51" t="s">
-        <v>710</v>
-      </c>
-      <c r="C51" s="52"/>
+      <c r="C51" s="53"/>
       <c r="P51" s="38"/>
       <c r="R51" s="39"/>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="49" t="s">
+    <row r="52" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="52" t="s">
+        <v>710</v>
+      </c>
+      <c r="C52" s="53"/>
+      <c r="P52" s="38"/>
+      <c r="R52" s="39"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" s="50" t="s">
         <v>717</v>
       </c>
-      <c r="C52" s="50"/>
-    </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="49" t="s">
+      <c r="C53" s="51"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" s="50" t="s">
         <v>718</v>
       </c>
-      <c r="C53" s="50"/>
+      <c r="C54" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C4:L4"/>
@@ -5114,6 +5160,11 @@
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C6:L6"/>
     <mergeCell ref="C7:L7"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -5131,16 +5182,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="54" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5151,7 +5202,7 @@
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="53"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="24" t="s">
         <v>109</v>
       </c>
@@ -5160,7 +5211,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="53"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="24" t="s">
         <v>129</v>
       </c>
@@ -5169,7 +5220,7 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="53"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="24" t="s">
         <v>130</v>
       </c>
@@ -5178,13 +5229,13 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="53"/>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5213,12 +5264,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -5398,18 +5449,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="F3" s="63" t="s">
+      <c r="C3" s="65"/>
+      <c r="F3" s="64" t="s">
         <v>456</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="J3" s="63" t="s">
+      <c r="G3" s="65"/>
+      <c r="J3" s="64" t="s">
         <v>196</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -5600,10 +5651,10 @@
       <c r="G14" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="J14" s="63" t="s">
+      <c r="J14" s="64" t="s">
         <v>455</v>
       </c>
-      <c r="K14" s="64"/>
+      <c r="K14" s="65"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -6562,10 +6613,10 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="63" t="s">
+      <c r="B100" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="C100" s="64"/>
+      <c r="C100" s="65"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
@@ -6896,10 +6947,10 @@
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="63" t="s">
+      <c r="B144" s="64" t="s">
         <v>604</v>
       </c>
-      <c r="C144" s="64"/>
+      <c r="C144" s="65"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">

</xml_diff>

<commit_message>
Variations support was added.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="737">
   <si>
     <t>name</t>
   </si>
@@ -2246,6 +2246,15 @@
   </si>
   <si>
     <t>Is method use cache by input arguments, if cache is enabled.</t>
+  </si>
+  <si>
+    <t>Recalculation</t>
+  </si>
+  <si>
+    <t>recalculation</t>
+  </si>
+  <si>
+    <t>Recalculation types for partial calculation feature</t>
   </si>
 </sst>
 </file>
@@ -2629,7 +2638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2737,14 +2746,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2752,14 +2755,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3130,218 +3142,212 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="44" t="s">
         <v>708</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3350,6 +3356,12 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3357,21 +3369,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T54"/>
+  <dimension ref="B1:T55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="S38" sqref="S38"/>
+      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
@@ -3394,18 +3406,18 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
       <c r="P1" s="38"/>
       <c r="R1" s="39"/>
     </row>
@@ -3413,18 +3425,18 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
       <c r="P2" s="38"/>
       <c r="R2" s="39"/>
     </row>
@@ -3432,35 +3444,35 @@
       <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
     </row>
     <row r="4" spans="2:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
       <c r="P4" s="38"/>
       <c r="R4" s="39"/>
     </row>
@@ -3468,18 +3480,18 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
       <c r="P5" s="38"/>
       <c r="R5" s="39"/>
     </row>
@@ -3487,18 +3499,18 @@
       <c r="B6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
       <c r="P6" s="38"/>
       <c r="R6" s="39"/>
     </row>
@@ -3506,52 +3518,52 @@
       <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
     </row>
     <row r="9" spans="2:20" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
       <c r="P9" s="38"/>
       <c r="R9" s="39"/>
     </row>
@@ -3570,27 +3582,27 @@
       <c r="R10" s="39"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
     </row>
     <row r="12" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
@@ -4925,7 +4937,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
         <v>475</v>
       </c>
@@ -5036,7 +5048,7 @@
       </c>
       <c r="T43" s="25"/>
     </row>
-    <row r="44" spans="2:20" s="40" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" s="40" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="25" t="s">
         <v>732</v>
       </c>
@@ -5075,81 +5087,125 @@
         <v>733</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="25" t="s">
+    <row r="45" spans="2:20" s="41" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
+        <v>734</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>734</v>
+      </c>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
+      <c r="P45" s="25"/>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="T45" s="25" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C47" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25" t="s">
+      <c r="D47" s="25"/>
+      <c r="E47" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H46" s="25" t="s">
+      <c r="F47" s="25"/>
+      <c r="G47" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25" t="s">
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25" t="s">
         <v>467</v>
       </c>
-      <c r="N46" s="25"/>
-      <c r="O46" s="25"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25" t="s">
+      <c r="N47" s="25"/>
+      <c r="O47" s="25"/>
+      <c r="P47" s="25"/>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="25"/>
+      <c r="S47" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="T46" s="25" t="s">
+      <c r="T47" s="25" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B50" s="49" t="s">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B51" s="50" t="s">
         <v>711</v>
       </c>
-      <c r="C50" s="49"/>
-    </row>
-    <row r="51" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="52" t="s">
+      <c r="C51" s="50"/>
+    </row>
+    <row r="52" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="53" t="s">
         <v>712</v>
       </c>
-      <c r="C51" s="53"/>
-      <c r="P51" s="38"/>
-      <c r="R51" s="39"/>
-    </row>
-    <row r="52" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="52" t="s">
-        <v>710</v>
-      </c>
-      <c r="C52" s="53"/>
+      <c r="C52" s="54"/>
       <c r="P52" s="38"/>
       <c r="R52" s="39"/>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="50" t="s">
+    <row r="53" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="53" t="s">
+        <v>710</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="P53" s="38"/>
+      <c r="R53" s="39"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" s="51" t="s">
         <v>717</v>
       </c>
-      <c r="C53" s="51"/>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="50" t="s">
+      <c r="C54" s="52"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" s="51" t="s">
         <v>718</v>
       </c>
-      <c r="C54" s="51"/>
+      <c r="C55" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C4:L4"/>
@@ -5160,11 +5216,6 @@
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C6:L6"/>
     <mergeCell ref="C7:L7"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -5176,22 +5227,22 @@
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:F9"/>
+      <selection activeCell="C10" sqref="C10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="55" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5202,7 +5253,7 @@
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="24" t="s">
         <v>109</v>
       </c>
@@ -5211,7 +5262,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="24" t="s">
         <v>129</v>
       </c>
@@ -5220,7 +5271,7 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="24" t="s">
         <v>130</v>
       </c>
@@ -5229,13 +5280,13 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5264,12 +5315,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -5433,7 +5484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K216"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
@@ -5449,18 +5500,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="F3" s="64" t="s">
+      <c r="C3" s="66"/>
+      <c r="F3" s="65" t="s">
         <v>456</v>
       </c>
-      <c r="G3" s="65"/>
-      <c r="J3" s="64" t="s">
+      <c r="G3" s="66"/>
+      <c r="J3" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="K3" s="65"/>
+      <c r="K3" s="66"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -5651,10 +5702,10 @@
       <c r="G14" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="J14" s="64" t="s">
+      <c r="J14" s="65" t="s">
         <v>455</v>
       </c>
-      <c r="K14" s="65"/>
+      <c r="K14" s="66"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -6613,10 +6664,10 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="64" t="s">
+      <c r="B100" s="65" t="s">
         <v>181</v>
       </c>
-      <c r="C100" s="65"/>
+      <c r="C100" s="66"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
@@ -6947,10 +6998,10 @@
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="64" t="s">
+      <c r="B144" s="65" t="s">
         <v>604</v>
       </c>
-      <c r="C144" s="65"/>
+      <c r="C144" s="66"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="6" t="s">

</xml_diff>

<commit_message>
Recalculation property was renamed to recalculate. Type of property in TableDefenition.xls was changed.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -13,12 +13,12 @@
     <sheet name="Runtime Scope" sheetId="3" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="145621" calcMode="manual" iterate="1" iterateCount="1000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="745">
   <si>
     <t>name</t>
   </si>
@@ -2248,13 +2248,37 @@
     <t>Is method use cache by input arguments, if cache is enabled.</t>
   </si>
   <si>
-    <t>Recalculation</t>
-  </si>
-  <si>
-    <t>recalculation</t>
-  </si>
-  <si>
     <t>Recalculation types for partial calculation feature</t>
+  </si>
+  <si>
+    <t>Data EnumPropertyDefinition recalculate</t>
+  </si>
+  <si>
+    <t>ALWAYS</t>
+  </si>
+  <si>
+    <t>NEVER</t>
+  </si>
+  <si>
+    <t>ANALYZE</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>Analyze</t>
+  </si>
+  <si>
+    <t>data: recalculate</t>
+  </si>
+  <si>
+    <t>recalculate</t>
+  </si>
+  <si>
+    <t>Recalculate</t>
   </si>
 </sst>
 </file>
@@ -2390,7 +2414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2633,12 +2657,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2749,29 +2799,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2824,6 +2874,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3142,52 +3194,52 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="48" t="s">
         <v>97</v>
       </c>
       <c r="D5" s="47"/>
@@ -3202,46 +3254,46 @@
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -3250,13 +3302,13 @@
       <c r="C9" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -3277,7 +3329,7 @@
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="48" t="s">
         <v>708</v>
       </c>
       <c r="D11" s="47"/>
@@ -3292,7 +3344,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="42" t="s">
         <v>115</v>
       </c>
       <c r="D12" s="47"/>
@@ -3307,7 +3359,7 @@
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="42" t="s">
         <v>102</v>
       </c>
       <c r="D13" s="47"/>
@@ -3322,32 +3374,38 @@
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="C8:J8"/>
@@ -3356,12 +3414,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3371,10 +3423,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
-      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,18 +3458,18 @@
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="P1" s="38"/>
       <c r="R1" s="39"/>
     </row>
@@ -3425,18 +3477,18 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
       <c r="P2" s="38"/>
       <c r="R2" s="39"/>
     </row>
@@ -3444,24 +3496,24 @@
       <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
     </row>
     <row r="4" spans="2:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="48" t="s">
         <v>97</v>
       </c>
       <c r="D4" s="47"/>
@@ -3480,18 +3532,18 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
       <c r="P5" s="38"/>
       <c r="R5" s="39"/>
     </row>
@@ -3499,18 +3551,18 @@
       <c r="B6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
       <c r="P6" s="38"/>
       <c r="R6" s="39"/>
     </row>
@@ -3518,18 +3570,18 @@
       <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -3538,15 +3590,15 @@
       <c r="C8" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="2:20" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -5089,16 +5141,16 @@
     </row>
     <row r="45" spans="2:20" s="41" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>734</v>
+        <v>151</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25" t="s">
@@ -5115,7 +5167,9 @@
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
       <c r="N45" s="25"/>
-      <c r="O45" s="25"/>
+      <c r="O45" s="25" t="s">
+        <v>742</v>
+      </c>
       <c r="P45" s="25"/>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
@@ -5123,7 +5177,7 @@
         <v>145</v>
       </c>
       <c r="T45" s="25" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="47" spans="2:20" ht="45" x14ac:dyDescent="0.25">
@@ -5201,11 +5255,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C4:L4"/>
@@ -5216,6 +5265,11 @@
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C6:L6"/>
     <mergeCell ref="C7:L7"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -5484,8 +5538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5888,6 +5942,10 @@
       <c r="G24" s="9" t="s">
         <v>228</v>
       </c>
+      <c r="J24" s="65" t="s">
+        <v>735</v>
+      </c>
+      <c r="K24" s="66"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
@@ -5902,6 +5960,12 @@
       <c r="G25" s="9" t="s">
         <v>230</v>
       </c>
+      <c r="J25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
@@ -5916,6 +5980,12 @@
       <c r="G26" s="9" t="s">
         <v>232</v>
       </c>
+      <c r="J26" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
@@ -5930,6 +6000,12 @@
       <c r="G27" s="9" t="s">
         <v>234</v>
       </c>
+      <c r="J27" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
@@ -5944,6 +6020,12 @@
       <c r="G28" s="9" t="s">
         <v>236</v>
       </c>
+      <c r="J28" s="67" t="s">
+        <v>737</v>
+      </c>
+      <c r="K28" s="68" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
@@ -5957,6 +6039,12 @@
       </c>
       <c r="G29" s="9" t="s">
         <v>238</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -7583,13 +7671,14 @@
   <sortState ref="J16:K20">
     <sortCondition ref="J16"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B144:C144"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B100:C100"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-4648 [Precision] cannot use minus in the _res_.$ syntax: error displays EPBDS-4641 Add possibility to set precision property to the MODULE and CATEGORY
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -2304,10 +2304,10 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>XLS_TEST_METHOD, XLS_RUN_METHOD</t>
-  </si>
-  <si>
     <t>Precision of comparing the returned results with the expected ones</t>
+  </si>
+  <si>
+    <t>XLS_TEST_METHOD, XLS_RUN_METHOD, XLS_PROPERTIES</t>
   </si>
 </sst>
 </file>
@@ -2795,17 +2795,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3216,212 +3216,217 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3431,11 +3436,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3446,8 +3446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R42" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
+    <sheetView tabSelected="1" topLeftCell="K42" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,154 +3477,154 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="L46" s="32"/>
       <c r="M46" s="32" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="N46" s="32"/>
       <c r="O46" s="32"/>
@@ -5217,10 +5217,10 @@
       <c r="Q46" s="32"/>
       <c r="R46" s="32"/>
       <c r="S46" s="32" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="T46" s="33" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5295,21 +5295,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="B11:T11"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="B11:T11"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
EPBDS-4643 [Precision] Something went wrong after submiting 'precision' property with double minus
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="755">
   <si>
     <t>Display Name</t>
   </si>
@@ -2301,13 +2301,13 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>Integer</t>
-  </si>
-  <si>
     <t>Precision of comparing the returned results with the expected ones</t>
   </si>
   <si>
     <t>XLS_TEST_METHOD, XLS_RUN_METHOD, XLS_PROPERTIES</t>
+  </si>
+  <si>
+    <t>regexp:(-?[0-9]+)</t>
   </si>
 </sst>
 </file>
@@ -3446,8 +3446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K42" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5193,7 +5193,7 @@
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32" t="s">
-        <v>752</v>
+        <v>59</v>
       </c>
       <c r="F46" s="32"/>
       <c r="G46" s="32" t="s">
@@ -5209,10 +5209,12 @@
       </c>
       <c r="L46" s="32"/>
       <c r="M46" s="32" t="s">
+        <v>753</v>
+      </c>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32" t="s">
         <v>754</v>
       </c>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
       <c r="P46" s="32"/>
       <c r="Q46" s="32"/>
       <c r="R46" s="32"/>
@@ -5220,7 +5222,7 @@
         <v>84</v>
       </c>
       <c r="T46" s="33" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
EPBDS-4665 [Precision] remove precision property for RUN table
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/trunk/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -2304,10 +2304,10 @@
     <t>Precision of comparing the returned results with the expected ones</t>
   </si>
   <si>
-    <t>XLS_TEST_METHOD, XLS_RUN_METHOD, XLS_PROPERTIES</t>
-  </si>
-  <si>
     <t>regexp:(-?[0-9]+)</t>
+  </si>
+  <si>
+    <t>XLS_TEST_METHOD, XLS_PROPERTIES</t>
   </si>
 </sst>
 </file>
@@ -3446,8 +3446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="M52" sqref="M51:M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5143,7 +5143,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="45" spans="2:20" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:20" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="30" t="s">
         <v>203</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:20" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="31" t="s">
         <v>751</v>
       </c>
@@ -5209,11 +5209,11 @@
       </c>
       <c r="L46" s="32"/>
       <c r="M46" s="32" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="N46" s="32"/>
       <c r="O46" s="32" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="P46" s="32"/>
       <c r="Q46" s="32"/>

</xml_diff>